<commit_message>
Remove bounds in Service Heat Scen_B_SYS_Historic_Bounds.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F6702F-17BE-4563-B4EA-5BA71C41281C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6F5E0C-7A9F-4253-B7F0-72AD5B6D76A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -131,7 +131,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -923,9 +922,6 @@
     <t>FT-SRVLPG</t>
   </si>
   <si>
-    <t>FT-SRVHET</t>
-  </si>
-  <si>
     <t>FT-SRVETH</t>
   </si>
   <si>
@@ -1602,6 +1598,9 @@
   </si>
   <si>
     <t>Hannah Daly (UCC, h.daly@ucc.ie)</t>
+  </si>
+  <si>
+    <t>*FT-SRVHET</t>
   </si>
 </sst>
 </file>
@@ -6900,7 +6899,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1866BB23-5A03-40EF-B0E9-F9B9866A3EBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6944,7 +6943,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E3E5C63-B161-48E5-B8ED-0633D39A2895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6993,7 +6992,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CF24AC-7DD9-4FC1-A87D-1BF9925EB186}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7043,7 +7042,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FCE8A4C-8B6E-4F9C-92D9-9AF79E68BF41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7093,7 +7092,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49750B1E-CCA2-416D-82B9-48DD17660DD3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7142,7 +7141,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880F0CD6-2E6D-43FE-B69B-075C66F8CD54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -7518,7 +7517,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
@@ -7958,7 +7957,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
       <c r="A16" s="992" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B16" s="992"/>
       <c r="C16" s="992"/>
@@ -8044,10 +8043,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1">
       <c r="A19" s="983" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B19" s="991" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C19" s="991"/>
       <c r="D19" s="991"/>
@@ -8076,10 +8075,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1">
       <c r="A20" s="983" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B20" s="991" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C20" s="991"/>
       <c r="D20" s="991"/>
@@ -8108,10 +8107,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1">
       <c r="A21" s="983" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B21" s="986" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C21" s="986"/>
       <c r="D21" s="986"/>
@@ -8168,10 +8167,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1">
       <c r="A23" s="983" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B23" s="991" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C23" s="991"/>
       <c r="D23" s="991"/>
@@ -8201,7 +8200,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="983"/>
       <c r="B24" s="991" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C24" s="991"/>
       <c r="D24" s="991"/>
@@ -8231,7 +8230,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1">
       <c r="A25" s="983"/>
       <c r="B25" s="986" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C25" s="986"/>
       <c r="D25" s="986"/>
@@ -8260,10 +8259,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1">
       <c r="A26" s="983" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B26" s="991" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C26" s="991"/>
       <c r="D26" s="991"/>
@@ -8348,7 +8347,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1">
       <c r="A29" s="983" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B29" s="987">
         <v>1</v>
@@ -8380,10 +8379,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1">
       <c r="A30" s="983" t="s">
+        <v>449</v>
+      </c>
+      <c r="B30" s="993" t="s">
         <v>450</v>
-      </c>
-      <c r="B30" s="993" t="s">
-        <v>451</v>
       </c>
       <c r="C30" s="991"/>
       <c r="D30" s="991"/>
@@ -8412,10 +8411,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1">
       <c r="A31" s="983" t="s">
+        <v>451</v>
+      </c>
+      <c r="B31" s="991" t="s">
         <v>452</v>
-      </c>
-      <c r="B31" s="991" t="s">
-        <v>453</v>
       </c>
       <c r="C31" s="991"/>
       <c r="D31" s="991"/>
@@ -8445,7 +8444,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1">
       <c r="A32" s="989"/>
       <c r="B32" s="990" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C32" s="989"/>
       <c r="D32" s="989"/>
@@ -31303,8 +31302,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31467,7 +31466,7 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>217</v>
@@ -31515,7 +31514,7 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>460</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>217</v>
@@ -31638,17 +31637,17 @@
   <sheetData>
     <row r="1" spans="1:34" ht="21">
       <c r="A1" s="950" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:34">
       <c r="B5" s="949" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G5" s="948"/>
       <c r="H5" s="947"/>
@@ -31661,16 +31660,16 @@
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1">
       <c r="B6" s="946" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6" s="946" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="946" t="s">
         <v>215</v>
       </c>
       <c r="E6" s="946" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F6" s="945" t="str">
         <f>Regions!C$3</f>
@@ -31781,18 +31780,18 @@
         <v>IE-MN</v>
       </c>
       <c r="AG6" s="944" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AH6" s="944" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:34">
       <c r="C7" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E7" s="1">
         <v>2020</v>
@@ -31910,15 +31909,15 @@
         <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:34">
       <c r="C8" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E8" s="1">
         <v>2020</v>
@@ -32036,15 +32035,15 @@
         <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:34">
       <c r="C9" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E9" s="1">
         <v>2020</v>
@@ -32162,15 +32161,15 @@
         <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:34">
       <c r="C10" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E10" s="1">
         <v>2020</v>
@@ -32288,15 +32287,15 @@
         <v>T-CAR-BEV100_ELC21</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="C11" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E11" s="1">
         <v>2020</v>
@@ -32414,15 +32413,15 @@
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="C12" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E12" s="1">
         <v>2020</v>
@@ -32540,15 +32539,15 @@
         <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="C13" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E13" s="1">
         <v>2020</v>
@@ -32666,15 +32665,15 @@
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="C14" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E14" s="1">
         <v>2020</v>
@@ -32792,15 +32791,15 @@
         <v>T-LGT-ICE_DST61</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="C15" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E15" s="1">
         <v>2020</v>
@@ -32918,16 +32917,16 @@
         <v>T-LGT-BEV_ELC61</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="B16" s="938"/>
       <c r="C16" s="938" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D16" s="938" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E16" s="938">
         <v>2020</v>
@@ -33045,7 +33044,7 @@
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="AH16" s="938" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -33082,7 +33081,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -33093,7 +33092,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="B3" s="975" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -33104,39 +33103,39 @@
     </row>
     <row r="5" spans="1:11">
       <c r="B5" s="971" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C5" s="974" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D5" s="974" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E5" s="974" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="974" t="s">
         <v>244</v>
       </c>
-      <c r="F5" s="974" t="s">
+      <c r="G5" s="974" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="974" t="s">
-        <v>246</v>
-      </c>
       <c r="H5" s="973" t="s">
+        <v>422</v>
+      </c>
+      <c r="I5" s="973" t="s">
         <v>423</v>
       </c>
-      <c r="I5" s="973" t="s">
-        <v>424</v>
-      </c>
       <c r="J5" s="972" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K5" s="971" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="B6" s="938" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C6" s="938"/>
       <c r="D6" s="938"/>
@@ -33146,7 +33145,7 @@
       <c r="H6" s="938"/>
       <c r="I6" s="938"/>
       <c r="J6" s="938" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K6" s="970"/>
     </row>
@@ -33247,7 +33246,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -33258,7 +33257,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="B3" s="975" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -33269,39 +33268,39 @@
     </row>
     <row r="5" spans="1:11">
       <c r="B5" s="971" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C5" s="974" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D5" s="974" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E5" s="974" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="974" t="s">
         <v>244</v>
       </c>
-      <c r="F5" s="974" t="s">
+      <c r="G5" s="974" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="974" t="s">
-        <v>246</v>
-      </c>
       <c r="H5" s="973" t="s">
+        <v>422</v>
+      </c>
+      <c r="I5" s="973" t="s">
         <v>423</v>
       </c>
-      <c r="I5" s="973" t="s">
-        <v>424</v>
-      </c>
       <c r="J5" s="972" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K5" s="971" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="B6" s="938" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C6" s="938"/>
       <c r="D6" s="938"/>
@@ -33311,7 +33310,7 @@
       <c r="H6" s="938"/>
       <c r="I6" s="938"/>
       <c r="J6" s="938" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K6" s="938"/>
     </row>
@@ -33407,7 +33406,7 @@
   <sheetData>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C4" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","Emissions","CO2","2020")</f>
@@ -33416,7 +33415,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C5" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"CO2 Emissions in 2020")</f>
@@ -33425,7 +33424,7 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="1">
         <v>2020</v>
@@ -33436,7 +33435,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C7" s="941">
         <v>33792</v>
@@ -33447,44 +33446,44 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C13" s="1">
         <v>-1</v>
@@ -33492,7 +33491,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -33523,31 +33522,31 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="967" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B1" s="967"/>
       <c r="C1" s="967"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="969" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B2" s="967"/>
       <c r="C2" s="967"/>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="969" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B4" s="967"/>
       <c r="C4" s="967"/>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="968" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B5" s="968" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C5" s="968">
         <v>2020</v>
@@ -33558,7 +33557,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="967" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="967">
         <v>38233</v>
@@ -33569,7 +33568,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="967" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C7" s="967">
         <v>32600</v>
@@ -33580,7 +33579,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="967" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C8" s="967">
         <v>10474</v>
@@ -33591,7 +33590,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="967" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C9" s="967">
         <v>4013</v>
@@ -33602,7 +33601,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="967" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C10" s="967">
         <v>2459</v>
@@ -33613,7 +33612,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="967" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C11" s="967">
         <v>512</v>
@@ -33624,7 +33623,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="967" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C12" s="967">
         <v>33</v>
@@ -33633,7 +33632,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="938"/>
       <c r="B13" s="938" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C13" s="938">
         <f>SUM(C6:C12)</f>
@@ -33642,7 +33641,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="969" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B17" s="967"/>
       <c r="C17" s="967"/>
@@ -33650,10 +33649,10 @@
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="968" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B18" s="968" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C18" s="968">
         <v>2020</v>
@@ -33665,7 +33664,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="967" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C19" s="967">
         <v>20928</v>
@@ -33677,7 +33676,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="967" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C20" s="967">
         <v>727</v>
@@ -33689,7 +33688,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="967" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C21" s="967">
         <v>29</v>
@@ -33701,7 +33700,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="967" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C22" s="967">
         <v>27</v>
@@ -33713,7 +33712,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="967" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C23" s="967">
         <v>16</v>
@@ -33725,7 +33724,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="967" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C24" s="967">
         <v>2</v>
@@ -33737,7 +33736,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="967" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C25" s="967">
         <v>2</v>
@@ -33749,7 +33748,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="967" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C26" s="967">
         <v>1</v>
@@ -33759,7 +33758,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="938"/>
       <c r="B27" s="938" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C27" s="938">
         <f>SUM(C19:C26)</f>
@@ -33768,17 +33767,17 @@
     </row>
     <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="969" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B31" s="967"/>
       <c r="C31" s="967"/>
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="968" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B32" s="968" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C32" s="968">
         <v>2020</v>
@@ -33789,7 +33788,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="967" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C33" s="967">
         <v>2043</v>
@@ -33800,7 +33799,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="967" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C34" s="967">
         <v>16</v>
@@ -33811,7 +33810,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="967" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C35" s="967">
         <v>6</v>
@@ -33822,7 +33821,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="967" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C36" s="967">
         <v>1</v>
@@ -33831,7 +33830,7 @@
     <row r="37" spans="1:29">
       <c r="A37" s="938"/>
       <c r="B37" s="938" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C37" s="938">
         <f>SUM(C33:C36)</f>
@@ -33840,7 +33839,7 @@
     </row>
     <row r="40" spans="1:29" ht="15.75">
       <c r="B40" s="966" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -33929,7 +33928,7 @@
     </row>
     <row r="42" spans="1:29">
       <c r="B42" s="964" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C42" s="963">
         <v>4857000.0000000037</v>
@@ -34015,7 +34014,7 @@
     </row>
     <row r="43" spans="1:29">
       <c r="B43" s="961" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C43" s="962">
         <v>0.99999999999999956</v>
@@ -34101,7 +34100,7 @@
     </row>
     <row r="44" spans="1:29">
       <c r="B44" s="960" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C44" s="959"/>
       <c r="D44" s="959"/>
@@ -34133,628 +34132,628 @@
     </row>
     <row r="49" spans="2:3" ht="21">
       <c r="B49" s="994" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C49" s="994"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="957" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C50" s="957" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" thickBot="1">
       <c r="B51" s="956" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C51" s="955"/>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" s="952" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C52" s="952"/>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="951" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C53" s="951" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" s="951" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C54" s="951" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="952" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C55" s="952"/>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="951" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C56" s="951" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="951" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C57" s="951" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58" s="951" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C58" s="951" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="951" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C59" s="951" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="951" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C60" s="951" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="951" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C61" s="951" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="B62" s="951" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C62" s="951" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" s="951" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C63" s="951" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="951" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C64" s="951" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="951" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C65" s="951" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="B66" s="951" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C66" s="951" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="951" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C67" s="951" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" s="951" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C68" s="951" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="951" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C69" s="951" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" s="951" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C70" s="951" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="951" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C71" s="951" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="B72" s="951" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C72" s="951" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="B73" s="951" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C73" s="951" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="951" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C74" s="951" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="952" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C75" s="952"/>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" s="951" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C76" s="951" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="B77" s="951" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C77" s="951" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="78" spans="2:3">
       <c r="B78" s="951" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C78" s="951" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="951" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C79" s="951" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="951" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C80" s="951" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" s="951" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C81" s="951" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" s="951" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C82" s="951" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" s="951" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C83" s="951" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="84" spans="2:3">
       <c r="B84" s="951" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C84" s="951" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" s="951" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C85" s="951" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" s="951" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C86" s="951" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" s="951" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C87" s="951" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" s="951" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C88" s="951" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="B89" s="951" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C89" s="951" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" s="951" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C90" s="951" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" s="951" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C91" s="951" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="B92" s="951" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C92" s="951" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="B93" s="951" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C93" s="951" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="B94" s="951" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C94" s="951" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="B95" s="952" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C95" s="952"/>
     </row>
     <row r="96" spans="2:3">
       <c r="B96" s="951" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C96" s="951" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="951" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C97" s="951" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="B98" s="951" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C98" s="951" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="99" spans="2:3">
       <c r="B99" s="951" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C99" s="951" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="B100" s="951" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C100" s="951" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="101" spans="2:3">
       <c r="B101" s="952" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C101" s="952"/>
     </row>
     <row r="102" spans="2:3">
       <c r="B102" s="951" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C102" s="951" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="103" spans="2:3">
       <c r="B103" s="951" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C103" s="951" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="B104" s="951" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C104" s="951" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="B105" s="954" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C105" s="953"/>
     </row>
     <row r="106" spans="2:3">
       <c r="B106" s="952" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C106" s="952"/>
     </row>
     <row r="107" spans="2:3">
       <c r="B107" s="951" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C107" s="951" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="951" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C108" s="951" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="2:3">
       <c r="B109" s="951" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C109" s="951" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="951" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C110" s="951" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="951" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C111" s="951" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="951" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C112" s="951" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="951" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C113" s="951" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="952" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C114" s="952"/>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="951" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C115" s="951" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="951" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C116" s="951" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="117" spans="2:3">
       <c r="B117" s="951" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C117" s="951" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="118" spans="2:3">
       <c r="B118" s="951" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C118" s="951" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="2:3">
       <c r="B119" s="951" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C119" s="951" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="120" spans="2:3">
       <c r="B120" s="951" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C120" s="951" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="951" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C121" s="951" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="952" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C122" s="952"/>
     </row>
     <row r="123" spans="2:3">
       <c r="B123" s="951" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C123" s="951" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="2:3">
       <c r="B124" s="951" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C124" s="951" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="125" spans="2:3">
       <c r="B125" s="951" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C125" s="951" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="2:3">
       <c r="B126" s="951" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C126" s="951" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="2:3">
       <c r="B127" s="951" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C127" s="951" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="2:3">
       <c r="B128" s="951" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C128" s="951" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" s="951" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C129" s="951" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Do not constraint DH, ethanol and biodiesel in RSD by EB; and relax ELC use in SRV in 2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A859CD8-1C22-4547-B3D7-3251CAB90AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DC2955-6A54-4665-8392-4CB9B5734D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -142,6 +142,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={EA2214DE-E5ED-4BA3-B779-4C671AA758DE}</author>
+  </authors>
+  <commentList>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{EA2214DE-E5ED-4BA3-B779-4C671AA758DE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Relax this bound to avoid dummies</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
@@ -186,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="459">
   <si>
     <t>Development</t>
   </si>
@@ -839,12 +857,6 @@
     <t>FT-PWRWIN</t>
   </si>
   <si>
-    <t>*FT-PWRHFO</t>
-  </si>
-  <si>
-    <t>*FT-PWRDIS</t>
-  </si>
-  <si>
     <t>FT-SRVBGS</t>
   </si>
   <si>
@@ -1563,40 +1575,46 @@
     <t>2020 data</t>
   </si>
   <si>
+    <t>FT-RSDCOA</t>
+  </si>
+  <si>
+    <t>FT-RSDELC</t>
+  </si>
+  <si>
+    <t>FT-RSDGAS</t>
+  </si>
+  <si>
+    <t>FT-RSDLPG</t>
+  </si>
+  <si>
+    <t>FT-RSDSOL</t>
+  </si>
+  <si>
+    <t>FT-RSDWOO</t>
+  </si>
+  <si>
+    <t>FT-RSDKER</t>
+  </si>
+  <si>
+    <t>FT-RSDPEA</t>
+  </si>
+  <si>
     <t>FT-RSDBDL</t>
   </si>
   <si>
-    <t>FT-RSDCOA</t>
-  </si>
-  <si>
-    <t>FT-RSDELC</t>
-  </si>
-  <si>
     <t>FT-RSDETH</t>
   </si>
   <si>
-    <t>FT-RSDGAS</t>
-  </si>
-  <si>
     <t>FT-RSDHET</t>
   </si>
   <si>
-    <t>FT-RSDLPG</t>
-  </si>
-  <si>
-    <t>FT-RSDSOL</t>
-  </si>
-  <si>
-    <t>FT-RSDWOO</t>
-  </si>
-  <si>
-    <t>FT-RSDKER</t>
-  </si>
-  <si>
-    <t>FT-RSDPEA</t>
-  </si>
-  <si>
-    <t>*2018</t>
+    <t>*</t>
+  </si>
+  <si>
+    <t>FT-PWRHFO</t>
+  </si>
+  <si>
+    <t>FT-PWRDIS</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1841,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1926,6 +1944,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="157">
     <border>
@@ -3933,7 +3957,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="378">
+  <cellXfs count="379">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4974,6 +4998,7 @@
     <xf numFmtId="167" fontId="5" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5385,6 +5410,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{0EBAA6E2-D3EC-429B-B80A-AFBE5C02E277}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5646,6 +5677,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I8" dT="2022-09-16T03:05:16.52" personId="{0EBAA6E2-D3EC-429B-B80A-AFBE5C02E277}" id="{EA2214DE-E5ED-4BA3-B779-4C671AA758DE}">
+    <text>Relax this bound to avoid dummies</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B28889-4A29-4B8D-BD3E-384099A070C4}">
   <sheetPr codeName="Sheet13"/>
@@ -6089,12 +6128,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="375" t="s">
-        <v>406</v>
-      </c>
-      <c r="B16" s="375"/>
-      <c r="C16" s="375"/>
-      <c r="D16" s="375"/>
+      <c r="A16" s="376" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" s="376"/>
+      <c r="C16" s="376"/>
+      <c r="D16" s="376"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6176,13 +6215,13 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1">
       <c r="A19" s="67" t="s">
-        <v>407</v>
-      </c>
-      <c r="B19" s="374" t="s">
-        <v>418</v>
-      </c>
-      <c r="C19" s="374"/>
-      <c r="D19" s="374"/>
+        <v>405</v>
+      </c>
+      <c r="B19" s="375" t="s">
+        <v>416</v>
+      </c>
+      <c r="C19" s="375"/>
+      <c r="D19" s="375"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6208,13 +6247,13 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1">
       <c r="A20" s="67" t="s">
-        <v>408</v>
-      </c>
-      <c r="B20" s="374" t="s">
-        <v>421</v>
-      </c>
-      <c r="C20" s="374"/>
-      <c r="D20" s="374"/>
+        <v>406</v>
+      </c>
+      <c r="B20" s="375" t="s">
+        <v>419</v>
+      </c>
+      <c r="C20" s="375"/>
+      <c r="D20" s="375"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6240,10 +6279,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1">
       <c r="A21" s="67" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C21" s="70"/>
       <c r="D21" s="70"/>
@@ -6300,13 +6339,13 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1">
       <c r="A23" s="67" t="s">
-        <v>410</v>
-      </c>
-      <c r="B23" s="374" t="s">
-        <v>420</v>
-      </c>
-      <c r="C23" s="374"/>
-      <c r="D23" s="374"/>
+        <v>408</v>
+      </c>
+      <c r="B23" s="375" t="s">
+        <v>418</v>
+      </c>
+      <c r="C23" s="375"/>
+      <c r="D23" s="375"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6332,11 +6371,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="374" t="s">
-        <v>419</v>
-      </c>
-      <c r="C24" s="374"/>
-      <c r="D24" s="374"/>
+      <c r="B24" s="375" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" s="375"/>
+      <c r="D24" s="375"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6363,7 +6402,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1">
       <c r="A25" s="67"/>
       <c r="B25" s="70" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
@@ -6392,13 +6431,13 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1">
       <c r="A26" s="67" t="s">
-        <v>411</v>
-      </c>
-      <c r="B26" s="374" t="s">
-        <v>420</v>
-      </c>
-      <c r="C26" s="374"/>
-      <c r="D26" s="374"/>
+        <v>409</v>
+      </c>
+      <c r="B26" s="375" t="s">
+        <v>418</v>
+      </c>
+      <c r="C26" s="375"/>
+      <c r="D26" s="375"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6480,7 +6519,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1">
       <c r="A29" s="67" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B29" s="71">
         <v>1</v>
@@ -6512,13 +6551,13 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1">
       <c r="A30" s="67" t="s">
-        <v>413</v>
-      </c>
-      <c r="B30" s="376" t="s">
-        <v>414</v>
-      </c>
-      <c r="C30" s="374"/>
-      <c r="D30" s="374"/>
+        <v>411</v>
+      </c>
+      <c r="B30" s="377" t="s">
+        <v>412</v>
+      </c>
+      <c r="C30" s="375"/>
+      <c r="D30" s="375"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6544,13 +6583,13 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1">
       <c r="A31" s="67" t="s">
-        <v>415</v>
-      </c>
-      <c r="B31" s="374" t="s">
-        <v>416</v>
-      </c>
-      <c r="C31" s="374"/>
-      <c r="D31" s="374"/>
+        <v>413</v>
+      </c>
+      <c r="B31" s="375" t="s">
+        <v>414</v>
+      </c>
+      <c r="C31" s="375"/>
+      <c r="D31" s="375"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -6577,7 +6616,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1">
       <c r="A32" s="73"/>
       <c r="B32" s="74" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
@@ -9674,7 +9713,7 @@
     </row>
     <row r="10" spans="1:43" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -9756,7 +9795,7 @@
     </row>
     <row r="11" spans="1:43" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -9836,7 +9875,7 @@
     </row>
     <row r="12" spans="1:43" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -9888,7 +9927,7 @@
     </row>
     <row r="13" spans="1:43" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -9952,7 +9991,7 @@
     </row>
     <row r="14" spans="1:43" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -10192,7 +10231,7 @@
     </row>
     <row r="16" spans="1:43" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -10256,7 +10295,7 @@
     </row>
     <row r="17" spans="1:43" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -10320,7 +10359,7 @@
     </row>
     <row r="18" spans="1:43" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -10372,7 +10411,7 @@
     </row>
     <row r="19" spans="1:43" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -10433,7 +10472,7 @@
     </row>
     <row r="20" spans="1:43" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -10678,7 +10717,7 @@
     </row>
     <row r="22" spans="1:43" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -10742,7 +10781,7 @@
     </row>
     <row r="23" spans="1:43" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -10792,7 +10831,7 @@
     </row>
     <row r="24" spans="1:43" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -15402,7 +15441,7 @@
     </row>
     <row r="74" spans="1:43" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -15449,7 +15488,7 @@
     </row>
     <row r="75" spans="1:43" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -15543,7 +15582,7 @@
     </row>
     <row r="77" spans="1:43" ht="15">
       <c r="A77" s="365" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B77" s="362"/>
       <c r="C77" s="23"/>
@@ -15590,7 +15629,7 @@
     </row>
     <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B78" s="362"/>
       <c r="C78" s="23"/>
@@ -15875,7 +15914,7 @@
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
       <c r="A1" s="75" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B1" s="76" t="s">
         <v>160</v>
@@ -16996,7 +17035,7 @@
     </row>
     <row r="10" spans="1:43" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -17078,7 +17117,7 @@
     </row>
     <row r="11" spans="1:43" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -17158,7 +17197,7 @@
     </row>
     <row r="12" spans="1:43" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -17210,7 +17249,7 @@
     </row>
     <row r="13" spans="1:43" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -17274,7 +17313,7 @@
     </row>
     <row r="14" spans="1:43" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -17514,7 +17553,7 @@
     </row>
     <row r="16" spans="1:43" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -17578,7 +17617,7 @@
     </row>
     <row r="17" spans="1:43" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -17642,7 +17681,7 @@
     </row>
     <row r="18" spans="1:43" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -17694,7 +17733,7 @@
     </row>
     <row r="19" spans="1:43" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -17755,7 +17794,7 @@
     </row>
     <row r="20" spans="1:43" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -18000,7 +18039,7 @@
     </row>
     <row r="22" spans="1:43" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -18064,7 +18103,7 @@
     </row>
     <row r="23" spans="1:43" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -18114,7 +18153,7 @@
     </row>
     <row r="24" spans="1:43" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -22724,7 +22763,7 @@
     </row>
     <row r="74" spans="1:43" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -22771,7 +22810,7 @@
     </row>
     <row r="75" spans="1:43" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -22818,7 +22857,7 @@
     </row>
     <row r="76" spans="1:43" ht="12.75" customHeight="1">
       <c r="A76" s="363" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B76" s="364"/>
       <c r="C76" s="23"/>
@@ -22865,7 +22904,7 @@
     </row>
     <row r="77" spans="1:43" ht="15">
       <c r="A77" s="365" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B77" s="362"/>
       <c r="C77" s="23"/>
@@ -22912,7 +22951,7 @@
     </row>
     <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B78" s="362"/>
       <c r="C78" s="23"/>
@@ -23951,365 +23990,375 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FEB92-3C8E-4A89-8F18-2AEFFF284423}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="28" t="s">
         <v>199</v>
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="D3" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="29">
+      <c r="F3" s="29">
         <v>2018</v>
       </c>
-      <c r="F3" s="29">
+      <c r="G3" s="29">
         <v>2019</v>
       </c>
-      <c r="G3" s="29">
+      <c r="H3" s="29">
         <v>2020</v>
       </c>
-      <c r="H3" s="29">
+      <c r="I3" s="29">
         <v>2021</v>
       </c>
-      <c r="I3" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" t="s">
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="C4" t="s">
         <v>202</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="19" t="str">
+      <c r="E4" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E4" s="19">
+      <c r="F4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AG$10,'EB2018'!$AG$11,'EB2018'!$AH$10,'EB2018'!$AH$11),1)</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AG$10,'EB2019'!$AG$11,'EB2019'!$AH$10,'EB2019'!$AH$11),1)</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="G4" s="19">
+      <c r="H4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AG$10,'EB2020'!$AG$11,'EB2020'!$AH$10,'EB2020'!$AH$11),1)</f>
         <v>1.6</v>
       </c>
-      <c r="H4" s="19">
+      <c r="I4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AG$10,'EB2021'!$AG$11,'EB2021'!$AH$10,'EB2021'!$AH$11),1)</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" t="s">
+    <row r="5" spans="2:10">
+      <c r="C5" t="s">
         <v>203</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="19" t="str">
+      <c r="E5" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E5" s="19">
+      <c r="F5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$10,'EB2018'!$AE$11),1)</f>
         <v>3.2</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$10,'EB2019'!$AE$11),1)</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="G5" s="19">
+      <c r="H5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$10,'EB2020'!$AE$11),1)</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="H5" s="19">
+      <c r="I5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$10,'EB2021'!$AE$11),1)</f>
         <v>4.3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" t="s">
+    <row r="6" spans="2:10">
+      <c r="C6" t="s">
         <v>201</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="19" t="str">
+      <c r="E6" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$10,'EB2018'!$C$11),1)</f>
         <v>20.5</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$10,'EB2019'!$C$11),1)</f>
         <v>6.1999999999999993</v>
       </c>
-      <c r="G6" s="19">
+      <c r="H6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$10,'EB2020'!$C$11),1)</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="H6" s="19">
+      <c r="I6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$10,'EB2021'!$C$11),1)</f>
         <v>28.200000000000003</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>211</v>
+        <v>456</v>
       </c>
       <c r="C7" t="s">
+        <v>458</v>
+      </c>
+      <c r="D7" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="E7" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
-      <c r="I7">
+      <c r="I7" s="19"/>
+      <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
+    <row r="8" spans="2:10">
+      <c r="C8" t="s">
         <v>204</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>200</v>
       </c>
-      <c r="D8" s="19" t="str">
+      <c r="E8" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E8" s="19">
+      <c r="F8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$10,'EB2018'!$AA$11),1)</f>
         <v>103.1</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$10,'EB2019'!$AA$11),1)</f>
         <v>105.6</v>
       </c>
-      <c r="G8" s="19">
+      <c r="H8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$10,'EB2020'!$AA$11),1)</f>
         <v>107.5</v>
       </c>
-      <c r="H8" s="19">
+      <c r="I8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$10,'EB2021'!$AA$11),1)</f>
         <v>98.1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>210</v>
+        <v>456</v>
       </c>
       <c r="C9" t="s">
+        <v>457</v>
+      </c>
+      <c r="D9" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="E9" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
-      <c r="I9">
+      <c r="I9" s="19"/>
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" t="s">
+    <row r="10" spans="2:10">
+      <c r="C10" t="s">
         <v>205</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="19" t="str">
+      <c r="E10" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2018'!$AC$22),1)</f>
         <v>2.5</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2019'!$AC$22),1)</f>
         <v>3.2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="H10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2020'!$AC$22),1)</f>
         <v>3.4</v>
       </c>
-      <c r="H10" s="19">
+      <c r="I10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AC$22),1)</f>
         <v>2.7</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" t="s">
+    <row r="11" spans="2:10">
+      <c r="C11" t="s">
         <v>206</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="E11" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E11" s="19">
+      <c r="F11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AF$10,'EB2018'!$AF$11,'EB2018'!$AN$10,'EB2018'!$AN$11),1)</f>
         <v>8</v>
       </c>
-      <c r="F11" s="19">
+      <c r="G11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AF$10,'EB2019'!$AF$11,'EB2019'!$AN$10,'EB2019'!$AN$11),1)</f>
         <v>7.8</v>
       </c>
-      <c r="G11" s="19">
+      <c r="H11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AF$10,'EB2020'!$AF$11,'EB2020'!$AN$10,'EB2020'!$AN$11),1)</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="H11" s="19">
+      <c r="I11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AF$10,'EB2021'!$AF$11,'EB2021'!$AN$10,'EB2021'!$AN$11),1)</f>
         <v>7.8</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" t="s">
+    <row r="12" spans="2:10">
+      <c r="C12" t="s">
         <v>207</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>200</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="E12" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E12" s="19">
+      <c r="F12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$10,'EB2018'!$H$11),1)</f>
         <v>19.900000000000002</v>
       </c>
-      <c r="F12" s="19">
+      <c r="G12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$10,'EB2019'!$H$11),1)</f>
         <v>18.200000000000003</v>
       </c>
-      <c r="G12" s="19">
+      <c r="H12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$10,'EB2020'!$H$11),1)</f>
         <v>9</v>
       </c>
-      <c r="H12" s="19">
+      <c r="I12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$10,'EB2021'!$H$11),1)</f>
         <v>3</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" t="s">
+    <row r="13" spans="2:10">
+      <c r="C13" t="s">
         <v>208</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="E13" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E13" s="19">
+      <c r="F13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2018'!$AK$22),1)</f>
         <v>0.1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="G13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2019'!$AK$22),1)</f>
         <v>0.2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="H13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2020'!$AK$22),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="H13" s="19">
+      <c r="I13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AK$22),1)</f>
         <v>0.4</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14" t="s">
+    <row r="14" spans="2:10">
+      <c r="C14" t="s">
         <v>209</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>200</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="E14" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E14" s="19">
+      <c r="F14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2018'!$AD$22),1)</f>
         <v>31.200000000000003</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2019'!$AD$22),1)</f>
         <v>36.1</v>
       </c>
-      <c r="G14" s="19">
+      <c r="H14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2020'!$AD$22),1)</f>
         <v>41.6</v>
       </c>
-      <c r="H14" s="19">
+      <c r="I14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AD$22),1)</f>
         <v>35.200000000000003</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1</v>
       </c>
     </row>
@@ -24320,389 +24369,402 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="28" t="s">
         <v>199</v>
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="D3" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>458</v>
-      </c>
       <c r="F3" s="29">
+        <v>2018</v>
+      </c>
+      <c r="G3" s="29">
         <v>2019</v>
       </c>
-      <c r="G3" s="29">
+      <c r="H3" s="29">
         <v>2020</v>
       </c>
-      <c r="H3" s="29">
+      <c r="I3" s="29">
         <v>2021</v>
       </c>
-      <c r="I3" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="C4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="19" t="str">
+      <c r="E4" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E4" s="19">
+      <c r="F4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="19">
+      <c r="H4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="I4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" t="s">
-        <v>455</v>
-      </c>
+    <row r="5" spans="2:10">
       <c r="C5" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="19" t="str">
+      <c r="E5" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E5" s="19">
+      <c r="F5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
         <v>1.3</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="G5" s="19">
+      <c r="H5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H5" s="19">
+      <c r="I5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" t="s">
-        <v>448</v>
-      </c>
+    <row r="6" spans="2:10">
       <c r="C6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D6" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="19" t="str">
+      <c r="E6" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
         <v>9.1</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
         <v>7.8</v>
       </c>
-      <c r="G6" s="19">
+      <c r="H6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="H6" s="19">
+      <c r="I6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
         <v>7.8</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" t="s">
-        <v>457</v>
-      </c>
+    <row r="7" spans="2:10">
       <c r="C7" t="s">
+        <v>452</v>
+      </c>
+      <c r="D7" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="E7" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E7" s="19">
+      <c r="F7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
         <v>8.2999999999999989</v>
       </c>
-      <c r="F7" s="19">
+      <c r="G7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
         <v>7.6999999999999993</v>
       </c>
-      <c r="G7" s="19">
+      <c r="H7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
         <v>8</v>
       </c>
-      <c r="H7" s="19">
+      <c r="I7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
         <v>7.6</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
-        <v>449</v>
-      </c>
+    <row r="8" spans="2:10">
       <c r="C8" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" t="s">
         <v>200</v>
       </c>
-      <c r="D8" s="19" t="str">
+      <c r="E8" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E8" s="19">
+      <c r="F8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
         <v>29.5</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)</f>
         <v>29.3</v>
       </c>
-      <c r="G8" s="19">
+      <c r="H8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
         <v>31.5</v>
       </c>
-      <c r="H8" s="19">
+      <c r="I8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
         <v>31.5</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="C9" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="E9" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E9" s="19">
+      <c r="F9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="19">
+      <c r="G9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="H9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="19">
+      <c r="I9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" t="s">
-        <v>451</v>
-      </c>
+    <row r="10" spans="2:10">
       <c r="C10" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="19" t="str">
+      <c r="E10" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
         <v>25.3</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
         <v>24.8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="H10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
         <v>24.700000000000003</v>
       </c>
-      <c r="H10" s="19">
+      <c r="I10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
         <v>25</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D11" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="E11" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E11" s="19">
+      <c r="F11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="19">
+      <c r="G11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
+      <c r="H11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="19">
+      <c r="I11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" t="s">
-        <v>453</v>
-      </c>
+    <row r="12" spans="2:10">
       <c r="C12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" t="s">
         <v>200</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="E12" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E12" s="19">
+      <c r="F12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
         <v>2.3000000000000003</v>
       </c>
-      <c r="F12" s="19">
+      <c r="G12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
         <v>2.1</v>
       </c>
-      <c r="G12" s="19">
+      <c r="H12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
         <v>2.4</v>
       </c>
-      <c r="H12" s="19">
+      <c r="I12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
         <v>2.1</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" t="s">
-        <v>456</v>
-      </c>
+    <row r="13" spans="2:10">
       <c r="C13" t="s">
+        <v>451</v>
+      </c>
+      <c r="D13" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="E13" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E13" s="19">
+      <c r="F13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
         <v>50.300000000000004</v>
       </c>
-      <c r="F13" s="19">
+      <c r="G13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
         <v>49.9</v>
       </c>
-      <c r="G13" s="19">
+      <c r="H13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
         <v>56.2</v>
       </c>
-      <c r="H13" s="19">
+      <c r="I13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
         <v>51.2</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14" t="s">
-        <v>454</v>
-      </c>
+    <row r="14" spans="2:10">
       <c r="C14" t="s">
+        <v>449</v>
+      </c>
+      <c r="D14" t="s">
         <v>200</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="E14" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E14" s="19">
+      <c r="F14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="G14" s="19">
+      <c r="H14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="H14" s="19">
+      <c r="I14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1</v>
       </c>
     </row>
@@ -24712,396 +24774,401 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="28" t="s">
         <v>199</v>
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="D3" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="29">
+      <c r="F3" s="29">
         <v>2018</v>
       </c>
-      <c r="F3" s="29">
+      <c r="G3" s="29">
         <v>2019</v>
       </c>
-      <c r="G3" s="29">
+      <c r="H3" s="29">
         <v>2020</v>
       </c>
-      <c r="H3" s="29">
+      <c r="I3" s="29">
         <v>2021</v>
       </c>
-      <c r="I3" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" t="s">
-        <v>218</v>
-      </c>
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="19" t="str">
+      <c r="E4" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E4" s="19">
+      <c r="F4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$57),1)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$57),1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="19">
+      <c r="H4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$57),1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="I4" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$57),1)</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" t="s">
-        <v>212</v>
-      </c>
+    <row r="5" spans="2:10">
       <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="19" t="str">
+      <c r="E5" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E5" s="19">
+      <c r="F5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AH$57),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AH$57),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="G5" s="19">
+      <c r="H5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AH$57),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="H5" s="19">
+      <c r="I5" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AH$57),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" t="s">
-        <v>213</v>
-      </c>
+    <row r="6" spans="2:10">
       <c r="C6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="19" t="str">
+      <c r="E6" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$57),1)</f>
         <v>0.79999999999999993</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$57),1)</f>
         <v>0.6</v>
       </c>
-      <c r="G6" s="19">
+      <c r="H6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$57),1)</f>
         <v>0.7</v>
       </c>
-      <c r="H6" s="19">
+      <c r="I6" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$57),1)</f>
         <v>0.79999999999999993</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" t="s">
-        <v>214</v>
-      </c>
+    <row r="7" spans="2:10">
       <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="E7" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E7" s="19">
+      <c r="F7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="F7" s="19">
+      <c r="G7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="G7" s="19">
+      <c r="H7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="H7" s="19">
+      <c r="I7" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
-        <v>219</v>
-      </c>
+    <row r="8" spans="2:10">
       <c r="C8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" t="s">
         <v>200</v>
       </c>
-      <c r="D8" s="19" t="str">
+      <c r="E8" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E8" s="19">
+      <c r="F8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$57),1)</f>
         <v>45.2</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$57),1)</f>
         <v>46.9</v>
       </c>
-      <c r="G8" s="19">
+      <c r="H8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$57),1)</f>
         <v>47.1</v>
       </c>
-      <c r="H8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)</f>
-        <v>49.9</v>
-      </c>
-      <c r="I8">
+      <c r="I8" s="374">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)+0.8</f>
+        <v>50.699999999999996</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
-      <c r="B9" t="s">
-        <v>222</v>
-      </c>
+    <row r="9" spans="2:10">
       <c r="C9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="E9" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E9" s="19">
+      <c r="F9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$57),1)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="19">
+      <c r="G9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$57),1)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="H9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$57),1)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="19">
+      <c r="I9" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$57),1)</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" t="s">
-        <v>215</v>
-      </c>
+    <row r="10" spans="2:10">
       <c r="C10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="19" t="str">
+      <c r="E10" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$57),1)</f>
         <v>13.799999999999999</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$57),1)</f>
         <v>14.2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="H10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$57),1)</f>
         <v>14.7</v>
       </c>
-      <c r="H10" s="19">
+      <c r="I10" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$57),1)</f>
         <v>14.1</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" t="s">
-        <v>221</v>
-      </c>
+    <row r="11" spans="2:10">
       <c r="C11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="E11" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E11" s="19">
+      <c r="F11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$57),1)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="19">
+      <c r="G11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$57),1)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
+      <c r="H11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$57),1)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="19">
+      <c r="I11" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$57),1)</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
+    <row r="12" spans="2:10">
       <c r="C12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" t="s">
         <v>200</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="E12" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E12" s="19">
+      <c r="F12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$57),1)</f>
         <v>3</v>
       </c>
-      <c r="F12" s="19">
+      <c r="G12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$57),1)</f>
         <v>3</v>
       </c>
-      <c r="G12" s="19">
+      <c r="H12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$57),1)</f>
         <v>2.8000000000000003</v>
       </c>
-      <c r="H12" s="19">
+      <c r="I12" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$57),1)</f>
         <v>3</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" t="s">
-        <v>217</v>
-      </c>
+    <row r="13" spans="2:10">
       <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="E13" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E13" s="19">
+      <c r="F13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$57,'EB2018'!$S$57,'EB2018'!$U$57),1)</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="F13" s="19">
+      <c r="G13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$57,'EB2019'!$S$57,'EB2019'!$U$57),1)</f>
         <v>6.3999999999999995</v>
       </c>
-      <c r="G13" s="19">
+      <c r="H13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$57,'EB2020'!$S$57,'EB2020'!$U$57),1)</f>
         <v>6.8999999999999995</v>
       </c>
-      <c r="H13" s="19">
+      <c r="I13" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$57,'EB2021'!$S$57,'EB2021'!$U$57),1)</f>
         <v>6.5</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14" t="s">
-        <v>216</v>
-      </c>
+    <row r="14" spans="2:10">
       <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" t="s">
         <v>200</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="E14" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="E14" s="19">
+      <c r="F14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="G14" s="19">
+      <c r="H14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="H14" s="19">
+      <c r="I14" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -25127,17 +25194,17 @@
   <sheetData>
     <row r="1" spans="1:34" ht="21">
       <c r="A1" s="42" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:34">
       <c r="B5" s="41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="39"/>
@@ -25149,16 +25216,16 @@
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1">
       <c r="B6" s="38" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>198</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F6" s="37" t="str">
         <f>Regions!C$3</f>
@@ -25269,18 +25336,18 @@
         <v>IE-MN</v>
       </c>
       <c r="AG6" s="36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AH6" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:34">
       <c r="C7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E7">
         <v>2020</v>
@@ -25398,15 +25465,15 @@
         <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="AH7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:34">
       <c r="C8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8">
         <v>2020</v>
@@ -25524,15 +25591,15 @@
         <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="AH8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:34">
       <c r="C9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E9">
         <v>2020</v>
@@ -25650,15 +25717,15 @@
         <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="AH9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:34">
       <c r="C10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E10">
         <v>2020</v>
@@ -25776,15 +25843,15 @@
         <v>T-CAR-BEV100_ELC21</v>
       </c>
       <c r="AH10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="C11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E11">
         <v>2020</v>
@@ -25902,15 +25969,15 @@
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="AH11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="C12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12">
         <v>2020</v>
@@ -26028,15 +26095,15 @@
         <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="AH12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="C13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E13">
         <v>2020</v>
@@ -26154,15 +26221,15 @@
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="AH13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="C14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E14">
         <v>2020</v>
@@ -26280,15 +26347,15 @@
         <v>T-LGT-ICE_DST61</v>
       </c>
       <c r="AH14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="C15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E15">
         <v>2020</v>
@@ -26406,16 +26473,16 @@
         <v>T-LGT-BEV_ELC61</v>
       </c>
       <c r="AH15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E16" s="30">
         <v>2020</v>
@@ -26533,7 +26600,7 @@
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="AH16" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -26560,25 +26627,25 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="59" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="59" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C5" s="58">
         <v>2020</v>
@@ -26589,7 +26656,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C6">
         <v>38233</v>
@@ -26600,7 +26667,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C7">
         <v>32600</v>
@@ -26611,7 +26678,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C8">
         <v>10474</v>
@@ -26622,7 +26689,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C9">
         <v>4013</v>
@@ -26633,7 +26700,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C10">
         <v>2459</v>
@@ -26644,7 +26711,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C11">
         <v>512</v>
@@ -26655,7 +26722,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C12">
         <v>33</v>
@@ -26664,7 +26731,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="30"/>
       <c r="B13" s="30" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C13" s="30">
         <f>SUM(C6:C12)</f>
@@ -26673,15 +26740,15 @@
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="59" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C18" s="58">
         <v>2020</v>
@@ -26693,7 +26760,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C19">
         <v>20928</v>
@@ -26704,7 +26771,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C20">
         <v>727</v>
@@ -26715,7 +26782,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C21">
         <v>29</v>
@@ -26726,7 +26793,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C22">
         <v>27</v>
@@ -26737,7 +26804,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -26748,7 +26815,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -26759,7 +26826,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -26770,7 +26837,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -26779,7 +26846,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="30"/>
       <c r="B27" s="30" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C27" s="30">
         <f>SUM(C19:C26)</f>
@@ -26788,15 +26855,15 @@
     </row>
     <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="59" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C32" s="58">
         <v>2020</v>
@@ -26807,7 +26874,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C33">
         <v>2043</v>
@@ -26818,7 +26885,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C34">
         <v>16</v>
@@ -26829,7 +26896,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -26840,7 +26907,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -26849,7 +26916,7 @@
     <row r="37" spans="1:29">
       <c r="A37" s="30"/>
       <c r="B37" s="30" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C37" s="30">
         <f>SUM(C33:C36)</f>
@@ -26858,7 +26925,7 @@
     </row>
     <row r="40" spans="1:29" ht="15.75">
       <c r="B40" s="57" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -26947,7 +27014,7 @@
     </row>
     <row r="42" spans="1:29">
       <c r="B42" s="55" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C42" s="54">
         <v>4857000.0000000037</v>
@@ -27033,7 +27100,7 @@
     </row>
     <row r="43" spans="1:29">
       <c r="B43" s="52" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C43" s="53">
         <v>0.99999999999999956</v>
@@ -27119,7 +27186,7 @@
     </row>
     <row r="44" spans="1:29">
       <c r="B44" s="51" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
@@ -27150,629 +27217,629 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="377" t="s">
-        <v>384</v>
-      </c>
-      <c r="C49" s="377"/>
+      <c r="B49" s="378" t="s">
+        <v>382</v>
+      </c>
+      <c r="C49" s="378"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" thickBot="1">
       <c r="B51" s="47" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C51" s="46"/>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C52" s="43"/>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" s="21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C55" s="43"/>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58" s="21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="21" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="B62" s="21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="B66" s="21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="21" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" s="21" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="21" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" s="21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="B72" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="B73" s="21" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="43" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C75" s="43"/>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" s="21" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="B77" s="21" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="2:3">
       <c r="B78" s="21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" s="21" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" s="21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="84" spans="2:3">
       <c r="B84" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" s="21" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" s="21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" s="21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="B89" s="21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" s="21" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" s="21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="B92" s="21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="B93" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="B94" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="B95" s="43" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C95" s="43"/>
     </row>
     <row r="96" spans="2:3">
       <c r="B96" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="B98" s="21" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="99" spans="2:3">
       <c r="B99" s="21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="B100" s="21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="2:3">
       <c r="B101" s="43" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C101" s="43"/>
     </row>
     <row r="102" spans="2:3">
       <c r="B102" s="21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="2:3">
       <c r="B103" s="21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="B104" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="B105" s="45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C105" s="44"/>
     </row>
     <row r="106" spans="2:3">
       <c r="B106" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C106" s="43"/>
     </row>
     <row r="107" spans="2:3">
       <c r="B107" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C108" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="2:3">
       <c r="B109" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="21" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="21" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="43" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C114" s="43"/>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="117" spans="2:3">
       <c r="B117" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="118" spans="2:3">
       <c r="B118" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="2:3">
       <c r="B119" s="21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="2:3">
       <c r="B120" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C120" s="21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="43" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C122" s="43"/>
     </row>
     <row r="123" spans="2:3">
       <c r="B123" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="2:3">
       <c r="B124" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="2:3">
       <c r="B125" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C125" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="126" spans="2:3">
       <c r="B126" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" spans="2:3">
       <c r="B127" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="128" spans="2:3">
       <c r="B128" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -27791,11 +27858,11 @@
   <dimension ref="A1:AS80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="U56" sqref="U56"/>
+      <selection pane="bottomRight" activeCell="AP58" sqref="AP58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -28970,7 +29037,7 @@
     </row>
     <row r="10" spans="1:45" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -29052,7 +29119,7 @@
     </row>
     <row r="11" spans="1:45" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -29132,7 +29199,7 @@
     </row>
     <row r="12" spans="1:45" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -29184,7 +29251,7 @@
     </row>
     <row r="13" spans="1:45" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -29248,7 +29315,7 @@
     </row>
     <row r="14" spans="1:45" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -29490,7 +29557,7 @@
     </row>
     <row r="16" spans="1:45" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -29554,7 +29621,7 @@
     </row>
     <row r="17" spans="1:45" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -29618,7 +29685,7 @@
     </row>
     <row r="18" spans="1:45" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -29670,7 +29737,7 @@
     </row>
     <row r="19" spans="1:45" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -29731,7 +29798,7 @@
     </row>
     <row r="20" spans="1:45" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -29976,7 +30043,7 @@
     </row>
     <row r="22" spans="1:45" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -30040,7 +30107,7 @@
     </row>
     <row r="23" spans="1:45" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -30090,7 +30157,7 @@
     </row>
     <row r="24" spans="1:45" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -34733,7 +34800,7 @@
     </row>
     <row r="74" spans="1:45" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -34778,7 +34845,7 @@
     </row>
     <row r="75" spans="1:45" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -36249,7 +36316,7 @@
     </row>
     <row r="10" spans="1:44" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -36331,7 +36398,7 @@
     </row>
     <row r="11" spans="1:44" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -36411,7 +36478,7 @@
     </row>
     <row r="12" spans="1:44" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -36463,7 +36530,7 @@
     </row>
     <row r="13" spans="1:44" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -36527,7 +36594,7 @@
     </row>
     <row r="14" spans="1:44" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -36768,7 +36835,7 @@
     </row>
     <row r="16" spans="1:44" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -36832,7 +36899,7 @@
     </row>
     <row r="17" spans="1:44" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -36896,7 +36963,7 @@
     </row>
     <row r="18" spans="1:44" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -36948,7 +37015,7 @@
     </row>
     <row r="19" spans="1:44" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -37009,7 +37076,7 @@
     </row>
     <row r="20" spans="1:44" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -37254,7 +37321,7 @@
     </row>
     <row r="22" spans="1:44" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -37318,7 +37385,7 @@
     </row>
     <row r="23" spans="1:44" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -37368,7 +37435,7 @@
     </row>
     <row r="24" spans="1:44" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -41994,7 +42061,7 @@
     </row>
     <row r="74" spans="1:44" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -42041,7 +42108,7 @@
     </row>
     <row r="75" spans="1:44" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>

</xml_diff>

<commit_message>
Increase maximum electricity consumption in RSD in 2019
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479AC9AA-5569-4218-8B9F-29434FD3B2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7C9C23-1445-4576-AF0C-082E42413F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -5049,6 +5049,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5061,9 +5064,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6181,12 +6181,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="376" t="s">
+      <c r="A16" s="379" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="376"/>
-      <c r="C16" s="376"/>
-      <c r="D16" s="376"/>
+      <c r="B16" s="379"/>
+      <c r="C16" s="379"/>
+      <c r="D16" s="379"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6270,11 +6270,11 @@
       <c r="A19" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="375" t="s">
+      <c r="B19" s="378" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="375"/>
-      <c r="D19" s="375"/>
+      <c r="C19" s="378"/>
+      <c r="D19" s="378"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6302,11 +6302,11 @@
       <c r="A20" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="375" t="s">
+      <c r="B20" s="378" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="375"/>
-      <c r="D20" s="375"/>
+      <c r="C20" s="378"/>
+      <c r="D20" s="378"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6394,11 +6394,11 @@
       <c r="A23" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="375" t="s">
+      <c r="B23" s="378" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="375"/>
-      <c r="D23" s="375"/>
+      <c r="C23" s="378"/>
+      <c r="D23" s="378"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6424,11 +6424,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="375" t="s">
+      <c r="B24" s="378" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="375"/>
-      <c r="D24" s="375"/>
+      <c r="C24" s="378"/>
+      <c r="D24" s="378"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6486,11 +6486,11 @@
       <c r="A26" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="375" t="s">
+      <c r="B26" s="378" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="375"/>
-      <c r="D26" s="375"/>
+      <c r="C26" s="378"/>
+      <c r="D26" s="378"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6606,11 +6606,11 @@
       <c r="A30" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="377" t="s">
+      <c r="B30" s="380" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="375"/>
-      <c r="D30" s="375"/>
+      <c r="C30" s="378"/>
+      <c r="D30" s="378"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6638,11 +6638,11 @@
       <c r="A31" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="375" t="s">
+      <c r="B31" s="378" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="375"/>
-      <c r="D31" s="375"/>
+      <c r="C31" s="378"/>
+      <c r="D31" s="378"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -31686,7 +31686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07582334-99B5-48D6-84E8-990178E1C3A6}">
   <dimension ref="B3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -31749,26 +31749,26 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="380" t="s">
+      <c r="B8" s="376" t="s">
         <v>466</v>
       </c>
-      <c r="C8" s="380" t="s">
+      <c r="C8" s="376" t="s">
         <v>467</v>
       </c>
-      <c r="D8" s="380">
+      <c r="D8" s="376">
         <v>2019</v>
       </c>
-      <c r="E8" s="380" t="s">
+      <c r="E8" s="376" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="380">
+      <c r="F8" s="376">
         <v>1</v>
       </c>
-      <c r="G8" s="381">
+      <c r="G8" s="377">
         <f>4.015-0.025</f>
         <v>3.9899999999999998</v>
       </c>
-      <c r="H8" s="380" t="s">
+      <c r="H8" s="376" t="s">
         <v>471</v>
       </c>
     </row>
@@ -31787,7 +31787,7 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="379">
+      <c r="G9" s="375">
         <f>4.3-0.025</f>
         <v>4.2749999999999995</v>
       </c>
@@ -31807,7 +31807,7 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="379">
+      <c r="G10" s="375">
         <v>4.5</v>
       </c>
     </row>
@@ -31826,7 +31826,7 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="379">
+      <c r="G11" s="375">
         <v>4.7</v>
       </c>
     </row>
@@ -31847,25 +31847,25 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="380" t="s">
+      <c r="B13" s="376" t="s">
         <v>469</v>
       </c>
-      <c r="C13" s="380" t="s">
+      <c r="C13" s="376" t="s">
         <v>472</v>
       </c>
-      <c r="D13" s="380">
+      <c r="D13" s="376">
         <v>2019</v>
       </c>
-      <c r="E13" s="380" t="s">
+      <c r="E13" s="376" t="s">
         <v>223</v>
       </c>
-      <c r="F13" s="380">
+      <c r="F13" s="376">
         <v>1</v>
       </c>
-      <c r="G13" s="381">
+      <c r="G13" s="377">
         <v>0.02</v>
       </c>
-      <c r="H13" s="380" t="s">
+      <c r="H13" s="376" t="s">
         <v>470</v>
       </c>
     </row>
@@ -31884,7 +31884,7 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" s="379">
+      <c r="G14" s="375">
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
@@ -31903,7 +31903,7 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="379">
+      <c r="G15" s="375">
         <v>0.26100000000000001</v>
       </c>
     </row>
@@ -31922,7 +31922,7 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" s="379">
+      <c r="G16" s="375">
         <v>0.38400000000000001</v>
       </c>
     </row>
@@ -31951,8 +31951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
   <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32141,8 +32141,8 @@
         <v>29.5</v>
       </c>
       <c r="G8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)</f>
-        <v>29.3</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
+        <v>30.8</v>
       </c>
       <c r="H8" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
@@ -34797,10 +34797,10 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="378" t="s">
+      <c r="B49" s="381" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="378"/>
+      <c r="C49" s="381"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">

</xml_diff>

<commit_message>
Limit coal consumption in PWR to 30 PJ in 2022 and onwards
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7C9C23-1445-4576-AF0C-082E42413F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18304D-82FC-4DD7-8A33-04AAD2799907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -1674,7 +1674,7 @@
     <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1884,6 +1884,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -4007,7 +4014,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="382">
+  <cellXfs count="383">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5064,6 +5071,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -31306,10 +31314,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FEB92-3C8E-4A89-8F18-2AEFFF284423}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="B2:J14"/>
+  <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31319,13 +31327,13 @@
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:11">
       <c r="B2" s="28" t="s">
         <v>199</v>
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -31351,10 +31359,13 @@
         <v>2021</v>
       </c>
       <c r="J3" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
+        <v>2022</v>
+      </c>
+      <c r="K3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
       <c r="C4" t="s">
         <v>202</v>
       </c>
@@ -31381,11 +31392,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AG$10,'EB2021'!$AG$11,'EB2021'!$AH$10,'EB2021'!$AH$11),1)</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="19"/>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:11">
       <c r="C5" t="s">
         <v>203</v>
       </c>
@@ -31412,11 +31424,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$10,'EB2021'!$AE$11),1)</f>
         <v>4.3</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="19"/>
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:11">
       <c r="C6" t="s">
         <v>201</v>
       </c>
@@ -31443,11 +31456,14 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$10,'EB2021'!$C$11),1)</f>
         <v>28.200000000000003</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+      <c r="J6" s="382">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
         <v>456</v>
       </c>
@@ -31465,11 +31481,12 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7">
+      <c r="J7" s="19"/>
+      <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:11">
       <c r="C8" t="s">
         <v>204</v>
       </c>
@@ -31496,11 +31513,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$10,'EB2021'!$AA$11),1)</f>
         <v>98.1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="19"/>
+      <c r="K8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
         <v>456</v>
       </c>
@@ -31518,11 +31536,12 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9">
+      <c r="J9" s="19"/>
+      <c r="K9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:11">
       <c r="C10" t="s">
         <v>205</v>
       </c>
@@ -31549,11 +31568,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AC$22),1)</f>
         <v>2.7</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="19"/>
+      <c r="K10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:11">
       <c r="C11" t="s">
         <v>206</v>
       </c>
@@ -31580,11 +31600,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AF$10,'EB2021'!$AF$11,'EB2021'!$AN$10,'EB2021'!$AN$11),1)</f>
         <v>7.8</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="19"/>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:11">
       <c r="C12" t="s">
         <v>207</v>
       </c>
@@ -31611,11 +31632,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$10,'EB2021'!$H$11),1)</f>
         <v>3</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="19"/>
+      <c r="K12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:11">
       <c r="C13" t="s">
         <v>208</v>
       </c>
@@ -31642,11 +31664,12 @@
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AK$22),1)</f>
         <v>0.4</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="19"/>
+      <c r="K13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:11">
       <c r="C14" t="s">
         <v>209</v>
       </c>
@@ -31673,12 +31696,14 @@
         <f>ROUNDUP(Conversions!$B$2*SUM(-'EB2021'!$AD$22),1)</f>
         <v>35.200000000000003</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="19"/>
+      <c r="K14">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31951,8 +31976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
   <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Apply DH restriction to all steps in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18304D-82FC-4DD7-8A33-04AAD2799907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC660391-BB3A-47C8-B4ED-B8E884858A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -885,9 +885,6 @@
     <t>FT-SRVLPG</t>
   </si>
   <si>
-    <t>FT-SRVHET</t>
-  </si>
-  <si>
     <t>FT-SRVETH</t>
   </si>
   <si>
@@ -1658,6 +1655,9 @@
   </si>
   <si>
     <t>P*SOL*PV*</t>
+  </si>
+  <si>
+    <t>FT-SRVHET*</t>
   </si>
 </sst>
 </file>
@@ -5059,6 +5059,7 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5071,7 +5072,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6189,12 +6189,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="379" t="s">
-        <v>404</v>
-      </c>
-      <c r="B16" s="379"/>
-      <c r="C16" s="379"/>
-      <c r="D16" s="379"/>
+      <c r="A16" s="380" t="s">
+        <v>403</v>
+      </c>
+      <c r="B16" s="380"/>
+      <c r="C16" s="380"/>
+      <c r="D16" s="380"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6276,13 +6276,13 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1">
       <c r="A19" s="67" t="s">
-        <v>405</v>
-      </c>
-      <c r="B19" s="378" t="s">
-        <v>416</v>
-      </c>
-      <c r="C19" s="378"/>
-      <c r="D19" s="378"/>
+        <v>404</v>
+      </c>
+      <c r="B19" s="379" t="s">
+        <v>415</v>
+      </c>
+      <c r="C19" s="379"/>
+      <c r="D19" s="379"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6308,13 +6308,13 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1">
       <c r="A20" s="67" t="s">
-        <v>406</v>
-      </c>
-      <c r="B20" s="378" t="s">
-        <v>419</v>
-      </c>
-      <c r="C20" s="378"/>
-      <c r="D20" s="378"/>
+        <v>405</v>
+      </c>
+      <c r="B20" s="379" t="s">
+        <v>418</v>
+      </c>
+      <c r="C20" s="379"/>
+      <c r="D20" s="379"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6340,10 +6340,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1">
       <c r="A21" s="67" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C21" s="70"/>
       <c r="D21" s="70"/>
@@ -6400,13 +6400,13 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1">
       <c r="A23" s="67" t="s">
-        <v>408</v>
-      </c>
-      <c r="B23" s="378" t="s">
-        <v>418</v>
-      </c>
-      <c r="C23" s="378"/>
-      <c r="D23" s="378"/>
+        <v>407</v>
+      </c>
+      <c r="B23" s="379" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" s="379"/>
+      <c r="D23" s="379"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6432,11 +6432,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="378" t="s">
-        <v>417</v>
-      </c>
-      <c r="C24" s="378"/>
-      <c r="D24" s="378"/>
+      <c r="B24" s="379" t="s">
+        <v>416</v>
+      </c>
+      <c r="C24" s="379"/>
+      <c r="D24" s="379"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6463,7 +6463,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1">
       <c r="A25" s="67"/>
       <c r="B25" s="70" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
@@ -6492,13 +6492,13 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1">
       <c r="A26" s="67" t="s">
-        <v>409</v>
-      </c>
-      <c r="B26" s="378" t="s">
-        <v>418</v>
-      </c>
-      <c r="C26" s="378"/>
-      <c r="D26" s="378"/>
+        <v>408</v>
+      </c>
+      <c r="B26" s="379" t="s">
+        <v>417</v>
+      </c>
+      <c r="C26" s="379"/>
+      <c r="D26" s="379"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1">
       <c r="A29" s="67" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B29" s="71">
         <v>1</v>
@@ -6612,13 +6612,13 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1">
       <c r="A30" s="67" t="s">
+        <v>410</v>
+      </c>
+      <c r="B30" s="381" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="380" t="s">
-        <v>412</v>
-      </c>
-      <c r="C30" s="378"/>
-      <c r="D30" s="378"/>
+      <c r="C30" s="379"/>
+      <c r="D30" s="379"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6644,13 +6644,13 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1">
       <c r="A31" s="67" t="s">
+        <v>412</v>
+      </c>
+      <c r="B31" s="379" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="378" t="s">
-        <v>414</v>
-      </c>
-      <c r="C31" s="378"/>
-      <c r="D31" s="378"/>
+      <c r="C31" s="379"/>
+      <c r="D31" s="379"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -6677,7 +6677,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1">
       <c r="A32" s="73"/>
       <c r="B32" s="74" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
@@ -9781,7 +9781,7 @@
     </row>
     <row r="10" spans="1:44" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -9863,7 +9863,7 @@
     </row>
     <row r="11" spans="1:44" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -9943,7 +9943,7 @@
     </row>
     <row r="12" spans="1:44" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -9995,7 +9995,7 @@
     </row>
     <row r="13" spans="1:44" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -10059,7 +10059,7 @@
     </row>
     <row r="14" spans="1:44" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -10300,7 +10300,7 @@
     </row>
     <row r="16" spans="1:44" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -10364,7 +10364,7 @@
     </row>
     <row r="17" spans="1:44" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -10428,7 +10428,7 @@
     </row>
     <row r="18" spans="1:44" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -10480,7 +10480,7 @@
     </row>
     <row r="19" spans="1:44" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -10541,7 +10541,7 @@
     </row>
     <row r="20" spans="1:44" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -10786,7 +10786,7 @@
     </row>
     <row r="22" spans="1:44" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -10850,7 +10850,7 @@
     </row>
     <row r="23" spans="1:44" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -10900,7 +10900,7 @@
     </row>
     <row r="24" spans="1:44" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -15526,7 +15526,7 @@
     </row>
     <row r="74" spans="1:44" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -15573,7 +15573,7 @@
     </row>
     <row r="75" spans="1:44" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -17037,7 +17037,7 @@
     </row>
     <row r="10" spans="1:43" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -17119,7 +17119,7 @@
     </row>
     <row r="11" spans="1:43" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -17199,7 +17199,7 @@
     </row>
     <row r="12" spans="1:43" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -17251,7 +17251,7 @@
     </row>
     <row r="13" spans="1:43" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -17315,7 +17315,7 @@
     </row>
     <row r="14" spans="1:43" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -17555,7 +17555,7 @@
     </row>
     <row r="16" spans="1:43" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -17619,7 +17619,7 @@
     </row>
     <row r="17" spans="1:43" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -17683,7 +17683,7 @@
     </row>
     <row r="18" spans="1:43" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -17735,7 +17735,7 @@
     </row>
     <row r="19" spans="1:43" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -17796,7 +17796,7 @@
     </row>
     <row r="20" spans="1:43" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -18041,7 +18041,7 @@
     </row>
     <row r="22" spans="1:43" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -18105,7 +18105,7 @@
     </row>
     <row r="23" spans="1:43" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -18155,7 +18155,7 @@
     </row>
     <row r="24" spans="1:43" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -22765,7 +22765,7 @@
     </row>
     <row r="74" spans="1:43" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -22812,7 +22812,7 @@
     </row>
     <row r="75" spans="1:43" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -22906,7 +22906,7 @@
     </row>
     <row r="77" spans="1:43" ht="15">
       <c r="A77" s="365" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B77" s="362"/>
       <c r="C77" s="23"/>
@@ -22953,7 +22953,7 @@
     </row>
     <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B78" s="362"/>
       <c r="C78" s="23"/>
@@ -23238,7 +23238,7 @@
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
       <c r="A1" s="75" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B1" s="76" t="s">
         <v>160</v>
@@ -24359,7 +24359,7 @@
     </row>
     <row r="10" spans="1:43" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -24441,7 +24441,7 @@
     </row>
     <row r="11" spans="1:43" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -24521,7 +24521,7 @@
     </row>
     <row r="12" spans="1:43" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -24573,7 +24573,7 @@
     </row>
     <row r="13" spans="1:43" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -24637,7 +24637,7 @@
     </row>
     <row r="14" spans="1:43" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -24877,7 +24877,7 @@
     </row>
     <row r="16" spans="1:43" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -24941,7 +24941,7 @@
     </row>
     <row r="17" spans="1:43" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -25005,7 +25005,7 @@
     </row>
     <row r="18" spans="1:43" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -25057,7 +25057,7 @@
     </row>
     <row r="19" spans="1:43" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -25118,7 +25118,7 @@
     </row>
     <row r="20" spans="1:43" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -25363,7 +25363,7 @@
     </row>
     <row r="22" spans="1:43" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -25427,7 +25427,7 @@
     </row>
     <row r="23" spans="1:43" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -25477,7 +25477,7 @@
     </row>
     <row r="24" spans="1:43" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -30087,7 +30087,7 @@
     </row>
     <row r="74" spans="1:43" ht="12.75" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -30134,7 +30134,7 @@
     </row>
     <row r="75" spans="1:43" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
@@ -30181,7 +30181,7 @@
     </row>
     <row r="76" spans="1:43" ht="12.75" customHeight="1">
       <c r="A76" s="363" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B76" s="364"/>
       <c r="C76" s="23"/>
@@ -30228,7 +30228,7 @@
     </row>
     <row r="77" spans="1:43" ht="15">
       <c r="A77" s="365" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B77" s="362"/>
       <c r="C77" s="23"/>
@@ -30275,7 +30275,7 @@
     </row>
     <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B78" s="362"/>
       <c r="C78" s="23"/>
@@ -31316,8 +31316,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31335,7 +31335,7 @@
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>197</v>
@@ -31456,7 +31456,7 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$10,'EB2021'!$C$11),1)</f>
         <v>28.200000000000003</v>
       </c>
-      <c r="J6" s="382">
+      <c r="J6" s="378">
         <v>30</v>
       </c>
       <c r="K6">
@@ -31465,10 +31465,10 @@
     </row>
     <row r="7" spans="2:11">
       <c r="B7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D7" t="s">
         <v>200</v>
@@ -31520,10 +31520,10 @@
     </row>
     <row r="9" spans="2:11">
       <c r="B9" t="s">
+        <v>455</v>
+      </c>
+      <c r="C9" t="s">
         <v>456</v>
-      </c>
-      <c r="C9" t="s">
-        <v>457</v>
       </c>
       <c r="D9" t="s">
         <v>200</v>
@@ -31734,57 +31734,57 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="2:8">
       <c r="E5" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
       <c r="B6" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>461</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>465</v>
-      </c>
-      <c r="G6" s="29" t="s">
+      <c r="H6" s="29" t="s">
         <v>462</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="376" t="s">
+        <v>465</v>
+      </c>
+      <c r="C8" s="376" t="s">
         <v>466</v>
-      </c>
-      <c r="C8" s="376" t="s">
-        <v>467</v>
       </c>
       <c r="D8" s="376">
         <v>2019</v>
       </c>
       <c r="E8" s="376" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F8" s="376">
         <v>1</v>
@@ -31794,7 +31794,7 @@
         <v>3.9899999999999998</v>
       </c>
       <c r="H8" s="376" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -31873,16 +31873,16 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="376" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C13" s="376" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D13" s="376">
         <v>2019</v>
       </c>
       <c r="E13" s="376" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F13" s="376">
         <v>1</v>
@@ -31891,7 +31891,7 @@
         <v>0.02</v>
       </c>
       <c r="H13" s="376" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -31977,7 +31977,7 @@
   <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31996,7 +31996,7 @@
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>197</v>
@@ -32025,10 +32025,10 @@
     </row>
     <row r="4" spans="2:10">
       <c r="B4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D4" t="s">
         <v>200</v>
@@ -32059,7 +32059,7 @@
     </row>
     <row r="5" spans="2:10">
       <c r="C5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
         <v>200</v>
@@ -32090,7 +32090,7 @@
     </row>
     <row r="6" spans="2:10">
       <c r="C6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D6" t="s">
         <v>200</v>
@@ -32121,7 +32121,7 @@
     </row>
     <row r="7" spans="2:10">
       <c r="C7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D7" t="s">
         <v>200</v>
@@ -32152,7 +32152,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="C8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D8" t="s">
         <v>200</v>
@@ -32183,10 +32183,10 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D9" t="s">
         <v>200</v>
@@ -32217,7 +32217,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="C10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D10" t="s">
         <v>200</v>
@@ -32248,10 +32248,10 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D11" t="s">
         <v>200</v>
@@ -32282,7 +32282,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="C12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D12" t="s">
         <v>200</v>
@@ -32313,7 +32313,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="C13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D13" t="s">
         <v>200</v>
@@ -32344,7 +32344,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="C14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D14" t="s">
         <v>200</v>
@@ -32383,8 +32383,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32403,7 +32403,7 @@
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>197</v>
@@ -32587,7 +32587,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="C9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
         <v>200</v>
@@ -32649,7 +32649,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="C11" t="s">
-        <v>219</v>
+        <v>472</v>
       </c>
       <c r="D11" t="s">
         <v>200</v>
@@ -32799,17 +32799,17 @@
   <sheetData>
     <row r="1" spans="1:34" ht="21">
       <c r="A1" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:34">
       <c r="B5" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="39"/>
@@ -32821,16 +32821,16 @@
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1">
       <c r="B6" s="38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>198</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F6" s="37" t="str">
         <f>Regions!C$3</f>
@@ -32941,18 +32941,18 @@
         <v>IE-MN</v>
       </c>
       <c r="AG6" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AH6" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:34">
       <c r="C7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E7">
         <v>2020</v>
@@ -33070,15 +33070,15 @@
         <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="AH7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:34">
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8">
         <v>2020</v>
@@ -33196,15 +33196,15 @@
         <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="AH8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:34">
       <c r="C9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9">
         <v>2020</v>
@@ -33322,15 +33322,15 @@
         <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="AH9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:34">
       <c r="C10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10">
         <v>2020</v>
@@ -33448,15 +33448,15 @@
         <v>T-CAR-BEV100_ELC21</v>
       </c>
       <c r="AH10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="C11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E11">
         <v>2020</v>
@@ -33574,15 +33574,15 @@
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="AH11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="C12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12">
         <v>2020</v>
@@ -33700,15 +33700,15 @@
         <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="AH12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="C13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E13">
         <v>2020</v>
@@ -33826,15 +33826,15 @@
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="AH13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E14">
         <v>2020</v>
@@ -33952,15 +33952,15 @@
         <v>T-LGT-ICE_DST61</v>
       </c>
       <c r="AH14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="C15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E15">
         <v>2020</v>
@@ -34078,16 +34078,16 @@
         <v>T-LGT-BEV_ELC61</v>
       </c>
       <c r="AH15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E16" s="30">
         <v>2020</v>
@@ -34205,7 +34205,7 @@
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="AH16" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -34232,25 +34232,25 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="59" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="59" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="58" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C5" s="58">
         <v>2020</v>
@@ -34261,7 +34261,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C6">
         <v>38233</v>
@@ -34272,7 +34272,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C7">
         <v>32600</v>
@@ -34283,7 +34283,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C8">
         <v>10474</v>
@@ -34294,7 +34294,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C9">
         <v>4013</v>
@@ -34305,7 +34305,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C10">
         <v>2459</v>
@@ -34316,7 +34316,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C11">
         <v>512</v>
@@ -34327,7 +34327,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C12">
         <v>33</v>
@@ -34336,7 +34336,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="30"/>
       <c r="B13" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C13" s="30">
         <f>SUM(C6:C12)</f>
@@ -34345,15 +34345,15 @@
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="59" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="58" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C18" s="58">
         <v>2020</v>
@@ -34365,7 +34365,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C19">
         <v>20928</v>
@@ -34376,7 +34376,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C20">
         <v>727</v>
@@ -34387,7 +34387,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C21">
         <v>29</v>
@@ -34398,7 +34398,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C22">
         <v>27</v>
@@ -34409,7 +34409,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -34420,7 +34420,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -34431,7 +34431,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -34442,7 +34442,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -34451,7 +34451,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="30"/>
       <c r="B27" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C27" s="30">
         <f>SUM(C19:C26)</f>
@@ -34460,15 +34460,15 @@
     </row>
     <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="59" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="58" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C32" s="58">
         <v>2020</v>
@@ -34479,7 +34479,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C33">
         <v>2043</v>
@@ -34490,7 +34490,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C34">
         <v>16</v>
@@ -34501,7 +34501,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -34512,7 +34512,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -34521,7 +34521,7 @@
     <row r="37" spans="1:29">
       <c r="A37" s="30"/>
       <c r="B37" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C37" s="30">
         <f>SUM(C33:C36)</f>
@@ -34530,7 +34530,7 @@
     </row>
     <row r="40" spans="1:29" ht="15.75">
       <c r="B40" s="57" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -34619,7 +34619,7 @@
     </row>
     <row r="42" spans="1:29">
       <c r="B42" s="55" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C42" s="54">
         <v>4857000.0000000037</v>
@@ -34705,7 +34705,7 @@
     </row>
     <row r="43" spans="1:29">
       <c r="B43" s="52" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C43" s="53">
         <v>0.99999999999999956</v>
@@ -34791,7 +34791,7 @@
     </row>
     <row r="44" spans="1:29">
       <c r="B44" s="51" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
@@ -34822,629 +34822,629 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="381" t="s">
-        <v>382</v>
-      </c>
-      <c r="C49" s="381"/>
+      <c r="B49" s="382" t="s">
+        <v>381</v>
+      </c>
+      <c r="C49" s="382"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" thickBot="1">
       <c r="B51" s="47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C51" s="46"/>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" s="43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C52" s="43"/>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C55" s="43"/>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58" s="21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="21" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="B62" s="21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="B66" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="21" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="B72" s="21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="B73" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C75" s="43"/>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="B77" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="78" spans="2:3">
       <c r="B78" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84" spans="2:3">
       <c r="B84" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" s="21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="B89" s="21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="B92" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="B93" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="B94" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="B95" s="43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C95" s="43"/>
     </row>
     <row r="96" spans="2:3">
       <c r="B96" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="B98" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="99" spans="2:3">
       <c r="B99" s="21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="B100" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" spans="2:3">
       <c r="B101" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C101" s="43"/>
     </row>
     <row r="102" spans="2:3">
       <c r="B102" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="2:3">
       <c r="B103" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="B104" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="B105" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C105" s="44"/>
     </row>
     <row r="106" spans="2:3">
       <c r="B106" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C106" s="43"/>
     </row>
     <row r="107" spans="2:3">
       <c r="B107" s="21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C108" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="109" spans="2:3">
       <c r="B109" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C114" s="43"/>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="117" spans="2:3">
       <c r="B117" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="118" spans="2:3">
       <c r="B118" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="2:3">
       <c r="B119" s="21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="120" spans="2:3">
       <c r="B120" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C120" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C122" s="43"/>
     </row>
     <row r="123" spans="2:3">
       <c r="B123" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="2:3">
       <c r="B124" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="125" spans="2:3">
       <c r="B125" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C125" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" spans="2:3">
       <c r="B126" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="2:3">
       <c r="B127" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="2:3">
       <c r="B128" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -36642,7 +36642,7 @@
     </row>
     <row r="10" spans="1:45" ht="12.75" customHeight="1">
       <c r="A10" s="152" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B10" s="153"/>
       <c r="C10" s="154">
@@ -36724,7 +36724,7 @@
     </row>
     <row r="11" spans="1:45" ht="12.75" customHeight="1">
       <c r="A11" s="101" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B11" s="102"/>
       <c r="C11" s="103">
@@ -36804,7 +36804,7 @@
     </row>
     <row r="12" spans="1:45" ht="12.75" customHeight="1">
       <c r="A12" s="101" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B12" s="102"/>
       <c r="C12" s="103"/>
@@ -36856,7 +36856,7 @@
     </row>
     <row r="13" spans="1:45" ht="12.75" customHeight="1">
       <c r="A13" s="101" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B13" s="102"/>
       <c r="C13" s="103">
@@ -36920,7 +36920,7 @@
     </row>
     <row r="14" spans="1:45" ht="12.75" customHeight="1">
       <c r="A14" s="165" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B14" s="166"/>
       <c r="C14" s="167">
@@ -37162,7 +37162,7 @@
     </row>
     <row r="16" spans="1:45" ht="12.75" customHeight="1">
       <c r="A16" s="152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B16" s="153"/>
       <c r="C16" s="154">
@@ -37226,7 +37226,7 @@
     </row>
     <row r="17" spans="1:45" ht="12.75" customHeight="1">
       <c r="A17" s="101" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="102"/>
       <c r="C17" s="103">
@@ -37290,7 +37290,7 @@
     </row>
     <row r="18" spans="1:45" ht="12.75" customHeight="1">
       <c r="A18" s="101" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B18" s="102"/>
       <c r="C18" s="103"/>
@@ -37342,7 +37342,7 @@
     </row>
     <row r="19" spans="1:45" ht="12.75" customHeight="1">
       <c r="A19" s="101" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B19" s="102"/>
       <c r="C19" s="103"/>
@@ -37403,7 +37403,7 @@
     </row>
     <row r="20" spans="1:45" ht="12.75" customHeight="1">
       <c r="A20" s="165" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="167"/>
@@ -37648,7 +37648,7 @@
     </row>
     <row r="22" spans="1:45" ht="12.75" customHeight="1">
       <c r="A22" s="152" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="153"/>
       <c r="C22" s="203"/>
@@ -37712,7 +37712,7 @@
     </row>
     <row r="23" spans="1:45" ht="12.75" customHeight="1">
       <c r="A23" s="207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="178"/>
       <c r="C23" s="208"/>
@@ -37762,7 +37762,7 @@
     </row>
     <row r="24" spans="1:45" ht="12.75" customHeight="1" thickBot="1">
       <c r="A24" s="116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="117"/>
       <c r="C24" s="217">
@@ -42405,7 +42405,7 @@
     </row>
     <row r="74" spans="1:45" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A74" s="207" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B74" s="185"/>
       <c r="C74" s="185"/>
@@ -42450,7 +42450,7 @@
     </row>
     <row r="75" spans="1:45" ht="12.75" customHeight="1">
       <c r="A75" s="362" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>

</xml_diff>

<commit_message>
Apply historical bounds to electricity exchange
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,31 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51BFB7D-B57D-4BE8-8B61-0CB83C802CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6FBEBB-C133-4C33-BF90-8C8AA431B303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
     <sheet name="Regions" sheetId="2" r:id="rId2"/>
-    <sheet name="PWR" sheetId="8" r:id="rId3"/>
-    <sheet name="PWR-CAPs" sheetId="24" r:id="rId4"/>
-    <sheet name="RSD" sheetId="23" r:id="rId5"/>
-    <sheet name="SRV" sheetId="14" r:id="rId6"/>
-    <sheet name="TRA" sheetId="15" r:id="rId7"/>
-    <sheet name="CO2-config" sheetId="27" r:id="rId8"/>
-    <sheet name="CO2-NET-single" sheetId="25" r:id="rId9"/>
-    <sheet name="CO2-NET-multi" sheetId="26" r:id="rId10"/>
-    <sheet name="New vehicle sales" sheetId="16" r:id="rId11"/>
-    <sheet name="EB2018" sheetId="3" r:id="rId12"/>
-    <sheet name="EB2019" sheetId="11" r:id="rId13"/>
-    <sheet name="EB2020" sheetId="12" r:id="rId14"/>
-    <sheet name="EB2021" sheetId="22" r:id="rId15"/>
-    <sheet name="Conversions" sheetId="9" r:id="rId16"/>
+    <sheet name="SUP" sheetId="28" r:id="rId3"/>
+    <sheet name="PWR" sheetId="8" r:id="rId4"/>
+    <sheet name="PWR-CAPs" sheetId="24" r:id="rId5"/>
+    <sheet name="RSD" sheetId="23" r:id="rId6"/>
+    <sheet name="SRV" sheetId="14" r:id="rId7"/>
+    <sheet name="TRA" sheetId="15" r:id="rId8"/>
+    <sheet name="CO2-config" sheetId="27" r:id="rId9"/>
+    <sheet name="CO2-NET-single" sheetId="25" r:id="rId10"/>
+    <sheet name="CO2-NET-multi" sheetId="26" r:id="rId11"/>
+    <sheet name="New vehicle sales" sheetId="16" r:id="rId12"/>
+    <sheet name="EB2018" sheetId="3" r:id="rId13"/>
+    <sheet name="EB2019" sheetId="11" r:id="rId14"/>
+    <sheet name="EB2020" sheetId="12" r:id="rId15"/>
+    <sheet name="EB2021" sheetId="22" r:id="rId16"/>
+    <sheet name="Conversions" sheetId="9" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId17"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -58,23 +56,23 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_Regression_Y" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
-    <definedName name="aa" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec2" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec3" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elecc" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -92,12 +90,12 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="12">'EB2019'!$A$1:$AQ$80</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="13">'EB2020'!$A$1:$AQ$76</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="14">'EB2021'!$A$1:$AQ$76</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="12">'EB2019'!$A:$B,'EB2019'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="13">'EB2020'!$A:$B,'EB2020'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="14">'EB2021'!$A:$B,'EB2021'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="13">'EB2019'!$A$1:$AQ$80</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="14">'EB2020'!$A$1:$AQ$76</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="15">'EB2021'!$A$1:$AQ$76</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="13">'EB2019'!$A:$B,'EB2019'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="14">'EB2020'!$A:$B,'EB2020'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="15">'EB2021'!$A:$B,'EB2021'!$1:$1</definedName>
     <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
     <definedName name="RiskAfterSimMacro" hidden="1">""</definedName>
     <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
@@ -120,11 +118,11 @@
     <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
     <definedName name="RiskUseFixedSeed" hidden="1">TRUE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
-    <definedName name="table6" localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="15" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -212,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="501">
   <si>
     <t>Development</t>
   </si>
@@ -1710,6 +1708,45 @@
   </si>
   <si>
     <t>LO</t>
+  </si>
+  <si>
+    <t>UC_IRE</t>
+  </si>
+  <si>
+    <t>*Pja</t>
+  </si>
+  <si>
+    <t>UC_Historic_IMPELC</t>
+  </si>
+  <si>
+    <t>UC_Historic_EXPELC</t>
+  </si>
+  <si>
+    <t>Historic electricity import</t>
+  </si>
+  <si>
+    <t>Historic electricity export</t>
+  </si>
+  <si>
+    <t>Pset_Set</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>IMPELC*</t>
+  </si>
+  <si>
+    <t>EXPELC*</t>
+  </si>
+  <si>
+    <t>imp</t>
+  </si>
+  <si>
+    <t>exp</t>
   </si>
 </sst>
 </file>
@@ -4073,7 +4110,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="389">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5119,6 +5156,12 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5131,12 +5174,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5536,130 +5574,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Regions"/>
-      <sheetName val="PWR"/>
-      <sheetName val="SRV"/>
-      <sheetName val="TRA"/>
-      <sheetName val="SYS-emi_single"/>
-      <sheetName val="SYS-emi_multi"/>
-      <sheetName val="emi_config"/>
-      <sheetName val="New vehicle sales"/>
-      <sheetName val="EB2018"/>
-      <sheetName val="EB2019"/>
-      <sheetName val="EB2020"/>
-      <sheetName val="Conversions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>IE</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>National</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>IE-CW</v>
-          </cell>
-          <cell r="F3" t="str">
-            <v>IE-D</v>
-          </cell>
-          <cell r="G3" t="str">
-            <v>IE-KE</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>IE-KK</v>
-          </cell>
-          <cell r="I3" t="str">
-            <v>IE-LS</v>
-          </cell>
-          <cell r="J3" t="str">
-            <v>IE-LD</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>IE-LH</v>
-          </cell>
-          <cell r="L3" t="str">
-            <v>IE-MH</v>
-          </cell>
-          <cell r="M3" t="str">
-            <v>IE-OY</v>
-          </cell>
-          <cell r="N3" t="str">
-            <v>IE-WH</v>
-          </cell>
-          <cell r="O3" t="str">
-            <v>IE-WX</v>
-          </cell>
-          <cell r="P3" t="str">
-            <v>IE-WW</v>
-          </cell>
-          <cell r="Q3" t="str">
-            <v>IE-CE</v>
-          </cell>
-          <cell r="R3" t="str">
-            <v>IE-CO</v>
-          </cell>
-          <cell r="S3" t="str">
-            <v>IE-KY</v>
-          </cell>
-          <cell r="T3" t="str">
-            <v>IE-LK</v>
-          </cell>
-          <cell r="U3" t="str">
-            <v>IE-TA</v>
-          </cell>
-          <cell r="V3" t="str">
-            <v>IE-WD</v>
-          </cell>
-          <cell r="W3" t="str">
-            <v>IE-G</v>
-          </cell>
-          <cell r="X3" t="str">
-            <v>IE-LM</v>
-          </cell>
-          <cell r="Y3" t="str">
-            <v>IE-MO</v>
-          </cell>
-          <cell r="Z3" t="str">
-            <v>IE-RN</v>
-          </cell>
-          <cell r="AA3" t="str">
-            <v>IE-SO</v>
-          </cell>
-          <cell r="AB3" t="str">
-            <v>IE-CN</v>
-          </cell>
-          <cell r="AC3" t="str">
-            <v>IE-DL</v>
-          </cell>
-          <cell r="AD3" t="str">
-            <v>IE-MN</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Balyk, Olexandr" id="{0EBAA6E2-D3EC-429B-B80A-AFBE5C02E277}" userId="Balyk, Olexandr" providerId="None"/>
@@ -6378,12 +6292,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="380" t="s">
+      <c r="A16" s="386" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="380"/>
-      <c r="C16" s="380"/>
-      <c r="D16" s="380"/>
+      <c r="B16" s="386"/>
+      <c r="C16" s="386"/>
+      <c r="D16" s="386"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6467,11 +6381,11 @@
       <c r="A19" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="379" t="s">
+      <c r="B19" s="385" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="379"/>
-      <c r="D19" s="379"/>
+      <c r="C19" s="385"/>
+      <c r="D19" s="385"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6499,11 +6413,11 @@
       <c r="A20" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="379" t="s">
+      <c r="B20" s="385" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="379"/>
-      <c r="D20" s="379"/>
+      <c r="C20" s="385"/>
+      <c r="D20" s="385"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6591,11 +6505,11 @@
       <c r="A23" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="379" t="s">
+      <c r="B23" s="385" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="379"/>
-      <c r="D23" s="379"/>
+      <c r="C23" s="385"/>
+      <c r="D23" s="385"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6621,11 +6535,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="379" t="s">
+      <c r="B24" s="385" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="379"/>
-      <c r="D24" s="379"/>
+      <c r="C24" s="385"/>
+      <c r="D24" s="385"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6683,11 +6597,11 @@
       <c r="A26" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="379" t="s">
+      <c r="B26" s="385" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="379"/>
-      <c r="D26" s="379"/>
+      <c r="C26" s="385"/>
+      <c r="D26" s="385"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6803,11 +6717,11 @@
       <c r="A30" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="381" t="s">
+      <c r="B30" s="387" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="379"/>
-      <c r="D30" s="379"/>
+      <c r="C30" s="385"/>
+      <c r="D30" s="385"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6835,11 +6749,11 @@
       <c r="A31" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="379" t="s">
+      <c r="B31" s="385" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="379"/>
-      <c r="D31" s="379"/>
+      <c r="C31" s="385"/>
+      <c r="D31" s="385"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -8791,6 +8705,167 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A43B5DB-8BF6-4C1B-AB8E-D3EEC4E992CB}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="379" t="str">
+        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
+        <v>~UC_Sets: R_E: IE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="379" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="G4" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="380" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="381" t="s">
+        <v>474</v>
+      </c>
+      <c r="D5" s="381" t="s">
+        <v>475</v>
+      </c>
+      <c r="E5" s="381" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="381" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="381" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="382" t="s">
+        <v>476</v>
+      </c>
+      <c r="I5" s="382" t="s">
+        <v>477</v>
+      </c>
+      <c r="J5" s="383" t="s">
+        <v>462</v>
+      </c>
+      <c r="K5" s="380" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="K6" s="384"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" t="str">
+        <f>VLOOKUP(B$5, 'CO2-config'!$B$4:$D$14,2,FALSE) &amp; "_Single"</f>
+        <v>UC_Emissions_CO2_2020_Single</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(C$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(D$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F7">
+        <v>2018</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(G$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>LO</v>
+      </c>
+      <c r="H7">
+        <f>VLOOKUP(H$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
+        <f>VLOOKUP(K$5, 'CO2-config'!$B$4:$D$14,2,FALSE) &amp; " - Single"</f>
+        <v>CO2 Emissions in 2020 - Single</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8" t="str">
+        <f>VLOOKUP(C$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(D$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E8" t="str">
+        <f>VLOOKUP(E$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F8">
+        <f>F7</f>
+        <v>2018</v>
+      </c>
+      <c r="I8">
+        <f>VLOOKUP(I$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F9,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A089DB7-F6A5-44DD-9B0D-8CBAFF1788E4}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -8818,13 +8893,13 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="383" t="str">
-        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!D3:AD3)</f>
+      <c r="B2" s="379" t="str">
+        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="383" t="s">
+      <c r="B3" s="379" t="s">
         <v>459</v>
       </c>
     </row>
@@ -8835,34 +8910,34 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="384" t="s">
+      <c r="B5" s="380" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="385" t="s">
+      <c r="C5" s="381" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="385" t="s">
+      <c r="D5" s="381" t="s">
         <v>475</v>
       </c>
-      <c r="E5" s="385" t="s">
+      <c r="E5" s="381" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="385" t="s">
+      <c r="F5" s="381" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="385" t="s">
+      <c r="G5" s="381" t="s">
         <v>227</v>
       </c>
-      <c r="H5" s="386" t="s">
+      <c r="H5" s="382" t="s">
         <v>476</v>
       </c>
-      <c r="I5" s="386" t="s">
+      <c r="I5" s="382" t="s">
         <v>477</v>
       </c>
-      <c r="J5" s="387" t="s">
+      <c r="J5" s="383" t="s">
         <v>480</v>
       </c>
-      <c r="K5" s="384" t="s">
+      <c r="K5" s="380" t="s">
         <v>463</v>
       </c>
     </row>
@@ -8952,7 +9027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12490C26-C7DC-403B-9901-8AE03883042B}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AC129"/>
@@ -9559,10 +9634,10 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="382" t="s">
+      <c r="B49" s="388" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="382"/>
+      <c r="C49" s="388"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
@@ -10192,7 +10267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6617C6-BD81-4C8E-89D7-FC0076ADEEA7}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
@@ -10200,7 +10275,7 @@
   <dimension ref="A1:AS80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
@@ -17478,7 +17553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEC878B-F7E3-4802-BC50-10F92160064D}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AR80"/>
@@ -24741,7 +24816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9945E26-E686-40E8-A01F-A87690AEE355}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AQ85"/>
@@ -32064,16 +32139,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4685A7-279E-44B2-B92C-436990F54D25}">
   <dimension ref="A1:AQ85"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="95" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="AO57" sqref="AO57"/>
+      <selection pane="bottomRight" activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -39386,7 +39461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A846FF-BBF5-4A02-BAF4-3C4772884C84}">
   <sheetPr codeName="Sheet9">
     <tabColor theme="0" tint="-0.499984740745262"/>
@@ -39428,8 +39503,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -40189,12 +40264,269 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89305455-607F-41AA-8109-096F19F6FE72}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="379" t="str">
+        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="379" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="H4" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="380" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="381" t="s">
+        <v>474</v>
+      </c>
+      <c r="D5" s="381" t="s">
+        <v>494</v>
+      </c>
+      <c r="E5" s="381" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="381" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="381" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="381" t="s">
+        <v>486</v>
+      </c>
+      <c r="I5" s="382" t="s">
+        <v>488</v>
+      </c>
+      <c r="J5" s="383" t="s">
+        <v>462</v>
+      </c>
+      <c r="K5" s="380" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="K6" s="384"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" t="s">
+        <v>495</v>
+      </c>
+      <c r="D7" t="s">
+        <v>496</v>
+      </c>
+      <c r="E7" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7">
+        <v>2018</v>
+      </c>
+      <c r="G7" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="389">
+        <f>Conversions!$B$2*'EB2018'!$AO$3</f>
+        <v>5.8385184241824009</v>
+      </c>
+      <c r="K7" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8" s="389">
+        <f>Conversions!$B$2*'EB2019'!$AO$3</f>
+        <v>7.8478965511531191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9" t="s">
+        <v>223</v>
+      </c>
+      <c r="J9" s="389">
+        <f>Conversions!$B$2*'EB2020'!$AO$3</f>
+        <v>6.3411436804464003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10">
+        <v>2021</v>
+      </c>
+      <c r="G10" t="s">
+        <v>223</v>
+      </c>
+      <c r="J10" s="389">
+        <f>Conversions!$B$2*'EB2021'!$AO$3</f>
+        <v>8.8241634675727223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>223</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" t="s">
+        <v>491</v>
+      </c>
+      <c r="C12" t="s">
+        <v>495</v>
+      </c>
+      <c r="D12" t="s">
+        <v>496</v>
+      </c>
+      <c r="E12" t="s">
+        <v>498</v>
+      </c>
+      <c r="F12">
+        <v>2018</v>
+      </c>
+      <c r="G12" t="s">
+        <v>223</v>
+      </c>
+      <c r="H12" t="s">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="389">
+        <f>Conversions!$B$2*'EB2018'!$AO$4</f>
+        <v>5.9383641411770398</v>
+      </c>
+      <c r="K12" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="F13">
+        <v>2019</v>
+      </c>
+      <c r="G13" t="s">
+        <v>223</v>
+      </c>
+      <c r="J13" s="389">
+        <f>Conversions!$B$2*'EB2019'!$AO$4</f>
+        <v>5.5271334489739186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14">
+        <v>2020</v>
+      </c>
+      <c r="G14" t="s">
+        <v>223</v>
+      </c>
+      <c r="J14" s="389">
+        <f>Conversions!$B$2*'EB2020'!$AO$4</f>
+        <v>6.8879157977152801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15">
+        <v>2021</v>
+      </c>
+      <c r="G15" t="s">
+        <v>223</v>
+      </c>
+      <c r="J15" s="389">
+        <f>Conversions!$B$2*'EB2021'!$AO$4</f>
+        <v>3.1077995112374399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>223</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FEB92-3C8E-4A89-8F18-2AEFFF284423}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40584,12 +40916,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07582334-99B5-48D6-84E8-990178E1C3A6}">
   <dimension ref="B3:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40849,7 +41181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
   <dimension ref="B2:J14"/>
   <sheetViews>
@@ -41255,7 +41587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J14"/>
@@ -41654,7 +41986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC29CEA2-2536-449C-BE94-1AB8A11FBF6A}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AH16"/>
@@ -43092,7 +43424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40162BAB-2A61-4FF8-AC40-4BD254BCBC14}">
   <dimension ref="B4:D14"/>
   <sheetViews>
@@ -43205,165 +43537,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A43B5DB-8BF6-4C1B-AB8E-D3EEC4E992CB}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" s="383" t="str">
-        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3)</f>
-        <v>~UC_Sets: R_E: IE</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="B3" s="383" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="G4" t="str">
-        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
-        <v>~UC_T</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="B5" s="384" t="s">
-        <v>461</v>
-      </c>
-      <c r="C5" s="385" t="s">
-        <v>474</v>
-      </c>
-      <c r="D5" s="385" t="s">
-        <v>475</v>
-      </c>
-      <c r="E5" s="385" t="s">
-        <v>225</v>
-      </c>
-      <c r="F5" s="385" t="s">
-        <v>226</v>
-      </c>
-      <c r="G5" s="385" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" s="386" t="s">
-        <v>476</v>
-      </c>
-      <c r="I5" s="386" t="s">
-        <v>477</v>
-      </c>
-      <c r="J5" s="387" t="s">
-        <v>462</v>
-      </c>
-      <c r="K5" s="384" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="B6" s="30" t="s">
-        <v>464</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30" t="s">
-        <v>478</v>
-      </c>
-      <c r="K6" s="388"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="B7" t="str">
-        <f>VLOOKUP(B$5, 'CO2-config'!$B$4:$D$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_Emissions_CO2_2020_Single</v>
-      </c>
-      <c r="C7" t="str">
-        <f>VLOOKUP(C$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(D$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="F7">
-        <v>2018</v>
-      </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(G$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>LO</v>
-      </c>
-      <c r="H7">
-        <f>VLOOKUP(H$5, 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F7,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" t="str">
-        <f>VLOOKUP(K$5, 'CO2-config'!$B$4:$D$14,2,FALSE) &amp; " - Single"</f>
-        <v>CO2 Emissions in 2020 - Single</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="C8" t="str">
-        <f>VLOOKUP(C$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(D$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="E8" t="str">
-        <f>VLOOKUP(E$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-      <c r="F8">
-        <f>F7</f>
-        <v>2018</v>
-      </c>
-      <c r="I8">
-        <f>VLOOKUP(I$5, 'CO2-config'!$B$4:$D$14,MATCH($F8,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F9,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Move historic biogas production constraint and add bounds for 2019-2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6FBEBB-C133-4C33-BF90-8C8AA431B303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817D68D-3EAE-41FC-A469-18345AD6C5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="506">
   <si>
     <t>Development</t>
   </si>
@@ -1716,12 +1716,6 @@
     <t>*Pja</t>
   </si>
   <si>
-    <t>UC_Historic_IMPELC</t>
-  </si>
-  <si>
-    <t>UC_Historic_EXPELC</t>
-  </si>
-  <si>
     <t>Historic electricity import</t>
   </si>
   <si>
@@ -1747,6 +1741,27 @@
   </si>
   <si>
     <t>exp</t>
+  </si>
+  <si>
+    <t>UC_COMPRD</t>
+  </si>
+  <si>
+    <t>BIOGAS*G</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Historic production of biogas</t>
+  </si>
+  <si>
+    <t>UC_Historic_BIOGAS-Production</t>
+  </si>
+  <si>
+    <t>UC_Historic_ELC-Export</t>
+  </si>
+  <si>
+    <t>UC_Historic_ELC-Import</t>
   </si>
 </sst>
 </file>
@@ -5162,6 +5177,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5174,7 +5190,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6292,12 +6307,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="386" t="s">
+      <c r="A16" s="387" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="386"/>
-      <c r="C16" s="386"/>
-      <c r="D16" s="386"/>
+      <c r="B16" s="387"/>
+      <c r="C16" s="387"/>
+      <c r="D16" s="387"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6381,11 +6396,11 @@
       <c r="A19" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="385" t="s">
+      <c r="B19" s="386" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="385"/>
-      <c r="D19" s="385"/>
+      <c r="C19" s="386"/>
+      <c r="D19" s="386"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6413,11 +6428,11 @@
       <c r="A20" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="385" t="s">
+      <c r="B20" s="386" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="385"/>
-      <c r="D20" s="385"/>
+      <c r="C20" s="386"/>
+      <c r="D20" s="386"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6505,11 +6520,11 @@
       <c r="A23" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="385" t="s">
+      <c r="B23" s="386" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="385"/>
-      <c r="D23" s="385"/>
+      <c r="C23" s="386"/>
+      <c r="D23" s="386"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6535,11 +6550,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="385" t="s">
+      <c r="B24" s="386" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="385"/>
-      <c r="D24" s="385"/>
+      <c r="C24" s="386"/>
+      <c r="D24" s="386"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6597,11 +6612,11 @@
       <c r="A26" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="385" t="s">
+      <c r="B26" s="386" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="385"/>
-      <c r="D26" s="385"/>
+      <c r="C26" s="386"/>
+      <c r="D26" s="386"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6717,11 +6732,11 @@
       <c r="A30" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="387" t="s">
+      <c r="B30" s="388" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="385"/>
-      <c r="D30" s="385"/>
+      <c r="C30" s="386"/>
+      <c r="D30" s="386"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6749,11 +6764,11 @@
       <c r="A31" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="385" t="s">
+      <c r="B31" s="386" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="385"/>
-      <c r="D31" s="385"/>
+      <c r="C31" s="386"/>
+      <c r="D31" s="386"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -9634,10 +9649,10 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="388" t="s">
+      <c r="B49" s="389" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="388"/>
+      <c r="C49" s="389"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
@@ -10279,7 +10294,7 @@
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="AP58" sqref="AP58"/>
+      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -17558,12 +17573,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AJ80" sqref="AJ80"/>
       <selection pane="topRight" activeCell="AJ80" sqref="AJ80"/>
       <selection pane="bottomLeft" activeCell="AJ80" sqref="AJ80"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24821,12 +24836,12 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AQ85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="95" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -32143,12 +32158,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4685A7-279E-44B2-B92C-436990F54D25}">
   <dimension ref="A1:AQ85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="95" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="AO3" sqref="AO3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -40265,21 +40280,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89305455-607F-41AA-8109-096F19F6FE72}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -40314,7 +40330,7 @@
         <v>474</v>
       </c>
       <c r="D5" s="381" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E5" s="381" t="s">
         <v>225</v>
@@ -40356,16 +40372,16 @@
     </row>
     <row r="7" spans="1:11">
       <c r="B7" t="s">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="C7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D7" t="s">
+        <v>494</v>
+      </c>
+      <c r="E7" t="s">
         <v>495</v>
-      </c>
-      <c r="D7" t="s">
-        <v>496</v>
-      </c>
-      <c r="E7" t="s">
-        <v>497</v>
       </c>
       <c r="F7">
         <v>2018</v>
@@ -40374,17 +40390,17 @@
         <v>223</v>
       </c>
       <c r="H7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="389">
+      <c r="J7" s="385">
         <f>Conversions!$B$2*'EB2018'!$AO$3</f>
         <v>5.8385184241824009</v>
       </c>
       <c r="K7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -40394,7 +40410,7 @@
       <c r="G8" t="s">
         <v>223</v>
       </c>
-      <c r="J8" s="389">
+      <c r="J8" s="385">
         <f>Conversions!$B$2*'EB2019'!$AO$3</f>
         <v>7.8478965511531191</v>
       </c>
@@ -40406,7 +40422,7 @@
       <c r="G9" t="s">
         <v>223</v>
       </c>
-      <c r="J9" s="389">
+      <c r="J9" s="385">
         <f>Conversions!$B$2*'EB2020'!$AO$3</f>
         <v>6.3411436804464003</v>
       </c>
@@ -40418,7 +40434,7 @@
       <c r="G10" t="s">
         <v>223</v>
       </c>
-      <c r="J10" s="389">
+      <c r="J10" s="385">
         <f>Conversions!$B$2*'EB2021'!$AO$3</f>
         <v>8.8241634675727223</v>
       </c>
@@ -40436,16 +40452,16 @@
     </row>
     <row r="12" spans="1:11">
       <c r="B12" t="s">
-        <v>491</v>
+        <v>504</v>
       </c>
       <c r="C12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E12" t="s">
         <v>496</v>
-      </c>
-      <c r="E12" t="s">
-        <v>498</v>
       </c>
       <c r="F12">
         <v>2018</v>
@@ -40454,17 +40470,17 @@
         <v>223</v>
       </c>
       <c r="H12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="389">
+      <c r="J12" s="385">
         <f>Conversions!$B$2*'EB2018'!$AO$4</f>
         <v>5.9383641411770398</v>
       </c>
       <c r="K12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -40474,7 +40490,7 @@
       <c r="G13" t="s">
         <v>223</v>
       </c>
-      <c r="J13" s="389">
+      <c r="J13" s="385">
         <f>Conversions!$B$2*'EB2019'!$AO$4</f>
         <v>5.5271334489739186</v>
       </c>
@@ -40486,7 +40502,7 @@
       <c r="G14" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="389">
+      <c r="J14" s="385">
         <f>Conversions!$B$2*'EB2020'!$AO$4</f>
         <v>6.8879157977152801</v>
       </c>
@@ -40498,7 +40514,7 @@
       <c r="G15" t="s">
         <v>223</v>
       </c>
-      <c r="J15" s="389">
+      <c r="J15" s="385">
         <f>Conversions!$B$2*'EB2021'!$AO$4</f>
         <v>3.1077995112374399</v>
       </c>
@@ -40511,6 +40527,114 @@
         <v>223</v>
       </c>
       <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="H19" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="380" t="s">
+        <v>461</v>
+      </c>
+      <c r="C20" s="381" t="s">
+        <v>474</v>
+      </c>
+      <c r="D20" s="381" t="s">
+        <v>492</v>
+      </c>
+      <c r="E20" s="381" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="381" t="s">
+        <v>226</v>
+      </c>
+      <c r="G20" s="381" t="s">
+        <v>227</v>
+      </c>
+      <c r="H20" s="381" t="s">
+        <v>486</v>
+      </c>
+      <c r="I20" t="s">
+        <v>499</v>
+      </c>
+      <c r="J20" s="383" t="s">
+        <v>462</v>
+      </c>
+      <c r="K20" s="380" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" t="s">
+        <v>503</v>
+      </c>
+      <c r="C21" t="s">
+        <v>500</v>
+      </c>
+      <c r="F21">
+        <v>2018</v>
+      </c>
+      <c r="G21" t="s">
+        <v>501</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" s="19">
+        <f>Conversions!$B$2*'EB2018'!$AH$2</f>
+        <v>0.70393223471436184</v>
+      </c>
+      <c r="K21" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="F22">
+        <v>2019</v>
+      </c>
+      <c r="G22" t="s">
+        <v>501</v>
+      </c>
+      <c r="J22" s="19">
+        <f>Conversions!$B$2*'EB2019'!$AH$2</f>
+        <v>0.78962633124536741</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="F23">
+        <v>2020</v>
+      </c>
+      <c r="G23" t="s">
+        <v>501</v>
+      </c>
+      <c r="J23" s="19">
+        <f>Conversions!$B$2*'EB2020'!$AH$2</f>
+        <v>0.87833840712769273</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="F24">
+        <v>2021</v>
+      </c>
+      <c r="G24" t="s">
+        <v>501</v>
+      </c>
+      <c r="J24" s="19">
+        <f>Conversions!$B$2*'EB2021'!$AH$2</f>
+        <v>0.94933194191684911</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>501</v>
+      </c>
+      <c r="J25">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Specify historic ELC consumption in AGR, IND and TRA
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817D68D-3EAE-41FC-A469-18345AD6C5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564D4CAE-9409-406C-9709-3778A167363B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -18,18 +18,21 @@
     <sheet name="SUP" sheetId="28" r:id="rId3"/>
     <sheet name="PWR" sheetId="8" r:id="rId4"/>
     <sheet name="PWR-CAPs" sheetId="24" r:id="rId5"/>
-    <sheet name="RSD" sheetId="23" r:id="rId6"/>
-    <sheet name="SRV" sheetId="14" r:id="rId7"/>
-    <sheet name="TRA" sheetId="15" r:id="rId8"/>
-    <sheet name="CO2-config" sheetId="27" r:id="rId9"/>
-    <sheet name="CO2-NET-single" sheetId="25" r:id="rId10"/>
-    <sheet name="CO2-NET-multi" sheetId="26" r:id="rId11"/>
-    <sheet name="New vehicle sales" sheetId="16" r:id="rId12"/>
-    <sheet name="EB2018" sheetId="3" r:id="rId13"/>
-    <sheet name="EB2019" sheetId="11" r:id="rId14"/>
-    <sheet name="EB2020" sheetId="12" r:id="rId15"/>
-    <sheet name="EB2021" sheetId="22" r:id="rId16"/>
-    <sheet name="Conversions" sheetId="9" r:id="rId17"/>
+    <sheet name="AGR" sheetId="29" r:id="rId6"/>
+    <sheet name="IND" sheetId="31" r:id="rId7"/>
+    <sheet name="RSD" sheetId="23" r:id="rId8"/>
+    <sheet name="SRV" sheetId="14" r:id="rId9"/>
+    <sheet name="TRA" sheetId="30" r:id="rId10"/>
+    <sheet name="TRA-CAPs" sheetId="15" r:id="rId11"/>
+    <sheet name="CO2-config" sheetId="27" r:id="rId12"/>
+    <sheet name="CO2-NET-single" sheetId="25" r:id="rId13"/>
+    <sheet name="CO2-NET-multi" sheetId="26" r:id="rId14"/>
+    <sheet name="New vehicle sales" sheetId="16" r:id="rId15"/>
+    <sheet name="EB2018" sheetId="3" r:id="rId16"/>
+    <sheet name="EB2019" sheetId="11" r:id="rId17"/>
+    <sheet name="EB2020" sheetId="12" r:id="rId18"/>
+    <sheet name="EB2021" sheetId="22" r:id="rId19"/>
+    <sheet name="Conversions" sheetId="9" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -56,23 +59,23 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_Regression_Y" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
-    <definedName name="aa" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec2" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec3" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elecc" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -90,12 +93,12 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="13">'EB2019'!$A$1:$AQ$80</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="14">'EB2020'!$A$1:$AQ$76</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="15">'EB2021'!$A$1:$AQ$76</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="13">'EB2019'!$A:$B,'EB2019'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="14">'EB2020'!$A:$B,'EB2020'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="15">'EB2021'!$A:$B,'EB2021'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="16">'EB2019'!$A$1:$AQ$80</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="17">'EB2020'!$A$1:$AQ$76</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="18">'EB2021'!$A$1:$AQ$76</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="16">'EB2019'!$A:$B,'EB2019'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="17">'EB2020'!$A:$B,'EB2020'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="18">'EB2021'!$A:$B,'EB2021'!$1:$1</definedName>
     <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
     <definedName name="RiskAfterSimMacro" hidden="1">""</definedName>
     <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
@@ -118,11 +121,11 @@
     <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
     <definedName name="RiskUseFixedSeed" hidden="1">TRUE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
-    <definedName name="table6" localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="16" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="19" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -210,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="512">
   <si>
     <t>Development</t>
   </si>
@@ -1762,6 +1765,24 @@
   </si>
   <si>
     <t>UC_Historic_ELC-Import</t>
+  </si>
+  <si>
+    <t>FT-AGRELC</t>
+  </si>
+  <si>
+    <t>FT-TRAELC</t>
+  </si>
+  <si>
+    <t>FT-INDELC</t>
+  </si>
+  <si>
+    <t>TRAELC</t>
+  </si>
+  <si>
+    <t>UC_Historic_TRAELC-cons_Multi</t>
+  </si>
+  <si>
+    <t>Historic electricity consumption in TRA - Multi</t>
   </si>
 </sst>
 </file>
@@ -8720,11 +8741,1783 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
+  <dimension ref="B2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="379" t="str">
+        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!E3:AD3)</f>
+        <v>~UC_Sets: R_S: IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="379" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="G4" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="380" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="381" t="s">
+        <v>474</v>
+      </c>
+      <c r="D5" s="381" t="s">
+        <v>475</v>
+      </c>
+      <c r="E5" s="381" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="381" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="381" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="382" t="s">
+        <v>499</v>
+      </c>
+      <c r="I5" s="383" t="s">
+        <v>480</v>
+      </c>
+      <c r="J5" s="380" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>510</v>
+      </c>
+      <c r="C7" t="s">
+        <v>509</v>
+      </c>
+      <c r="F7">
+        <v>2018</v>
+      </c>
+      <c r="G7" t="s">
+        <v>501</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19">
+        <f>F17</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8" t="s">
+        <v>501</v>
+      </c>
+      <c r="I8" s="19">
+        <f>G17</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9" t="s">
+        <v>501</v>
+      </c>
+      <c r="I9" s="19">
+        <f>H17</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="F10">
+        <v>2021</v>
+      </c>
+      <c r="G10" t="s">
+        <v>501</v>
+      </c>
+      <c r="I10" s="19">
+        <f>I17</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F11,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B16" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="29">
+        <v>2018</v>
+      </c>
+      <c r="G16" s="29">
+        <v>2019</v>
+      </c>
+      <c r="H16" s="29">
+        <v>2020</v>
+      </c>
+      <c r="I16" s="29">
+        <v>2021</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" t="s">
+        <v>507</v>
+      </c>
+      <c r="D17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F17" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$45),1)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G17" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$45),1)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H17" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$45),1)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I17" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$45),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC29CEA2-2536-449C-BE94-1AB8A11FBF6A}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:AH16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="32" width="6.85546875" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="21">
+      <c r="A1" s="42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="B5" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" thickBot="1">
+      <c r="B6" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" s="37" t="str">
+        <f>Regions!C$3</f>
+        <v>IE</v>
+      </c>
+      <c r="G6" s="37" t="str">
+        <f>Regions!E$3</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="H6" s="37" t="str">
+        <f>Regions!F$3</f>
+        <v>IE-D</v>
+      </c>
+      <c r="I6" s="37" t="str">
+        <f>Regions!G$3</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="J6" s="37" t="str">
+        <f>Regions!H$3</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="K6" s="37" t="str">
+        <f>Regions!I$3</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="L6" s="37" t="str">
+        <f>Regions!J$3</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="M6" s="37" t="str">
+        <f>Regions!K$3</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="N6" s="37" t="str">
+        <f>Regions!L$3</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="O6" s="37" t="str">
+        <f>Regions!M$3</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="P6" s="37" t="str">
+        <f>Regions!N$3</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="Q6" s="37" t="str">
+        <f>Regions!O$3</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="R6" s="37" t="str">
+        <f>Regions!P$3</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="S6" s="37" t="str">
+        <f>Regions!Q$3</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="T6" s="37" t="str">
+        <f>Regions!R$3</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="U6" s="37" t="str">
+        <f>Regions!S$3</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="V6" s="37" t="str">
+        <f>Regions!T$3</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="W6" s="37" t="str">
+        <f>Regions!U$3</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="X6" s="37" t="str">
+        <f>Regions!V$3</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="Y6" s="37" t="str">
+        <f>Regions!W$3</f>
+        <v>IE-G</v>
+      </c>
+      <c r="Z6" s="37" t="str">
+        <f>Regions!X$3</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="AA6" s="37" t="str">
+        <f>Regions!Y$3</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="AB6" s="37" t="str">
+        <f>Regions!Z$3</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AC6" s="37" t="str">
+        <f>Regions!AA$3</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AD6" s="37" t="str">
+        <f>Regions!AB$3</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AE6" s="37" t="str">
+        <f>Regions!AC$3</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AF6" s="37" t="str">
+        <f>Regions!AD$3</f>
+        <v>IE-MN</v>
+      </c>
+      <c r="AG6" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH6" s="36" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="C7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
+      <c r="F7" s="35">
+        <f>'New vehicle sales'!C6/1000</f>
+        <v>38.232999999999997</v>
+      </c>
+      <c r="G7" s="33">
+        <f>$F$7*'New vehicle sales'!D43</f>
+        <v>0.45710685960227732</v>
+      </c>
+      <c r="H7" s="33">
+        <f>$F$7*'New vehicle sales'!E43</f>
+        <v>10.817941425680914</v>
+      </c>
+      <c r="I7" s="33">
+        <f>$F$7*'New vehicle sales'!F43</f>
+        <v>1.7864839578610465</v>
+      </c>
+      <c r="J7" s="33">
+        <f>$F$7*'New vehicle sales'!G43</f>
+        <v>0.79673343448417733</v>
+      </c>
+      <c r="K7" s="33">
+        <f>$F$7*'New vehicle sales'!H43</f>
+        <v>0.68003196247688613</v>
+      </c>
+      <c r="L7" s="33">
+        <f>$F$7*'New vehicle sales'!I43</f>
+        <v>0.32816919610278722</v>
+      </c>
+      <c r="M7" s="33">
+        <f>$F$7*'New vehicle sales'!J43</f>
+        <v>1.0348092547772767</v>
+      </c>
+      <c r="N7" s="33">
+        <f>$F$7*'New vehicle sales'!K43</f>
+        <v>1.5660076990842859</v>
+      </c>
+      <c r="O7" s="33">
+        <f>$F$7*'New vehicle sales'!L43</f>
+        <v>0.62594863840113013</v>
+      </c>
+      <c r="P7" s="33">
+        <f>$F$7*'New vehicle sales'!M43</f>
+        <v>0.71273406742946244</v>
+      </c>
+      <c r="Q7" s="33">
+        <f>$F$7*'New vehicle sales'!N43</f>
+        <v>1.2021174951410833</v>
+      </c>
+      <c r="R7" s="33">
+        <f>$F$7*'New vehicle sales'!O43</f>
+        <v>1.1435299037246951</v>
+      </c>
+      <c r="S7" s="33">
+        <f>$F$7*'New vehicle sales'!P43</f>
+        <v>0.95398134155420122</v>
+      </c>
+      <c r="T7" s="33">
+        <f>$F$7*'New vehicle sales'!Q43</f>
+        <v>4.3586855662644748</v>
+      </c>
+      <c r="U7" s="33">
+        <f>$F$7*'New vehicle sales'!R43</f>
+        <v>1.185939066101201</v>
+      </c>
+      <c r="V7" s="33">
+        <f>$F$7*'New vehicle sales'!S43</f>
+        <v>1.5648434945131779</v>
+      </c>
+      <c r="W7" s="33">
+        <f>$F$7*'New vehicle sales'!T43</f>
+        <v>1.2810505650622175</v>
+      </c>
+      <c r="X7" s="33">
+        <f>$F$7*'New vehicle sales'!U43</f>
+        <v>0.93277676036594825</v>
+      </c>
+      <c r="Y7" s="33">
+        <f>$F$7*'New vehicle sales'!V43</f>
+        <v>2.0719469186967694</v>
+      </c>
+      <c r="Z7" s="33">
+        <f>$F$7*'New vehicle sales'!W43</f>
+        <v>0.25728118121786298</v>
+      </c>
+      <c r="AA7" s="33">
+        <f>$F$7*'New vehicle sales'!X43</f>
+        <v>1.0478403169766459</v>
+      </c>
+      <c r="AB7" s="33">
+        <f>$F$7*'New vehicle sales'!Y43</f>
+        <v>0.518223585086935</v>
+      </c>
+      <c r="AC7" s="33">
+        <f>$F$7*'New vehicle sales'!Z43</f>
+        <v>0.52618032115568125</v>
+      </c>
+      <c r="AD7" s="33">
+        <f>$F$7*'New vehicle sales'!AA43</f>
+        <v>0.6116168786809365</v>
+      </c>
+      <c r="AE7" s="33">
+        <f>$F$7*'New vehicle sales'!AB43</f>
+        <v>1.2781520971300098</v>
+      </c>
+      <c r="AF7" s="33">
+        <f>$F$7*'New vehicle sales'!AC43</f>
+        <v>0.49286801242790335</v>
+      </c>
+      <c r="AG7" t="str">
+        <f>'New vehicle sales'!B57</f>
+        <v>T-CAR-ICE_DST21</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8">
+        <v>2020</v>
+      </c>
+      <c r="F8" s="35">
+        <f>'New vehicle sales'!C7/1000</f>
+        <v>32.6</v>
+      </c>
+      <c r="G8" s="33">
+        <f>$F$8*'New vehicle sales'!D43</f>
+        <v>0.38975972649371593</v>
+      </c>
+      <c r="H8" s="33">
+        <f>$F$8*'New vehicle sales'!E43</f>
+        <v>9.2240967352077483</v>
+      </c>
+      <c r="I8" s="33">
+        <f>$F$8*'New vehicle sales'!F43</f>
+        <v>1.5232751033471117</v>
+      </c>
+      <c r="J8" s="33">
+        <f>$F$8*'New vehicle sales'!G43</f>
+        <v>0.67934794455533654</v>
+      </c>
+      <c r="K8" s="33">
+        <f>$F$8*'New vehicle sales'!H43</f>
+        <v>0.57984050366820528</v>
+      </c>
+      <c r="L8" s="33">
+        <f>$F$8*'New vehicle sales'!I43</f>
+        <v>0.27981889448776881</v>
+      </c>
+      <c r="M8" s="33">
+        <f>$F$8*'New vehicle sales'!J43</f>
+        <v>0.88234723159938333</v>
+      </c>
+      <c r="N8" s="33">
+        <f>$F$8*'New vehicle sales'!K43</f>
+        <v>1.3352823736078185</v>
+      </c>
+      <c r="O8" s="33">
+        <f>$F$8*'New vehicle sales'!L43</f>
+        <v>0.53372546260761244</v>
+      </c>
+      <c r="P8" s="33">
+        <f>$F$8*'New vehicle sales'!M43</f>
+        <v>0.60772449449952859</v>
+      </c>
+      <c r="Q8" s="33">
+        <f>$F$8*'New vehicle sales'!N43</f>
+        <v>1.0250053707948454</v>
+      </c>
+      <c r="R8" s="33">
+        <f>$F$8*'New vehicle sales'!O43</f>
+        <v>0.97504969166492472</v>
+      </c>
+      <c r="S8" s="33">
+        <f>$F$8*'New vehicle sales'!P43</f>
+        <v>0.81342797412358336</v>
+      </c>
+      <c r="T8" s="33">
+        <f>$F$8*'New vehicle sales'!Q43</f>
+        <v>3.7165053608197605</v>
+      </c>
+      <c r="U8" s="33">
+        <f>$F$8*'New vehicle sales'!R43</f>
+        <v>1.0112105656082222</v>
+      </c>
+      <c r="V8" s="33">
+        <f>$F$8*'New vehicle sales'!S43</f>
+        <v>1.3342896953189549</v>
+      </c>
+      <c r="W8" s="33">
+        <f>$F$8*'New vehicle sales'!T43</f>
+        <v>1.0923089587798052</v>
+      </c>
+      <c r="X8" s="33">
+        <f>$F$8*'New vehicle sales'!U43</f>
+        <v>0.79534753715193462</v>
+      </c>
+      <c r="Y8" s="33">
+        <f>$F$8*'New vehicle sales'!V43</f>
+        <v>1.7666798197764939</v>
+      </c>
+      <c r="Z8" s="33">
+        <f>$F$8*'New vehicle sales'!W43</f>
+        <v>0.21937505578171562</v>
+      </c>
+      <c r="AA8" s="33">
+        <f>$F$8*'New vehicle sales'!X43</f>
+        <v>0.89345838237749231</v>
+      </c>
+      <c r="AB8" s="33">
+        <f>$F$8*'New vehicle sales'!Y43</f>
+        <v>0.44187191363047851</v>
+      </c>
+      <c r="AC8" s="33">
+        <f>$F$8*'New vehicle sales'!Z43</f>
+        <v>0.44865635628057465</v>
+      </c>
+      <c r="AD8" s="33">
+        <f>$F$8*'New vehicle sales'!AA43</f>
+        <v>0.52150525056884189</v>
+      </c>
+      <c r="AE8" s="33">
+        <f>$F$8*'New vehicle sales'!AB43</f>
+        <v>1.0898375321433926</v>
+      </c>
+      <c r="AF8" s="33">
+        <f>$F$8*'New vehicle sales'!AC43</f>
+        <v>0.42025206510474333</v>
+      </c>
+      <c r="AG8" t="str">
+        <f>'New vehicle sales'!B56</f>
+        <v>T-CAR-ICE_GSL21</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
+      <c r="C9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9">
+        <v>2020</v>
+      </c>
+      <c r="F9" s="35">
+        <f>'New vehicle sales'!C8/1000</f>
+        <v>10.474</v>
+      </c>
+      <c r="G9" s="33">
+        <f>$F$9*'New vehicle sales'!D43</f>
+        <v>0.12522525691089512</v>
+      </c>
+      <c r="H9" s="33">
+        <f>$F$9*'New vehicle sales'!E43</f>
+        <v>2.9635947608762563</v>
+      </c>
+      <c r="I9" s="33">
+        <f>$F$9*'New vehicle sales'!F43</f>
+        <v>0.4894105347379647</v>
+      </c>
+      <c r="J9" s="33">
+        <f>$F$9*'New vehicle sales'!G43</f>
+        <v>0.21826657580590783</v>
+      </c>
+      <c r="K9" s="33">
+        <f>$F$9*'New vehicle sales'!H43</f>
+        <v>0.18629599495155771</v>
+      </c>
+      <c r="L9" s="33">
+        <f>$F$9*'New vehicle sales'!I43</f>
+        <v>8.9902549106284979E-2</v>
+      </c>
+      <c r="M9" s="33">
+        <f>$F$9*'New vehicle sales'!J43</f>
+        <v>0.28348788048380186</v>
+      </c>
+      <c r="N9" s="33">
+        <f>$F$9*'New vehicle sales'!K43</f>
+        <v>0.42901066199902738</v>
+      </c>
+      <c r="O9" s="33">
+        <f>$F$9*'New vehicle sales'!L43</f>
+        <v>0.17147976979607768</v>
+      </c>
+      <c r="P9" s="33">
+        <f>$F$9*'New vehicle sales'!M43</f>
+        <v>0.19525479617754793</v>
+      </c>
+      <c r="Q9" s="33">
+        <f>$F$9*'New vehicle sales'!N43</f>
+        <v>0.32932227772101874</v>
+      </c>
+      <c r="R9" s="33">
+        <f>$F$9*'New vehicle sales'!O43</f>
+        <v>0.31327210032203745</v>
+      </c>
+      <c r="S9" s="33">
+        <f>$F$9*'New vehicle sales'!P43</f>
+        <v>0.26134492641013535</v>
+      </c>
+      <c r="T9" s="33">
+        <f>$F$9*'New vehicle sales'!Q43</f>
+        <v>1.1940698512032568</v>
+      </c>
+      <c r="U9" s="33">
+        <f>$F$9*'New vehicle sales'!R43</f>
+        <v>0.32489016761289935</v>
+      </c>
+      <c r="V9" s="33">
+        <f>$F$9*'New vehicle sales'!S43</f>
+        <v>0.4286917260359121</v>
+      </c>
+      <c r="W9" s="33">
+        <f>$F$9*'New vehicle sales'!T43</f>
+        <v>0.35094613602023556</v>
+      </c>
+      <c r="X9" s="33">
+        <f>$F$9*'New vehicle sales'!U43</f>
+        <v>0.2555358927647044</v>
+      </c>
+      <c r="Y9" s="33">
+        <f>$F$9*'New vehicle sales'!V43</f>
+        <v>0.56761363289383426</v>
+      </c>
+      <c r="Z9" s="33">
+        <f>$F$9*'New vehicle sales'!W43</f>
+        <v>7.0482648290113165E-2</v>
+      </c>
+      <c r="AA9" s="33">
+        <f>$F$9*'New vehicle sales'!X43</f>
+        <v>0.28705776371232683</v>
+      </c>
+      <c r="AB9" s="33">
+        <f>$F$9*'New vehicle sales'!Y43</f>
+        <v>0.14196829519526477</v>
+      </c>
+      <c r="AC9" s="33">
+        <f>$F$9*'New vehicle sales'!Z43</f>
+        <v>0.14414805753628032</v>
+      </c>
+      <c r="AD9" s="33">
+        <f>$F$9*'New vehicle sales'!AA43</f>
+        <v>0.16755355811221012</v>
+      </c>
+      <c r="AE9" s="33">
+        <f>$F$9*'New vehicle sales'!AB43</f>
+        <v>0.3501520954499967</v>
+      </c>
+      <c r="AF9" s="33">
+        <f>$F$9*'New vehicle sales'!AC43</f>
+        <v>0.13502208987445036</v>
+      </c>
+      <c r="AG9" t="str">
+        <f>'New vehicle sales'!B62</f>
+        <v>T-CAR-HEV_GSL21</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
+      <c r="C10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10">
+        <v>2020</v>
+      </c>
+      <c r="F10" s="35">
+        <f>'New vehicle sales'!C9/1000</f>
+        <v>4.0129999999999999</v>
+      </c>
+      <c r="G10" s="33">
+        <f>$F$10*'New vehicle sales'!D43</f>
+        <v>4.7978704982186565E-2</v>
+      </c>
+      <c r="H10" s="33">
+        <f>$F$10*'New vehicle sales'!E43</f>
+        <v>1.135469331238917</v>
+      </c>
+      <c r="I10" s="33">
+        <f>$F$10*'New vehicle sales'!F43</f>
+        <v>0.18751236164821961</v>
+      </c>
+      <c r="J10" s="33">
+        <f>$F$10*'New vehicle sales'!G43</f>
+        <v>8.3626481641121644E-2</v>
+      </c>
+      <c r="K10" s="33">
+        <f>$F$10*'New vehicle sales'!H43</f>
+        <v>7.1377298810445008E-2</v>
+      </c>
+      <c r="L10" s="33">
+        <f>$F$10*'New vehicle sales'!I43</f>
+        <v>3.4445190907344055E-2</v>
+      </c>
+      <c r="M10" s="33">
+        <f>$F$10*'New vehicle sales'!J43</f>
+        <v>0.10861532025792409</v>
+      </c>
+      <c r="N10" s="33">
+        <f>$F$10*'New vehicle sales'!K43</f>
+        <v>0.16437080261620171</v>
+      </c>
+      <c r="O10" s="33">
+        <f>$F$10*'New vehicle sales'!L43</f>
+        <v>6.570062213019473E-2</v>
+      </c>
+      <c r="P10" s="33">
+        <f>$F$10*'New vehicle sales'!M43</f>
+        <v>7.4809766761552404E-2</v>
+      </c>
+      <c r="Q10" s="33">
+        <f>$F$10*'New vehicle sales'!N43</f>
+        <v>0.12617627463189307</v>
+      </c>
+      <c r="R10" s="33">
+        <f>$F$10*'New vehicle sales'!O43</f>
+        <v>0.12002682247396756</v>
+      </c>
+      <c r="S10" s="33">
+        <f>$F$10*'New vehicle sales'!P43</f>
+        <v>0.10013148650791226</v>
+      </c>
+      <c r="T10" s="33">
+        <f>$F$10*'New vehicle sales'!Q43</f>
+        <v>0.45749496972299686</v>
+      </c>
+      <c r="U10" s="33">
+        <f>$F$10*'New vehicle sales'!R43</f>
+        <v>0.12447815950263176</v>
+      </c>
+      <c r="V10" s="33">
+        <f>$F$10*'New vehicle sales'!S43</f>
+        <v>0.16424860574585784</v>
+      </c>
+      <c r="W10" s="33">
+        <f>$F$10*'New vehicle sales'!T43</f>
+        <v>0.13446122244120728</v>
+      </c>
+      <c r="X10" s="33">
+        <f>$F$10*'New vehicle sales'!U43</f>
+        <v>9.7905817993580169E-2</v>
+      </c>
+      <c r="Y10" s="33">
+        <f>$F$10*'New vehicle sales'!V43</f>
+        <v>0.21747503425653589</v>
+      </c>
+      <c r="Z10" s="33">
+        <f>$F$10*'New vehicle sales'!W43</f>
+        <v>2.7004665608957815E-2</v>
+      </c>
+      <c r="AA10" s="33">
+        <f>$F$10*'New vehicle sales'!X43</f>
+        <v>0.10998308246873854</v>
+      </c>
+      <c r="AB10" s="33">
+        <f>$F$10*'New vehicle sales'!Y43</f>
+        <v>5.4393619306721167E-2</v>
+      </c>
+      <c r="AC10" s="33">
+        <f>$F$10*'New vehicle sales'!Z43</f>
+        <v>5.5228771710243735E-2</v>
+      </c>
+      <c r="AD10" s="33">
+        <f>$F$10*'New vehicle sales'!AA43</f>
+        <v>6.4196336519409883E-2</v>
+      </c>
+      <c r="AE10" s="33">
+        <f>$F$10*'New vehicle sales'!AB43</f>
+        <v>0.13415699437090289</v>
+      </c>
+      <c r="AF10" s="33">
+        <f>$F$10*'New vehicle sales'!AC43</f>
+        <v>5.1732255744335424E-2</v>
+      </c>
+      <c r="AG10" t="str">
+        <f>'New vehicle sales'!B70</f>
+        <v>T-CAR-BEV100_ELC21</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
+      <c r="C11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11">
+        <v>2020</v>
+      </c>
+      <c r="F11" s="35">
+        <f>'New vehicle sales'!C10/1000</f>
+        <v>2.4590000000000001</v>
+      </c>
+      <c r="G11" s="33">
+        <f>$F$11*'New vehicle sales'!D43</f>
+        <v>2.9399360964664036E-2</v>
+      </c>
+      <c r="H11" s="33">
+        <f>$F$11*'New vehicle sales'!E43</f>
+        <v>0.69576852367717346</v>
+      </c>
+      <c r="I11" s="33">
+        <f>$F$11*'New vehicle sales'!F43</f>
+        <v>0.11489979997332969</v>
+      </c>
+      <c r="J11" s="33">
+        <f>$F$11*'New vehicle sales'!G43</f>
+        <v>5.1242840357716951E-2</v>
+      </c>
+      <c r="K11" s="33">
+        <f>$F$11*'New vehicle sales'!H43</f>
+        <v>4.3737049034359404E-2</v>
+      </c>
+      <c r="L11" s="33">
+        <f>$F$11*'New vehicle sales'!I43</f>
+        <v>2.1106584709982317E-2</v>
+      </c>
+      <c r="M11" s="33">
+        <f>$F$11*'New vehicle sales'!J43</f>
+        <v>6.6554964493953483E-2</v>
+      </c>
+      <c r="N11" s="33">
+        <f>$F$11*'New vehicle sales'!K43</f>
+        <v>0.10071961216876153</v>
+      </c>
+      <c r="O11" s="33">
+        <f>$F$11*'New vehicle sales'!L43</f>
+        <v>4.0258616949451501E-2</v>
+      </c>
+      <c r="P11" s="33">
+        <f>$F$11*'New vehicle sales'!M43</f>
+        <v>4.5840323066697573E-2</v>
+      </c>
+      <c r="Q11" s="33">
+        <f>$F$11*'New vehicle sales'!N43</f>
+        <v>7.7315589165169479E-2</v>
+      </c>
+      <c r="R11" s="33">
+        <f>$F$11*'New vehicle sales'!O43</f>
+        <v>7.3547459871289869E-2</v>
+      </c>
+      <c r="S11" s="33">
+        <f>$F$11*'New vehicle sales'!P43</f>
+        <v>6.135642295613164E-2</v>
+      </c>
+      <c r="T11" s="33">
+        <f>$F$11*'New vehicle sales'!Q43</f>
+        <v>0.28033394730845984</v>
+      </c>
+      <c r="U11" s="33">
+        <f>$F$11*'New vehicle sales'!R43</f>
+        <v>7.6275054626706085E-2</v>
+      </c>
+      <c r="V11" s="33">
+        <f>$F$11*'New vehicle sales'!S43</f>
+        <v>0.10064473499353713</v>
+      </c>
+      <c r="W11" s="33">
+        <f>$F$11*'New vehicle sales'!T43</f>
+        <v>8.2392261645384685E-2</v>
+      </c>
+      <c r="X11" s="33">
+        <f>$F$11*'New vehicle sales'!U43</f>
+        <v>5.9992625578423532E-2</v>
+      </c>
+      <c r="Y11" s="33">
+        <f>$F$11*'New vehicle sales'!V43</f>
+        <v>0.13325968333835578</v>
+      </c>
+      <c r="Z11" s="33">
+        <f>$F$11*'New vehicle sales'!W43</f>
+        <v>1.6547339330283396E-2</v>
+      </c>
+      <c r="AA11" s="33">
+        <f>$F$11*'New vehicle sales'!X43</f>
+        <v>6.7393072462155021E-2</v>
+      </c>
+      <c r="AB11" s="33">
+        <f>$F$11*'New vehicle sales'!Y43</f>
+        <v>3.3330154466789774E-2</v>
+      </c>
+      <c r="AC11" s="33">
+        <f>$F$11*'New vehicle sales'!Z43</f>
+        <v>3.3841901229875244E-2</v>
+      </c>
+      <c r="AD11" s="33">
+        <f>$F$11*'New vehicle sales'!AA43</f>
+        <v>3.9336853102723376E-2</v>
+      </c>
+      <c r="AE11" s="33">
+        <f>$F$11*'New vehicle sales'!AB43</f>
+        <v>8.2205843298791478E-2</v>
+      </c>
+      <c r="AF11" s="33">
+        <f>$F$11*'New vehicle sales'!AC43</f>
+        <v>3.1699381229833248E-2</v>
+      </c>
+      <c r="AG11" t="str">
+        <f>'New vehicle sales'!B66</f>
+        <v>T-CAR-PHEV40_GSL21</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
+      <c r="C12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12">
+        <v>2020</v>
+      </c>
+      <c r="F12" s="35">
+        <f>'New vehicle sales'!C11/1000</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G12" s="33">
+        <f>$F$12*'New vehicle sales'!D43</f>
+        <v>6.1213797535209372E-3</v>
+      </c>
+      <c r="H12" s="33">
+        <f>$F$12*'New vehicle sales'!E43</f>
+        <v>0.14486924933823211</v>
+      </c>
+      <c r="I12" s="33">
+        <f>$F$12*'New vehicle sales'!F43</f>
+        <v>2.3923829843979179E-2</v>
+      </c>
+      <c r="J12" s="33">
+        <f>$F$12*'New vehicle sales'!G43</f>
+        <v>1.0669513730439641E-2</v>
+      </c>
+      <c r="K12" s="33">
+        <f>$F$12*'New vehicle sales'!H43</f>
+        <v>9.106697480923959E-3</v>
+      </c>
+      <c r="L12" s="33">
+        <f>$F$12*'New vehicle sales'!I43</f>
+        <v>4.3947016557588231E-3</v>
+      </c>
+      <c r="M12" s="33">
+        <f>$F$12*'New vehicle sales'!J43</f>
+        <v>1.3857723391990314E-2</v>
+      </c>
+      <c r="N12" s="33">
+        <f>$F$12*'New vehicle sales'!K43</f>
+        <v>2.0971305990405004E-2</v>
+      </c>
+      <c r="O12" s="33">
+        <f>$F$12*'New vehicle sales'!L43</f>
+        <v>8.3824367133465503E-3</v>
+      </c>
+      <c r="P12" s="33">
+        <f>$F$12*'New vehicle sales'!M43</f>
+        <v>9.544630097661308E-3</v>
+      </c>
+      <c r="Q12" s="33">
+        <f>$F$12*'New vehicle sales'!N43</f>
+        <v>1.6098243860336221E-2</v>
+      </c>
+      <c r="R12" s="33">
+        <f>$F$12*'New vehicle sales'!O43</f>
+        <v>1.5313663869093296E-2</v>
+      </c>
+      <c r="S12" s="33">
+        <f>$F$12*'New vehicle sales'!P43</f>
+        <v>1.2775310513842781E-2</v>
+      </c>
+      <c r="T12" s="33">
+        <f>$F$12*'New vehicle sales'!Q43</f>
+        <v>5.8369654746617095E-2</v>
+      </c>
+      <c r="U12" s="33">
+        <f>$F$12*'New vehicle sales'!R43</f>
+        <v>1.5881589251270239E-2</v>
+      </c>
+      <c r="V12" s="33">
+        <f>$F$12*'New vehicle sales'!S43</f>
+        <v>2.0955715460224077E-2</v>
+      </c>
+      <c r="W12" s="33">
+        <f>$F$12*'New vehicle sales'!T43</f>
+        <v>1.7155281806603074E-2</v>
+      </c>
+      <c r="X12" s="33">
+        <f>$F$12*'New vehicle sales'!U43</f>
+        <v>1.2491347822754311E-2</v>
+      </c>
+      <c r="Y12" s="33">
+        <f>$F$12*'New vehicle sales'!V43</f>
+        <v>2.7746627844342481E-2</v>
+      </c>
+      <c r="Z12" s="33">
+        <f>$F$12*'New vehicle sales'!W43</f>
+        <v>3.4453996490870675E-3</v>
+      </c>
+      <c r="AA12" s="33">
+        <f>$F$12*'New vehicle sales'!X43</f>
+        <v>1.4032229809118897E-2</v>
+      </c>
+      <c r="AB12" s="33">
+        <f>$F$12*'New vehicle sales'!Y43</f>
+        <v>6.939828827570705E-3</v>
+      </c>
+      <c r="AC12" s="33">
+        <f>$F$12*'New vehicle sales'!Z43</f>
+        <v>7.0463820372900065E-3</v>
+      </c>
+      <c r="AD12" s="33">
+        <f>$F$12*'New vehicle sales'!AA43</f>
+        <v>8.1905119107744482E-3</v>
+      </c>
+      <c r="AE12" s="33">
+        <f>$F$12*'New vehicle sales'!AB43</f>
+        <v>1.7116466762497454E-2</v>
+      </c>
+      <c r="AF12" s="33">
+        <f>$F$12*'New vehicle sales'!AC43</f>
+        <v>6.6002778323198952E-3</v>
+      </c>
+      <c r="AG12" t="str">
+        <f>'New vehicle sales'!B63</f>
+        <v>T-CAR-HEV_DST21</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34">
+      <c r="C13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13">
+        <v>2020</v>
+      </c>
+      <c r="F13" s="35">
+        <f>'New vehicle sales'!C12/1000</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G13" s="33">
+        <f>$F$13*'New vehicle sales'!D43</f>
+        <v>3.9454205442615418E-4</v>
+      </c>
+      <c r="H13" s="33">
+        <f>$F$13*'New vehicle sales'!E43</f>
+        <v>9.3372758362532428E-3</v>
+      </c>
+      <c r="I13" s="33">
+        <f>$F$13*'New vehicle sales'!F43</f>
+        <v>1.5419655954127206E-3</v>
+      </c>
+      <c r="J13" s="33">
+        <f>$F$13*'New vehicle sales'!G43</f>
+        <v>6.8768350215724257E-4</v>
+      </c>
+      <c r="K13" s="33">
+        <f>$F$13*'New vehicle sales'!H43</f>
+        <v>5.8695511107517706E-4</v>
+      </c>
+      <c r="L13" s="33">
+        <f>$F$13*'New vehicle sales'!I43</f>
+        <v>2.8325225515633037E-4</v>
+      </c>
+      <c r="M13" s="33">
+        <f>$F$13*'New vehicle sales'!J43</f>
+        <v>8.9317357799937572E-4</v>
+      </c>
+      <c r="N13" s="33">
+        <f>$F$13*'New vehicle sales'!K43</f>
+        <v>1.3516662064128224E-3</v>
+      </c>
+      <c r="O13" s="33">
+        <f>$F$13*'New vehicle sales'!L43</f>
+        <v>5.4027424128991436E-4</v>
+      </c>
+      <c r="P13" s="33">
+        <f>$F$13*'New vehicle sales'!M43</f>
+        <v>6.1518123676332652E-4</v>
+      </c>
+      <c r="Q13" s="33">
+        <f>$F$13*'New vehicle sales'!N43</f>
+        <v>1.0375821238107332E-3</v>
+      </c>
+      <c r="R13" s="33">
+        <f>$F$13*'New vehicle sales'!O43</f>
+        <v>9.8701349156265377E-4</v>
+      </c>
+      <c r="S13" s="33">
+        <f>$F$13*'New vehicle sales'!P43</f>
+        <v>8.2340868546252298E-4</v>
+      </c>
+      <c r="T13" s="33">
+        <f>$F$13*'New vehicle sales'!Q43</f>
+        <v>3.7621066535905552E-3</v>
+      </c>
+      <c r="U13" s="33">
+        <f>$F$13*'New vehicle sales'!R43</f>
+        <v>1.0236180572107771E-3</v>
+      </c>
+      <c r="V13" s="33">
+        <f>$F$13*'New vehicle sales'!S43</f>
+        <v>1.3506613480222551E-3</v>
+      </c>
+      <c r="W13" s="33">
+        <f>$F$13*'New vehicle sales'!T43</f>
+        <v>1.1057115226912138E-3</v>
+      </c>
+      <c r="X13" s="33">
+        <f>$F$13*'New vehicle sales'!U43</f>
+        <v>8.051064026384614E-4</v>
+      </c>
+      <c r="Y13" s="33">
+        <f>$F$13*'New vehicle sales'!V43</f>
+        <v>1.7883568727798866E-3</v>
+      </c>
+      <c r="Z13" s="33">
+        <f>$F$13*'New vehicle sales'!W43</f>
+        <v>2.2206677425756489E-4</v>
+      </c>
+      <c r="AA13" s="33">
+        <f>$F$13*'New vehicle sales'!X43</f>
+        <v>9.0442106191586651E-4</v>
+      </c>
+      <c r="AB13" s="33">
+        <f>$F$13*'New vehicle sales'!Y43</f>
+        <v>4.4729365490201812E-4</v>
+      </c>
+      <c r="AC13" s="33">
+        <f>$F$13*'New vehicle sales'!Z43</f>
+        <v>4.5416134224720743E-4</v>
+      </c>
+      <c r="AD13" s="33">
+        <f>$F$13*'New vehicle sales'!AA43</f>
+        <v>5.2790408799913439E-4</v>
+      </c>
+      <c r="AE13" s="33">
+        <f>$F$13*'New vehicle sales'!AB43</f>
+        <v>1.1032097718015937E-3</v>
+      </c>
+      <c r="AF13" s="33">
+        <f>$F$13*'New vehicle sales'!AC43</f>
+        <v>4.2540853216124324E-4</v>
+      </c>
+      <c r="AG13" t="str">
+        <f>'New vehicle sales'!B69</f>
+        <v>T-CAR-PHEV40_DST21</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34">
+      <c r="C14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14">
+        <v>2020</v>
+      </c>
+      <c r="F14" s="34">
+        <f>'New vehicle sales'!C19/1000</f>
+        <v>20.928000000000001</v>
+      </c>
+      <c r="G14" s="33">
+        <f>($F$14*'New vehicle sales'!D43)</f>
+        <v>0.25021139742516835</v>
+      </c>
+      <c r="H14" s="33">
+        <f>($F$14*'New vehicle sales'!E43)</f>
+        <v>5.9215305667002385</v>
+      </c>
+      <c r="I14" s="33">
+        <f>($F$14*'New vehicle sales'!F43)</f>
+        <v>0.97788654487264892</v>
+      </c>
+      <c r="J14" s="33">
+        <f>($F$14*'New vehicle sales'!G43)</f>
+        <v>0.43611637373172035</v>
+      </c>
+      <c r="K14" s="33">
+        <f>($F$14*'New vehicle sales'!H43)</f>
+        <v>0.37223625953276684</v>
+      </c>
+      <c r="L14" s="33">
+        <f>($F$14*'New vehicle sales'!I43)</f>
+        <v>0.17963343017914188</v>
+      </c>
+      <c r="M14" s="33">
+        <f>($F$14*'New vehicle sales'!J43)</f>
+        <v>0.56643444364760409</v>
+      </c>
+      <c r="N14" s="33">
+        <f>($F$14*'New vehicle sales'!K43)</f>
+        <v>0.85720213235780451</v>
+      </c>
+      <c r="O14" s="33">
+        <f>($F$14*'New vehicle sales'!L43)</f>
+        <v>0.34263210065804023</v>
+      </c>
+      <c r="P14" s="33">
+        <f>($F$14*'New vehicle sales'!M43)</f>
+        <v>0.390136755241906</v>
+      </c>
+      <c r="Q14" s="33">
+        <f>($F$14*'New vehicle sales'!N43)</f>
+        <v>0.65801571779124313</v>
+      </c>
+      <c r="R14" s="33">
+        <f>($F$14*'New vehicle sales'!O43)</f>
+        <v>0.62594601064918842</v>
+      </c>
+      <c r="S14" s="33">
+        <f>($F$14*'New vehicle sales'!P43)</f>
+        <v>0.52219081725332372</v>
+      </c>
+      <c r="T14" s="33">
+        <f>($F$14*'New vehicle sales'!Q43)</f>
+        <v>2.3858596377679739</v>
+      </c>
+      <c r="U14" s="33">
+        <f>($F$14*'New vehicle sales'!R43)</f>
+        <v>0.64915996064567105</v>
+      </c>
+      <c r="V14" s="33">
+        <f>($F$14*'New vehicle sales'!S43)</f>
+        <v>0.85656486943665922</v>
+      </c>
+      <c r="W14" s="33">
+        <f>($F$14*'New vehicle sales'!T43)</f>
+        <v>0.70122214384490067</v>
+      </c>
+      <c r="X14" s="33">
+        <f>($F$14*'New vehicle sales'!U43)</f>
+        <v>0.51058384225508247</v>
+      </c>
+      <c r="Y14" s="33">
+        <f>($F$14*'New vehicle sales'!V43)</f>
+        <v>1.134143413137499</v>
+      </c>
+      <c r="Z14" s="33">
+        <f>($F$14*'New vehicle sales'!W43)</f>
+        <v>0.14083071065643388</v>
+      </c>
+      <c r="AA14" s="33">
+        <f>($F$14*'New vehicle sales'!X43)</f>
+        <v>0.573567393447735</v>
+      </c>
+      <c r="AB14" s="33">
+        <f>($F$14*'New vehicle sales'!Y43)</f>
+        <v>0.28366550332695256</v>
+      </c>
+      <c r="AC14" s="33">
+        <f>($F$14*'New vehicle sales'!Z43)</f>
+        <v>0.28802086577422903</v>
+      </c>
+      <c r="AD14" s="33">
+        <f>($F$14*'New vehicle sales'!AA43)</f>
+        <v>0.33478717435290561</v>
+      </c>
+      <c r="AE14" s="33">
+        <f>($F$14*'New vehicle sales'!AB43)</f>
+        <v>0.69963557891708339</v>
+      </c>
+      <c r="AF14" s="33">
+        <f>($F$14*'New vehicle sales'!AC43)</f>
+        <v>0.26978635639607573</v>
+      </c>
+      <c r="AG14" t="str">
+        <f>'New vehicle sales'!B107</f>
+        <v>T-LGT-ICE_DST61</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
+      <c r="C15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15">
+        <v>2020</v>
+      </c>
+      <c r="F15" s="34">
+        <f>'New vehicle sales'!C20/1000</f>
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="G15" s="33">
+        <f>($F$15*'New vehicle sales'!D43)</f>
+        <v>8.6918810172064865E-3</v>
+      </c>
+      <c r="H15" s="33">
+        <f>($F$15*'New vehicle sales'!E43)</f>
+        <v>0.20570301615018505</v>
+      </c>
+      <c r="I15" s="33">
+        <f>($F$15*'New vehicle sales'!F43)</f>
+        <v>3.3969969329243871E-2</v>
+      </c>
+      <c r="J15" s="33">
+        <f>($F$15*'New vehicle sales'!G43)</f>
+        <v>1.51498759414641E-2</v>
+      </c>
+      <c r="K15" s="33">
+        <f>($F$15*'New vehicle sales'!H43)</f>
+        <v>1.2930798962171324E-2</v>
+      </c>
+      <c r="L15" s="33">
+        <f>($F$15*'New vehicle sales'!I43)</f>
+        <v>6.2401330151106724E-3</v>
+      </c>
+      <c r="M15" s="33">
+        <f>($F$15*'New vehicle sales'!J43)</f>
+        <v>1.9676884581986246E-2</v>
+      </c>
+      <c r="N15" s="33">
+        <f>($F$15*'New vehicle sales'!K43)</f>
+        <v>2.9777616123094604E-2</v>
+      </c>
+      <c r="O15" s="33">
+        <f>($F$15*'New vehicle sales'!L43)</f>
+        <v>1.190240525508387E-2</v>
+      </c>
+      <c r="P15" s="33">
+        <f>($F$15*'New vehicle sales'!M43)</f>
+        <v>1.3552629064452678E-2</v>
+      </c>
+      <c r="Q15" s="33">
+        <f>($F$15*'New vehicle sales'!N43)</f>
+        <v>2.2858248606375847E-2</v>
+      </c>
+      <c r="R15" s="33">
+        <f>($F$15*'New vehicle sales'!O43)</f>
+        <v>2.1744206314122706E-2</v>
+      </c>
+      <c r="S15" s="33">
+        <f>($F$15*'New vehicle sales'!P43)</f>
+        <v>1.8139942858522856E-2</v>
+      </c>
+      <c r="T15" s="33">
+        <f>($F$15*'New vehicle sales'!Q43)</f>
+        <v>8.2880349610919196E-2</v>
+      </c>
+      <c r="U15" s="33">
+        <f>($F$15*'New vehicle sales'!R43)</f>
+        <v>2.2550615987643484E-2</v>
+      </c>
+      <c r="V15" s="33">
+        <f>($F$15*'New vehicle sales'!S43)</f>
+        <v>2.9755478788247858E-2</v>
+      </c>
+      <c r="W15" s="33">
+        <f>($F$15*'New vehicle sales'!T43)</f>
+        <v>2.4359159908985226E-2</v>
+      </c>
+      <c r="X15" s="33">
+        <f>($F$15*'New vehicle sales'!U43)</f>
+        <v>1.7736738021762469E-2</v>
+      </c>
+      <c r="Y15" s="33">
+        <f>($F$15*'New vehicle sales'!V43)</f>
+        <v>3.9398043833665984E-2</v>
+      </c>
+      <c r="Z15" s="33">
+        <f>($F$15*'New vehicle sales'!W43)</f>
+        <v>4.8921983298560508E-3</v>
+      </c>
+      <c r="AA15" s="33">
+        <f>($F$15*'New vehicle sales'!X43)</f>
+        <v>1.9924670060994996E-2</v>
+      </c>
+      <c r="AB15" s="33">
+        <f>($F$15*'New vehicle sales'!Y43)</f>
+        <v>9.8540147610232456E-3</v>
+      </c>
+      <c r="AC15" s="33">
+        <f>($F$15*'New vehicle sales'!Z43)</f>
+        <v>1.0005311994355144E-2</v>
+      </c>
+      <c r="AD15" s="33">
+        <f>($F$15*'New vehicle sales'!AA43)</f>
+        <v>1.1629887029556687E-2</v>
+      </c>
+      <c r="AE15" s="33">
+        <f>($F$15*'New vehicle sales'!AB43)</f>
+        <v>2.4304045578780561E-2</v>
+      </c>
+      <c r="AF15" s="33">
+        <f>($F$15*'New vehicle sales'!AC43)</f>
+        <v>9.3718788751886006E-3</v>
+      </c>
+      <c r="AG15" t="str">
+        <f>'New vehicle sales'!B113</f>
+        <v>T-LGT-BEV_ELC61</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="30">
+        <v>2020</v>
+      </c>
+      <c r="F16" s="32">
+        <f>'New vehicle sales'!C33/1000</f>
+        <v>2.0430000000000001</v>
+      </c>
+      <c r="G16" s="31">
+        <f>($F$16*'New vehicle sales'!D43)</f>
+        <v>2.4425739914928274E-2</v>
+      </c>
+      <c r="H16" s="31">
+        <f>($F$16*'New vehicle sales'!E43)</f>
+        <v>0.57806225858985982</v>
+      </c>
+      <c r="I16" s="31">
+        <f>($F$16*'New vehicle sales'!F43)</f>
+        <v>9.5461688225096611E-2</v>
+      </c>
+      <c r="J16" s="31">
+        <f>($F$16*'New vehicle sales'!G43)</f>
+        <v>4.2573860451734745E-2</v>
+      </c>
+      <c r="K16" s="31">
+        <f>($F$16*'New vehicle sales'!H43)</f>
+        <v>3.633785733110869E-2</v>
+      </c>
+      <c r="L16" s="31">
+        <f>($F$16*'New vehicle sales'!I43)</f>
+        <v>1.7535889614678273E-2</v>
+      </c>
+      <c r="M16" s="31">
+        <f>($F$16*'New vehicle sales'!J43)</f>
+        <v>5.5295564237961357E-2</v>
+      </c>
+      <c r="N16" s="31">
+        <f>($F$16*'New vehicle sales'!K43)</f>
+        <v>8.3680426051557469E-2</v>
+      </c>
+      <c r="O16" s="31">
+        <f>($F$16*'New vehicle sales'!L43)</f>
+        <v>3.3447887119857425E-2</v>
+      </c>
+      <c r="P16" s="31">
+        <f>($F$16*'New vehicle sales'!M43)</f>
+        <v>3.808531111234776E-2</v>
+      </c>
+      <c r="Q16" s="31">
+        <f>($F$16*'New vehicle sales'!N43)</f>
+        <v>6.4235766028646293E-2</v>
+      </c>
+      <c r="R16" s="31">
+        <f>($F$16*'New vehicle sales'!O43)</f>
+        <v>6.110510797765157E-2</v>
+      </c>
+      <c r="S16" s="31">
+        <f>($F$16*'New vehicle sales'!P43)</f>
+        <v>5.097648316363438E-2</v>
+      </c>
+      <c r="T16" s="31">
+        <f>($F$16*'New vehicle sales'!Q43)</f>
+        <v>0.23290860282683346</v>
+      </c>
+      <c r="U16" s="31">
+        <f>($F$16*'New vehicle sales'!R43)</f>
+        <v>6.3371263360049016E-2</v>
+      </c>
+      <c r="V16" s="31">
+        <f>($F$16*'New vehicle sales'!S43)</f>
+        <v>8.3618216182105062E-2</v>
+      </c>
+      <c r="W16" s="31">
+        <f>($F$16*'New vehicle sales'!T43)</f>
+        <v>6.8453595177519699E-2</v>
+      </c>
+      <c r="X16" s="31">
+        <f>($F$16*'New vehicle sales'!U43)</f>
+        <v>4.984340547243566E-2</v>
+      </c>
+      <c r="Y16" s="31">
+        <f>($F$16*'New vehicle sales'!V43)</f>
+        <v>0.11071554821482753</v>
+      </c>
+      <c r="Z16" s="31">
+        <f>($F$16*'New vehicle sales'!W43)</f>
+        <v>1.3747952115400154E-2</v>
+      </c>
+      <c r="AA16" s="31">
+        <f>($F$16*'New vehicle sales'!X43)</f>
+        <v>5.5991885742245916E-2</v>
+      </c>
+      <c r="AB16" s="31">
+        <f>($F$16*'New vehicle sales'!Y43)</f>
+        <v>2.7691543544388575E-2</v>
+      </c>
+      <c r="AC16" s="31">
+        <f>($F$16*'New vehicle sales'!Z43)</f>
+        <v>2.8116715824577115E-2</v>
+      </c>
+      <c r="AD16" s="31">
+        <f>($F$16*'New vehicle sales'!AA43)</f>
+        <v>3.2682062175219143E-2</v>
+      </c>
+      <c r="AE16" s="31">
+        <f>($F$16*'New vehicle sales'!AB43)</f>
+        <v>6.8298714054262299E-2</v>
+      </c>
+      <c r="AF16" s="31">
+        <f>($F$16*'New vehicle sales'!AC43)</f>
+        <v>2.6336655491073332E-2</v>
+      </c>
+      <c r="AG16" s="30" t="str">
+        <f>'New vehicle sales'!B123</f>
+        <v>T-HGT-ICE_DST81</v>
+      </c>
+      <c r="AH16" s="30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40162BAB-2A61-4FF8-AC40-4BD254BCBC14}">
+  <dimension ref="B4:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","Emissions","CO2","2020")</f>
+        <v>UC_Emissions_CO2_2020</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C5" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"CO2 Emissions in 2020")</f>
+        <v>CO2 Emissions in 2020</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6">
+        <v>2018</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>475</v>
+      </c>
+      <c r="C10" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>477</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>476</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A43B5DB-8BF6-4C1B-AB8E-D3EEC4E992CB}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8880,12 +10673,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A089DB7-F6A5-44DD-9B0D-8CBAFF1788E4}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B2" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9042,7 +10835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12490C26-C7DC-403B-9901-8AE03883042B}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AC129"/>
@@ -10282,7 +12075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6617C6-BD81-4C8E-89D7-FC0076ADEEA7}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
@@ -10290,11 +12083,11 @@
   <dimension ref="A1:AS80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="AO30" sqref="AO30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -17568,7 +19361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEC878B-F7E3-4802-BC50-10F92160064D}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AR80"/>
@@ -17578,7 +19371,7 @@
       <selection activeCell="AJ80" sqref="AJ80"/>
       <selection pane="topRight" activeCell="AJ80" sqref="AJ80"/>
       <selection pane="bottomLeft" activeCell="AJ80" sqref="AJ80"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24831,17 +26624,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9945E26-E686-40E8-A01F-A87690AEE355}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AQ85"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="AN20" sqref="AN20"/>
+      <selection pane="bottomRight" activeCell="AK33" sqref="AK33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -32154,16 +33947,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4685A7-279E-44B2-B92C-436990F54D25}">
   <dimension ref="A1:AQ85"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AP45" sqref="AP45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -39473,43 +41266,6 @@
     <oddFooter>&amp;L&amp;G&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A846FF-BBF5-4A02-BAF4-3C4772884C84}">
-  <sheetPr codeName="Sheet9">
-    <tabColor theme="0" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="21">
-        <v>4.1868000000000002E-2</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -40278,11 +42034,48 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A846FF-BBF5-4A02-BAF4-3C4772884C84}">
+  <sheetPr codeName="Sheet9">
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="21">
+        <v>4.1868000000000002E-2</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89305455-607F-41AA-8109-096F19F6FE72}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -40647,10 +42440,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FEB92-3C8E-4A89-8F18-2AEFFF284423}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="B2:K14"/>
+  <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40810,10 +42603,22 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$U$10,'EB2018'!$U$11),1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$U$10,'EB2019'!$U$11),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="H7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$U$10,'EB2020'!$U$11),1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$U$10,'EB2021'!$U$11),1)</f>
+        <v>1.3</v>
+      </c>
       <c r="J7" s="19"/>
       <c r="K7">
         <v>1</v>
@@ -40865,10 +42670,22 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="F9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$S$10,'EB2018'!$S$11),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$S$10,'EB2019'!$S$11),1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="H9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$S$10,'EB2020'!$S$11),1)</f>
+        <v>4</v>
+      </c>
+      <c r="I9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$S$10,'EB2021'!$S$11),1)</f>
+        <v>13.799999999999999</v>
+      </c>
       <c r="J9" s="19"/>
       <c r="K9">
         <v>1</v>
@@ -41033,6 +42850,18 @@
       <c r="K14">
         <v>1</v>
       </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="25" spans="6:9">
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41306,11 +43135,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
-  <dimension ref="B2:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E3FAF-1332-4EEA-86C9-3113D28D5888}">
+  <dimension ref="B2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41357,11 +43186,8 @@
       </c>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" t="s">
-        <v>456</v>
-      </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>506</v>
       </c>
       <c r="D4" t="s">
         <v>200</v>
@@ -41371,338 +43197,22 @@
         <v>IE,National</v>
       </c>
       <c r="F4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$70,'EB2018'!$AO$71),1)</f>
+        <v>2.1</v>
       </c>
       <c r="G4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$70,'EB2019'!$AO$71),1)</f>
+        <v>2</v>
       </c>
       <c r="H4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$70,'EB2020'!$AO$71),1)</f>
+        <v>2.1</v>
       </c>
       <c r="I4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$70,'EB2021'!$AO$71),1)</f>
+        <v>2.1</v>
       </c>
       <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="C5" t="s">
-        <v>450</v>
-      </c>
-      <c r="D5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="G5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="C6" t="s">
-        <v>445</v>
-      </c>
-      <c r="D6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
-        <v>9.1</v>
-      </c>
-      <c r="G6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
-        <v>7.8</v>
-      </c>
-      <c r="H6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
-        <v>7.8</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="C7" t="s">
-        <v>452</v>
-      </c>
-      <c r="D7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
-        <v>8.2999999999999989</v>
-      </c>
-      <c r="G7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
-        <v>7.6999999999999993</v>
-      </c>
-      <c r="H7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
-        <v>8</v>
-      </c>
-      <c r="I7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
-        <v>7.6</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="C8" t="s">
-        <v>446</v>
-      </c>
-      <c r="D8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
-        <v>29.5</v>
-      </c>
-      <c r="G8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
-        <v>30.8</v>
-      </c>
-      <c r="H8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
-        <v>31.5</v>
-      </c>
-      <c r="I8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
-        <v>31.5</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" t="s">
-        <v>456</v>
-      </c>
-      <c r="C9" t="s">
-        <v>454</v>
-      </c>
-      <c r="D9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="C10" t="s">
-        <v>447</v>
-      </c>
-      <c r="D10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E10" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
-        <v>25.3</v>
-      </c>
-      <c r="G10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
-        <v>24.8</v>
-      </c>
-      <c r="H10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
-        <v>24.700000000000003</v>
-      </c>
-      <c r="I10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
-        <v>25</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" t="s">
-        <v>456</v>
-      </c>
-      <c r="C11" t="s">
-        <v>455</v>
-      </c>
-      <c r="D11" t="s">
-        <v>200</v>
-      </c>
-      <c r="E11" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="C12" t="s">
-        <v>448</v>
-      </c>
-      <c r="D12" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
-        <v>2.3000000000000003</v>
-      </c>
-      <c r="G12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
-        <v>2.1</v>
-      </c>
-      <c r="H12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
-        <v>2.1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="C13" t="s">
-        <v>451</v>
-      </c>
-      <c r="D13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E13" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
-        <v>50.300000000000004</v>
-      </c>
-      <c r="G13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
-        <v>49.9</v>
-      </c>
-      <c r="H13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
-        <v>56.2</v>
-      </c>
-      <c r="I13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
-        <v>51.2</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="C14" t="s">
-        <v>449</v>
-      </c>
-      <c r="D14" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F14" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$56),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="G14" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$56),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="H14" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$56),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="I14" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$56),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="J14">
         <v>1</v>
       </c>
     </row>
@@ -41712,12 +43222,505 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C78897-D520-4428-BFE9-032417D86FB7}">
+  <dimension ref="B2:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B3" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="29">
+        <v>2018</v>
+      </c>
+      <c r="G3" s="29">
+        <v>2019</v>
+      </c>
+      <c r="H3" s="29">
+        <v>2020</v>
+      </c>
+      <c r="I3" s="29">
+        <v>2021</v>
+      </c>
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="C4" t="s">
+        <v>508</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$30),1)</f>
+        <v>23.6</v>
+      </c>
+      <c r="G4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$30),1)</f>
+        <v>24.1</v>
+      </c>
+      <c r="H4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$30),1)</f>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="I4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$30),1)</f>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
+  <dimension ref="B2:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B3" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="29">
+        <v>2018</v>
+      </c>
+      <c r="G3" s="29">
+        <v>2019</v>
+      </c>
+      <c r="H3" s="29">
+        <v>2020</v>
+      </c>
+      <c r="I3" s="29">
+        <v>2021</v>
+      </c>
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="C5" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F5" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="G5" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H5" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I5" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="C6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F6" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
+        <v>9.1</v>
+      </c>
+      <c r="G6" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
+        <v>7.8</v>
+      </c>
+      <c r="H6" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I6" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
+        <v>7.8</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="C7" t="s">
+        <v>452</v>
+      </c>
+      <c r="D7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="G7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
+        <v>7.6999999999999993</v>
+      </c>
+      <c r="H7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
+        <v>8</v>
+      </c>
+      <c r="I7" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
+        <v>7.6</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="C8" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F8" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
+        <v>29.5</v>
+      </c>
+      <c r="G8" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
+        <v>30.8</v>
+      </c>
+      <c r="H8" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
+        <v>31.5</v>
+      </c>
+      <c r="I8" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
+        <v>31.5</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="C10" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F10" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
+        <v>25.3</v>
+      </c>
+      <c r="G10" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
+        <v>24.8</v>
+      </c>
+      <c r="H10" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
+        <v>24.700000000000003</v>
+      </c>
+      <c r="I10" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F11" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="C12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F12" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="G12" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="H12" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I12" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="C13" t="s">
+        <v>451</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F13" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
+        <v>50.300000000000004</v>
+      </c>
+      <c r="G13" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
+        <v>49.9</v>
+      </c>
+      <c r="H13" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
+        <v>56.2</v>
+      </c>
+      <c r="I13" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
+        <v>51.2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="C14" t="s">
+        <v>449</v>
+      </c>
+      <c r="D14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$56),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$56),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="H14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$56),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$56),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42108,1557 +44111,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC29CEA2-2536-449C-BE94-1AB8A11FBF6A}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AH16"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="32" width="6.85546875" customWidth="1"/>
-    <col min="33" max="33" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:34" ht="21">
-      <c r="A1" s="42" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
-      <c r="A4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34">
-      <c r="B5" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-    </row>
-    <row r="6" spans="1:34" ht="15.75" thickBot="1">
-      <c r="B6" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F6" s="37" t="str">
-        <f>Regions!C$3</f>
-        <v>IE</v>
-      </c>
-      <c r="G6" s="37" t="str">
-        <f>Regions!E$3</f>
-        <v>IE-CW</v>
-      </c>
-      <c r="H6" s="37" t="str">
-        <f>Regions!F$3</f>
-        <v>IE-D</v>
-      </c>
-      <c r="I6" s="37" t="str">
-        <f>Regions!G$3</f>
-        <v>IE-KE</v>
-      </c>
-      <c r="J6" s="37" t="str">
-        <f>Regions!H$3</f>
-        <v>IE-KK</v>
-      </c>
-      <c r="K6" s="37" t="str">
-        <f>Regions!I$3</f>
-        <v>IE-LS</v>
-      </c>
-      <c r="L6" s="37" t="str">
-        <f>Regions!J$3</f>
-        <v>IE-LD</v>
-      </c>
-      <c r="M6" s="37" t="str">
-        <f>Regions!K$3</f>
-        <v>IE-LH</v>
-      </c>
-      <c r="N6" s="37" t="str">
-        <f>Regions!L$3</f>
-        <v>IE-MH</v>
-      </c>
-      <c r="O6" s="37" t="str">
-        <f>Regions!M$3</f>
-        <v>IE-OY</v>
-      </c>
-      <c r="P6" s="37" t="str">
-        <f>Regions!N$3</f>
-        <v>IE-WH</v>
-      </c>
-      <c r="Q6" s="37" t="str">
-        <f>Regions!O$3</f>
-        <v>IE-WX</v>
-      </c>
-      <c r="R6" s="37" t="str">
-        <f>Regions!P$3</f>
-        <v>IE-WW</v>
-      </c>
-      <c r="S6" s="37" t="str">
-        <f>Regions!Q$3</f>
-        <v>IE-CE</v>
-      </c>
-      <c r="T6" s="37" t="str">
-        <f>Regions!R$3</f>
-        <v>IE-CO</v>
-      </c>
-      <c r="U6" s="37" t="str">
-        <f>Regions!S$3</f>
-        <v>IE-KY</v>
-      </c>
-      <c r="V6" s="37" t="str">
-        <f>Regions!T$3</f>
-        <v>IE-LK</v>
-      </c>
-      <c r="W6" s="37" t="str">
-        <f>Regions!U$3</f>
-        <v>IE-TA</v>
-      </c>
-      <c r="X6" s="37" t="str">
-        <f>Regions!V$3</f>
-        <v>IE-WD</v>
-      </c>
-      <c r="Y6" s="37" t="str">
-        <f>Regions!W$3</f>
-        <v>IE-G</v>
-      </c>
-      <c r="Z6" s="37" t="str">
-        <f>Regions!X$3</f>
-        <v>IE-LM</v>
-      </c>
-      <c r="AA6" s="37" t="str">
-        <f>Regions!Y$3</f>
-        <v>IE-MO</v>
-      </c>
-      <c r="AB6" s="37" t="str">
-        <f>Regions!Z$3</f>
-        <v>IE-RN</v>
-      </c>
-      <c r="AC6" s="37" t="str">
-        <f>Regions!AA$3</f>
-        <v>IE-SO</v>
-      </c>
-      <c r="AD6" s="37" t="str">
-        <f>Regions!AB$3</f>
-        <v>IE-CN</v>
-      </c>
-      <c r="AE6" s="37" t="str">
-        <f>Regions!AC$3</f>
-        <v>IE-DL</v>
-      </c>
-      <c r="AF6" s="37" t="str">
-        <f>Regions!AD$3</f>
-        <v>IE-MN</v>
-      </c>
-      <c r="AG6" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="AH6" s="36" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34">
-      <c r="C7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7">
-        <v>2020</v>
-      </c>
-      <c r="F7" s="35">
-        <f>'New vehicle sales'!C6/1000</f>
-        <v>38.232999999999997</v>
-      </c>
-      <c r="G7" s="33">
-        <f>$F$7*'New vehicle sales'!D43</f>
-        <v>0.45710685960227732</v>
-      </c>
-      <c r="H7" s="33">
-        <f>$F$7*'New vehicle sales'!E43</f>
-        <v>10.817941425680914</v>
-      </c>
-      <c r="I7" s="33">
-        <f>$F$7*'New vehicle sales'!F43</f>
-        <v>1.7864839578610465</v>
-      </c>
-      <c r="J7" s="33">
-        <f>$F$7*'New vehicle sales'!G43</f>
-        <v>0.79673343448417733</v>
-      </c>
-      <c r="K7" s="33">
-        <f>$F$7*'New vehicle sales'!H43</f>
-        <v>0.68003196247688613</v>
-      </c>
-      <c r="L7" s="33">
-        <f>$F$7*'New vehicle sales'!I43</f>
-        <v>0.32816919610278722</v>
-      </c>
-      <c r="M7" s="33">
-        <f>$F$7*'New vehicle sales'!J43</f>
-        <v>1.0348092547772767</v>
-      </c>
-      <c r="N7" s="33">
-        <f>$F$7*'New vehicle sales'!K43</f>
-        <v>1.5660076990842859</v>
-      </c>
-      <c r="O7" s="33">
-        <f>$F$7*'New vehicle sales'!L43</f>
-        <v>0.62594863840113013</v>
-      </c>
-      <c r="P7" s="33">
-        <f>$F$7*'New vehicle sales'!M43</f>
-        <v>0.71273406742946244</v>
-      </c>
-      <c r="Q7" s="33">
-        <f>$F$7*'New vehicle sales'!N43</f>
-        <v>1.2021174951410833</v>
-      </c>
-      <c r="R7" s="33">
-        <f>$F$7*'New vehicle sales'!O43</f>
-        <v>1.1435299037246951</v>
-      </c>
-      <c r="S7" s="33">
-        <f>$F$7*'New vehicle sales'!P43</f>
-        <v>0.95398134155420122</v>
-      </c>
-      <c r="T7" s="33">
-        <f>$F$7*'New vehicle sales'!Q43</f>
-        <v>4.3586855662644748</v>
-      </c>
-      <c r="U7" s="33">
-        <f>$F$7*'New vehicle sales'!R43</f>
-        <v>1.185939066101201</v>
-      </c>
-      <c r="V7" s="33">
-        <f>$F$7*'New vehicle sales'!S43</f>
-        <v>1.5648434945131779</v>
-      </c>
-      <c r="W7" s="33">
-        <f>$F$7*'New vehicle sales'!T43</f>
-        <v>1.2810505650622175</v>
-      </c>
-      <c r="X7" s="33">
-        <f>$F$7*'New vehicle sales'!U43</f>
-        <v>0.93277676036594825</v>
-      </c>
-      <c r="Y7" s="33">
-        <f>$F$7*'New vehicle sales'!V43</f>
-        <v>2.0719469186967694</v>
-      </c>
-      <c r="Z7" s="33">
-        <f>$F$7*'New vehicle sales'!W43</f>
-        <v>0.25728118121786298</v>
-      </c>
-      <c r="AA7" s="33">
-        <f>$F$7*'New vehicle sales'!X43</f>
-        <v>1.0478403169766459</v>
-      </c>
-      <c r="AB7" s="33">
-        <f>$F$7*'New vehicle sales'!Y43</f>
-        <v>0.518223585086935</v>
-      </c>
-      <c r="AC7" s="33">
-        <f>$F$7*'New vehicle sales'!Z43</f>
-        <v>0.52618032115568125</v>
-      </c>
-      <c r="AD7" s="33">
-        <f>$F$7*'New vehicle sales'!AA43</f>
-        <v>0.6116168786809365</v>
-      </c>
-      <c r="AE7" s="33">
-        <f>$F$7*'New vehicle sales'!AB43</f>
-        <v>1.2781520971300098</v>
-      </c>
-      <c r="AF7" s="33">
-        <f>$F$7*'New vehicle sales'!AC43</f>
-        <v>0.49286801242790335</v>
-      </c>
-      <c r="AG7" t="str">
-        <f>'New vehicle sales'!B57</f>
-        <v>T-CAR-ICE_DST21</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34">
-      <c r="C8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8">
-        <v>2020</v>
-      </c>
-      <c r="F8" s="35">
-        <f>'New vehicle sales'!C7/1000</f>
-        <v>32.6</v>
-      </c>
-      <c r="G8" s="33">
-        <f>$F$8*'New vehicle sales'!D43</f>
-        <v>0.38975972649371593</v>
-      </c>
-      <c r="H8" s="33">
-        <f>$F$8*'New vehicle sales'!E43</f>
-        <v>9.2240967352077483</v>
-      </c>
-      <c r="I8" s="33">
-        <f>$F$8*'New vehicle sales'!F43</f>
-        <v>1.5232751033471117</v>
-      </c>
-      <c r="J8" s="33">
-        <f>$F$8*'New vehicle sales'!G43</f>
-        <v>0.67934794455533654</v>
-      </c>
-      <c r="K8" s="33">
-        <f>$F$8*'New vehicle sales'!H43</f>
-        <v>0.57984050366820528</v>
-      </c>
-      <c r="L8" s="33">
-        <f>$F$8*'New vehicle sales'!I43</f>
-        <v>0.27981889448776881</v>
-      </c>
-      <c r="M8" s="33">
-        <f>$F$8*'New vehicle sales'!J43</f>
-        <v>0.88234723159938333</v>
-      </c>
-      <c r="N8" s="33">
-        <f>$F$8*'New vehicle sales'!K43</f>
-        <v>1.3352823736078185</v>
-      </c>
-      <c r="O8" s="33">
-        <f>$F$8*'New vehicle sales'!L43</f>
-        <v>0.53372546260761244</v>
-      </c>
-      <c r="P8" s="33">
-        <f>$F$8*'New vehicle sales'!M43</f>
-        <v>0.60772449449952859</v>
-      </c>
-      <c r="Q8" s="33">
-        <f>$F$8*'New vehicle sales'!N43</f>
-        <v>1.0250053707948454</v>
-      </c>
-      <c r="R8" s="33">
-        <f>$F$8*'New vehicle sales'!O43</f>
-        <v>0.97504969166492472</v>
-      </c>
-      <c r="S8" s="33">
-        <f>$F$8*'New vehicle sales'!P43</f>
-        <v>0.81342797412358336</v>
-      </c>
-      <c r="T8" s="33">
-        <f>$F$8*'New vehicle sales'!Q43</f>
-        <v>3.7165053608197605</v>
-      </c>
-      <c r="U8" s="33">
-        <f>$F$8*'New vehicle sales'!R43</f>
-        <v>1.0112105656082222</v>
-      </c>
-      <c r="V8" s="33">
-        <f>$F$8*'New vehicle sales'!S43</f>
-        <v>1.3342896953189549</v>
-      </c>
-      <c r="W8" s="33">
-        <f>$F$8*'New vehicle sales'!T43</f>
-        <v>1.0923089587798052</v>
-      </c>
-      <c r="X8" s="33">
-        <f>$F$8*'New vehicle sales'!U43</f>
-        <v>0.79534753715193462</v>
-      </c>
-      <c r="Y8" s="33">
-        <f>$F$8*'New vehicle sales'!V43</f>
-        <v>1.7666798197764939</v>
-      </c>
-      <c r="Z8" s="33">
-        <f>$F$8*'New vehicle sales'!W43</f>
-        <v>0.21937505578171562</v>
-      </c>
-      <c r="AA8" s="33">
-        <f>$F$8*'New vehicle sales'!X43</f>
-        <v>0.89345838237749231</v>
-      </c>
-      <c r="AB8" s="33">
-        <f>$F$8*'New vehicle sales'!Y43</f>
-        <v>0.44187191363047851</v>
-      </c>
-      <c r="AC8" s="33">
-        <f>$F$8*'New vehicle sales'!Z43</f>
-        <v>0.44865635628057465</v>
-      </c>
-      <c r="AD8" s="33">
-        <f>$F$8*'New vehicle sales'!AA43</f>
-        <v>0.52150525056884189</v>
-      </c>
-      <c r="AE8" s="33">
-        <f>$F$8*'New vehicle sales'!AB43</f>
-        <v>1.0898375321433926</v>
-      </c>
-      <c r="AF8" s="33">
-        <f>$F$8*'New vehicle sales'!AC43</f>
-        <v>0.42025206510474333</v>
-      </c>
-      <c r="AG8" t="str">
-        <f>'New vehicle sales'!B56</f>
-        <v>T-CAR-ICE_GSL21</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34">
-      <c r="C9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9">
-        <v>2020</v>
-      </c>
-      <c r="F9" s="35">
-        <f>'New vehicle sales'!C8/1000</f>
-        <v>10.474</v>
-      </c>
-      <c r="G9" s="33">
-        <f>$F$9*'New vehicle sales'!D43</f>
-        <v>0.12522525691089512</v>
-      </c>
-      <c r="H9" s="33">
-        <f>$F$9*'New vehicle sales'!E43</f>
-        <v>2.9635947608762563</v>
-      </c>
-      <c r="I9" s="33">
-        <f>$F$9*'New vehicle sales'!F43</f>
-        <v>0.4894105347379647</v>
-      </c>
-      <c r="J9" s="33">
-        <f>$F$9*'New vehicle sales'!G43</f>
-        <v>0.21826657580590783</v>
-      </c>
-      <c r="K9" s="33">
-        <f>$F$9*'New vehicle sales'!H43</f>
-        <v>0.18629599495155771</v>
-      </c>
-      <c r="L9" s="33">
-        <f>$F$9*'New vehicle sales'!I43</f>
-        <v>8.9902549106284979E-2</v>
-      </c>
-      <c r="M9" s="33">
-        <f>$F$9*'New vehicle sales'!J43</f>
-        <v>0.28348788048380186</v>
-      </c>
-      <c r="N9" s="33">
-        <f>$F$9*'New vehicle sales'!K43</f>
-        <v>0.42901066199902738</v>
-      </c>
-      <c r="O9" s="33">
-        <f>$F$9*'New vehicle sales'!L43</f>
-        <v>0.17147976979607768</v>
-      </c>
-      <c r="P9" s="33">
-        <f>$F$9*'New vehicle sales'!M43</f>
-        <v>0.19525479617754793</v>
-      </c>
-      <c r="Q9" s="33">
-        <f>$F$9*'New vehicle sales'!N43</f>
-        <v>0.32932227772101874</v>
-      </c>
-      <c r="R9" s="33">
-        <f>$F$9*'New vehicle sales'!O43</f>
-        <v>0.31327210032203745</v>
-      </c>
-      <c r="S9" s="33">
-        <f>$F$9*'New vehicle sales'!P43</f>
-        <v>0.26134492641013535</v>
-      </c>
-      <c r="T9" s="33">
-        <f>$F$9*'New vehicle sales'!Q43</f>
-        <v>1.1940698512032568</v>
-      </c>
-      <c r="U9" s="33">
-        <f>$F$9*'New vehicle sales'!R43</f>
-        <v>0.32489016761289935</v>
-      </c>
-      <c r="V9" s="33">
-        <f>$F$9*'New vehicle sales'!S43</f>
-        <v>0.4286917260359121</v>
-      </c>
-      <c r="W9" s="33">
-        <f>$F$9*'New vehicle sales'!T43</f>
-        <v>0.35094613602023556</v>
-      </c>
-      <c r="X9" s="33">
-        <f>$F$9*'New vehicle sales'!U43</f>
-        <v>0.2555358927647044</v>
-      </c>
-      <c r="Y9" s="33">
-        <f>$F$9*'New vehicle sales'!V43</f>
-        <v>0.56761363289383426</v>
-      </c>
-      <c r="Z9" s="33">
-        <f>$F$9*'New vehicle sales'!W43</f>
-        <v>7.0482648290113165E-2</v>
-      </c>
-      <c r="AA9" s="33">
-        <f>$F$9*'New vehicle sales'!X43</f>
-        <v>0.28705776371232683</v>
-      </c>
-      <c r="AB9" s="33">
-        <f>$F$9*'New vehicle sales'!Y43</f>
-        <v>0.14196829519526477</v>
-      </c>
-      <c r="AC9" s="33">
-        <f>$F$9*'New vehicle sales'!Z43</f>
-        <v>0.14414805753628032</v>
-      </c>
-      <c r="AD9" s="33">
-        <f>$F$9*'New vehicle sales'!AA43</f>
-        <v>0.16755355811221012</v>
-      </c>
-      <c r="AE9" s="33">
-        <f>$F$9*'New vehicle sales'!AB43</f>
-        <v>0.3501520954499967</v>
-      </c>
-      <c r="AF9" s="33">
-        <f>$F$9*'New vehicle sales'!AC43</f>
-        <v>0.13502208987445036</v>
-      </c>
-      <c r="AG9" t="str">
-        <f>'New vehicle sales'!B62</f>
-        <v>T-CAR-HEV_GSL21</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34">
-      <c r="C10" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10">
-        <v>2020</v>
-      </c>
-      <c r="F10" s="35">
-        <f>'New vehicle sales'!C9/1000</f>
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="G10" s="33">
-        <f>$F$10*'New vehicle sales'!D43</f>
-        <v>4.7978704982186565E-2</v>
-      </c>
-      <c r="H10" s="33">
-        <f>$F$10*'New vehicle sales'!E43</f>
-        <v>1.135469331238917</v>
-      </c>
-      <c r="I10" s="33">
-        <f>$F$10*'New vehicle sales'!F43</f>
-        <v>0.18751236164821961</v>
-      </c>
-      <c r="J10" s="33">
-        <f>$F$10*'New vehicle sales'!G43</f>
-        <v>8.3626481641121644E-2</v>
-      </c>
-      <c r="K10" s="33">
-        <f>$F$10*'New vehicle sales'!H43</f>
-        <v>7.1377298810445008E-2</v>
-      </c>
-      <c r="L10" s="33">
-        <f>$F$10*'New vehicle sales'!I43</f>
-        <v>3.4445190907344055E-2</v>
-      </c>
-      <c r="M10" s="33">
-        <f>$F$10*'New vehicle sales'!J43</f>
-        <v>0.10861532025792409</v>
-      </c>
-      <c r="N10" s="33">
-        <f>$F$10*'New vehicle sales'!K43</f>
-        <v>0.16437080261620171</v>
-      </c>
-      <c r="O10" s="33">
-        <f>$F$10*'New vehicle sales'!L43</f>
-        <v>6.570062213019473E-2</v>
-      </c>
-      <c r="P10" s="33">
-        <f>$F$10*'New vehicle sales'!M43</f>
-        <v>7.4809766761552404E-2</v>
-      </c>
-      <c r="Q10" s="33">
-        <f>$F$10*'New vehicle sales'!N43</f>
-        <v>0.12617627463189307</v>
-      </c>
-      <c r="R10" s="33">
-        <f>$F$10*'New vehicle sales'!O43</f>
-        <v>0.12002682247396756</v>
-      </c>
-      <c r="S10" s="33">
-        <f>$F$10*'New vehicle sales'!P43</f>
-        <v>0.10013148650791226</v>
-      </c>
-      <c r="T10" s="33">
-        <f>$F$10*'New vehicle sales'!Q43</f>
-        <v>0.45749496972299686</v>
-      </c>
-      <c r="U10" s="33">
-        <f>$F$10*'New vehicle sales'!R43</f>
-        <v>0.12447815950263176</v>
-      </c>
-      <c r="V10" s="33">
-        <f>$F$10*'New vehicle sales'!S43</f>
-        <v>0.16424860574585784</v>
-      </c>
-      <c r="W10" s="33">
-        <f>$F$10*'New vehicle sales'!T43</f>
-        <v>0.13446122244120728</v>
-      </c>
-      <c r="X10" s="33">
-        <f>$F$10*'New vehicle sales'!U43</f>
-        <v>9.7905817993580169E-2</v>
-      </c>
-      <c r="Y10" s="33">
-        <f>$F$10*'New vehicle sales'!V43</f>
-        <v>0.21747503425653589</v>
-      </c>
-      <c r="Z10" s="33">
-        <f>$F$10*'New vehicle sales'!W43</f>
-        <v>2.7004665608957815E-2</v>
-      </c>
-      <c r="AA10" s="33">
-        <f>$F$10*'New vehicle sales'!X43</f>
-        <v>0.10998308246873854</v>
-      </c>
-      <c r="AB10" s="33">
-        <f>$F$10*'New vehicle sales'!Y43</f>
-        <v>5.4393619306721167E-2</v>
-      </c>
-      <c r="AC10" s="33">
-        <f>$F$10*'New vehicle sales'!Z43</f>
-        <v>5.5228771710243735E-2</v>
-      </c>
-      <c r="AD10" s="33">
-        <f>$F$10*'New vehicle sales'!AA43</f>
-        <v>6.4196336519409883E-2</v>
-      </c>
-      <c r="AE10" s="33">
-        <f>$F$10*'New vehicle sales'!AB43</f>
-        <v>0.13415699437090289</v>
-      </c>
-      <c r="AF10" s="33">
-        <f>$F$10*'New vehicle sales'!AC43</f>
-        <v>5.1732255744335424E-2</v>
-      </c>
-      <c r="AG10" t="str">
-        <f>'New vehicle sales'!B70</f>
-        <v>T-CAR-BEV100_ELC21</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34">
-      <c r="C11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11">
-        <v>2020</v>
-      </c>
-      <c r="F11" s="35">
-        <f>'New vehicle sales'!C10/1000</f>
-        <v>2.4590000000000001</v>
-      </c>
-      <c r="G11" s="33">
-        <f>$F$11*'New vehicle sales'!D43</f>
-        <v>2.9399360964664036E-2</v>
-      </c>
-      <c r="H11" s="33">
-        <f>$F$11*'New vehicle sales'!E43</f>
-        <v>0.69576852367717346</v>
-      </c>
-      <c r="I11" s="33">
-        <f>$F$11*'New vehicle sales'!F43</f>
-        <v>0.11489979997332969</v>
-      </c>
-      <c r="J11" s="33">
-        <f>$F$11*'New vehicle sales'!G43</f>
-        <v>5.1242840357716951E-2</v>
-      </c>
-      <c r="K11" s="33">
-        <f>$F$11*'New vehicle sales'!H43</f>
-        <v>4.3737049034359404E-2</v>
-      </c>
-      <c r="L11" s="33">
-        <f>$F$11*'New vehicle sales'!I43</f>
-        <v>2.1106584709982317E-2</v>
-      </c>
-      <c r="M11" s="33">
-        <f>$F$11*'New vehicle sales'!J43</f>
-        <v>6.6554964493953483E-2</v>
-      </c>
-      <c r="N11" s="33">
-        <f>$F$11*'New vehicle sales'!K43</f>
-        <v>0.10071961216876153</v>
-      </c>
-      <c r="O11" s="33">
-        <f>$F$11*'New vehicle sales'!L43</f>
-        <v>4.0258616949451501E-2</v>
-      </c>
-      <c r="P11" s="33">
-        <f>$F$11*'New vehicle sales'!M43</f>
-        <v>4.5840323066697573E-2</v>
-      </c>
-      <c r="Q11" s="33">
-        <f>$F$11*'New vehicle sales'!N43</f>
-        <v>7.7315589165169479E-2</v>
-      </c>
-      <c r="R11" s="33">
-        <f>$F$11*'New vehicle sales'!O43</f>
-        <v>7.3547459871289869E-2</v>
-      </c>
-      <c r="S11" s="33">
-        <f>$F$11*'New vehicle sales'!P43</f>
-        <v>6.135642295613164E-2</v>
-      </c>
-      <c r="T11" s="33">
-        <f>$F$11*'New vehicle sales'!Q43</f>
-        <v>0.28033394730845984</v>
-      </c>
-      <c r="U11" s="33">
-        <f>$F$11*'New vehicle sales'!R43</f>
-        <v>7.6275054626706085E-2</v>
-      </c>
-      <c r="V11" s="33">
-        <f>$F$11*'New vehicle sales'!S43</f>
-        <v>0.10064473499353713</v>
-      </c>
-      <c r="W11" s="33">
-        <f>$F$11*'New vehicle sales'!T43</f>
-        <v>8.2392261645384685E-2</v>
-      </c>
-      <c r="X11" s="33">
-        <f>$F$11*'New vehicle sales'!U43</f>
-        <v>5.9992625578423532E-2</v>
-      </c>
-      <c r="Y11" s="33">
-        <f>$F$11*'New vehicle sales'!V43</f>
-        <v>0.13325968333835578</v>
-      </c>
-      <c r="Z11" s="33">
-        <f>$F$11*'New vehicle sales'!W43</f>
-        <v>1.6547339330283396E-2</v>
-      </c>
-      <c r="AA11" s="33">
-        <f>$F$11*'New vehicle sales'!X43</f>
-        <v>6.7393072462155021E-2</v>
-      </c>
-      <c r="AB11" s="33">
-        <f>$F$11*'New vehicle sales'!Y43</f>
-        <v>3.3330154466789774E-2</v>
-      </c>
-      <c r="AC11" s="33">
-        <f>$F$11*'New vehicle sales'!Z43</f>
-        <v>3.3841901229875244E-2</v>
-      </c>
-      <c r="AD11" s="33">
-        <f>$F$11*'New vehicle sales'!AA43</f>
-        <v>3.9336853102723376E-2</v>
-      </c>
-      <c r="AE11" s="33">
-        <f>$F$11*'New vehicle sales'!AB43</f>
-        <v>8.2205843298791478E-2</v>
-      </c>
-      <c r="AF11" s="33">
-        <f>$F$11*'New vehicle sales'!AC43</f>
-        <v>3.1699381229833248E-2</v>
-      </c>
-      <c r="AG11" t="str">
-        <f>'New vehicle sales'!B66</f>
-        <v>T-CAR-PHEV40_GSL21</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34">
-      <c r="C12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E12">
-        <v>2020</v>
-      </c>
-      <c r="F12" s="35">
-        <f>'New vehicle sales'!C11/1000</f>
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="G12" s="33">
-        <f>$F$12*'New vehicle sales'!D43</f>
-        <v>6.1213797535209372E-3</v>
-      </c>
-      <c r="H12" s="33">
-        <f>$F$12*'New vehicle sales'!E43</f>
-        <v>0.14486924933823211</v>
-      </c>
-      <c r="I12" s="33">
-        <f>$F$12*'New vehicle sales'!F43</f>
-        <v>2.3923829843979179E-2</v>
-      </c>
-      <c r="J12" s="33">
-        <f>$F$12*'New vehicle sales'!G43</f>
-        <v>1.0669513730439641E-2</v>
-      </c>
-      <c r="K12" s="33">
-        <f>$F$12*'New vehicle sales'!H43</f>
-        <v>9.106697480923959E-3</v>
-      </c>
-      <c r="L12" s="33">
-        <f>$F$12*'New vehicle sales'!I43</f>
-        <v>4.3947016557588231E-3</v>
-      </c>
-      <c r="M12" s="33">
-        <f>$F$12*'New vehicle sales'!J43</f>
-        <v>1.3857723391990314E-2</v>
-      </c>
-      <c r="N12" s="33">
-        <f>$F$12*'New vehicle sales'!K43</f>
-        <v>2.0971305990405004E-2</v>
-      </c>
-      <c r="O12" s="33">
-        <f>$F$12*'New vehicle sales'!L43</f>
-        <v>8.3824367133465503E-3</v>
-      </c>
-      <c r="P12" s="33">
-        <f>$F$12*'New vehicle sales'!M43</f>
-        <v>9.544630097661308E-3</v>
-      </c>
-      <c r="Q12" s="33">
-        <f>$F$12*'New vehicle sales'!N43</f>
-        <v>1.6098243860336221E-2</v>
-      </c>
-      <c r="R12" s="33">
-        <f>$F$12*'New vehicle sales'!O43</f>
-        <v>1.5313663869093296E-2</v>
-      </c>
-      <c r="S12" s="33">
-        <f>$F$12*'New vehicle sales'!P43</f>
-        <v>1.2775310513842781E-2</v>
-      </c>
-      <c r="T12" s="33">
-        <f>$F$12*'New vehicle sales'!Q43</f>
-        <v>5.8369654746617095E-2</v>
-      </c>
-      <c r="U12" s="33">
-        <f>$F$12*'New vehicle sales'!R43</f>
-        <v>1.5881589251270239E-2</v>
-      </c>
-      <c r="V12" s="33">
-        <f>$F$12*'New vehicle sales'!S43</f>
-        <v>2.0955715460224077E-2</v>
-      </c>
-      <c r="W12" s="33">
-        <f>$F$12*'New vehicle sales'!T43</f>
-        <v>1.7155281806603074E-2</v>
-      </c>
-      <c r="X12" s="33">
-        <f>$F$12*'New vehicle sales'!U43</f>
-        <v>1.2491347822754311E-2</v>
-      </c>
-      <c r="Y12" s="33">
-        <f>$F$12*'New vehicle sales'!V43</f>
-        <v>2.7746627844342481E-2</v>
-      </c>
-      <c r="Z12" s="33">
-        <f>$F$12*'New vehicle sales'!W43</f>
-        <v>3.4453996490870675E-3</v>
-      </c>
-      <c r="AA12" s="33">
-        <f>$F$12*'New vehicle sales'!X43</f>
-        <v>1.4032229809118897E-2</v>
-      </c>
-      <c r="AB12" s="33">
-        <f>$F$12*'New vehicle sales'!Y43</f>
-        <v>6.939828827570705E-3</v>
-      </c>
-      <c r="AC12" s="33">
-        <f>$F$12*'New vehicle sales'!Z43</f>
-        <v>7.0463820372900065E-3</v>
-      </c>
-      <c r="AD12" s="33">
-        <f>$F$12*'New vehicle sales'!AA43</f>
-        <v>8.1905119107744482E-3</v>
-      </c>
-      <c r="AE12" s="33">
-        <f>$F$12*'New vehicle sales'!AB43</f>
-        <v>1.7116466762497454E-2</v>
-      </c>
-      <c r="AF12" s="33">
-        <f>$F$12*'New vehicle sales'!AC43</f>
-        <v>6.6002778323198952E-3</v>
-      </c>
-      <c r="AG12" t="str">
-        <f>'New vehicle sales'!B63</f>
-        <v>T-CAR-HEV_DST21</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34">
-      <c r="C13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E13">
-        <v>2020</v>
-      </c>
-      <c r="F13" s="35">
-        <f>'New vehicle sales'!C12/1000</f>
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="G13" s="33">
-        <f>$F$13*'New vehicle sales'!D43</f>
-        <v>3.9454205442615418E-4</v>
-      </c>
-      <c r="H13" s="33">
-        <f>$F$13*'New vehicle sales'!E43</f>
-        <v>9.3372758362532428E-3</v>
-      </c>
-      <c r="I13" s="33">
-        <f>$F$13*'New vehicle sales'!F43</f>
-        <v>1.5419655954127206E-3</v>
-      </c>
-      <c r="J13" s="33">
-        <f>$F$13*'New vehicle sales'!G43</f>
-        <v>6.8768350215724257E-4</v>
-      </c>
-      <c r="K13" s="33">
-        <f>$F$13*'New vehicle sales'!H43</f>
-        <v>5.8695511107517706E-4</v>
-      </c>
-      <c r="L13" s="33">
-        <f>$F$13*'New vehicle sales'!I43</f>
-        <v>2.8325225515633037E-4</v>
-      </c>
-      <c r="M13" s="33">
-        <f>$F$13*'New vehicle sales'!J43</f>
-        <v>8.9317357799937572E-4</v>
-      </c>
-      <c r="N13" s="33">
-        <f>$F$13*'New vehicle sales'!K43</f>
-        <v>1.3516662064128224E-3</v>
-      </c>
-      <c r="O13" s="33">
-        <f>$F$13*'New vehicle sales'!L43</f>
-        <v>5.4027424128991436E-4</v>
-      </c>
-      <c r="P13" s="33">
-        <f>$F$13*'New vehicle sales'!M43</f>
-        <v>6.1518123676332652E-4</v>
-      </c>
-      <c r="Q13" s="33">
-        <f>$F$13*'New vehicle sales'!N43</f>
-        <v>1.0375821238107332E-3</v>
-      </c>
-      <c r="R13" s="33">
-        <f>$F$13*'New vehicle sales'!O43</f>
-        <v>9.8701349156265377E-4</v>
-      </c>
-      <c r="S13" s="33">
-        <f>$F$13*'New vehicle sales'!P43</f>
-        <v>8.2340868546252298E-4</v>
-      </c>
-      <c r="T13" s="33">
-        <f>$F$13*'New vehicle sales'!Q43</f>
-        <v>3.7621066535905552E-3</v>
-      </c>
-      <c r="U13" s="33">
-        <f>$F$13*'New vehicle sales'!R43</f>
-        <v>1.0236180572107771E-3</v>
-      </c>
-      <c r="V13" s="33">
-        <f>$F$13*'New vehicle sales'!S43</f>
-        <v>1.3506613480222551E-3</v>
-      </c>
-      <c r="W13" s="33">
-        <f>$F$13*'New vehicle sales'!T43</f>
-        <v>1.1057115226912138E-3</v>
-      </c>
-      <c r="X13" s="33">
-        <f>$F$13*'New vehicle sales'!U43</f>
-        <v>8.051064026384614E-4</v>
-      </c>
-      <c r="Y13" s="33">
-        <f>$F$13*'New vehicle sales'!V43</f>
-        <v>1.7883568727798866E-3</v>
-      </c>
-      <c r="Z13" s="33">
-        <f>$F$13*'New vehicle sales'!W43</f>
-        <v>2.2206677425756489E-4</v>
-      </c>
-      <c r="AA13" s="33">
-        <f>$F$13*'New vehicle sales'!X43</f>
-        <v>9.0442106191586651E-4</v>
-      </c>
-      <c r="AB13" s="33">
-        <f>$F$13*'New vehicle sales'!Y43</f>
-        <v>4.4729365490201812E-4</v>
-      </c>
-      <c r="AC13" s="33">
-        <f>$F$13*'New vehicle sales'!Z43</f>
-        <v>4.5416134224720743E-4</v>
-      </c>
-      <c r="AD13" s="33">
-        <f>$F$13*'New vehicle sales'!AA43</f>
-        <v>5.2790408799913439E-4</v>
-      </c>
-      <c r="AE13" s="33">
-        <f>$F$13*'New vehicle sales'!AB43</f>
-        <v>1.1032097718015937E-3</v>
-      </c>
-      <c r="AF13" s="33">
-        <f>$F$13*'New vehicle sales'!AC43</f>
-        <v>4.2540853216124324E-4</v>
-      </c>
-      <c r="AG13" t="str">
-        <f>'New vehicle sales'!B69</f>
-        <v>T-CAR-PHEV40_DST21</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34">
-      <c r="C14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" t="s">
-        <v>222</v>
-      </c>
-      <c r="E14">
-        <v>2020</v>
-      </c>
-      <c r="F14" s="34">
-        <f>'New vehicle sales'!C19/1000</f>
-        <v>20.928000000000001</v>
-      </c>
-      <c r="G14" s="33">
-        <f>($F$14*'New vehicle sales'!D43)</f>
-        <v>0.25021139742516835</v>
-      </c>
-      <c r="H14" s="33">
-        <f>($F$14*'New vehicle sales'!E43)</f>
-        <v>5.9215305667002385</v>
-      </c>
-      <c r="I14" s="33">
-        <f>($F$14*'New vehicle sales'!F43)</f>
-        <v>0.97788654487264892</v>
-      </c>
-      <c r="J14" s="33">
-        <f>($F$14*'New vehicle sales'!G43)</f>
-        <v>0.43611637373172035</v>
-      </c>
-      <c r="K14" s="33">
-        <f>($F$14*'New vehicle sales'!H43)</f>
-        <v>0.37223625953276684</v>
-      </c>
-      <c r="L14" s="33">
-        <f>($F$14*'New vehicle sales'!I43)</f>
-        <v>0.17963343017914188</v>
-      </c>
-      <c r="M14" s="33">
-        <f>($F$14*'New vehicle sales'!J43)</f>
-        <v>0.56643444364760409</v>
-      </c>
-      <c r="N14" s="33">
-        <f>($F$14*'New vehicle sales'!K43)</f>
-        <v>0.85720213235780451</v>
-      </c>
-      <c r="O14" s="33">
-        <f>($F$14*'New vehicle sales'!L43)</f>
-        <v>0.34263210065804023</v>
-      </c>
-      <c r="P14" s="33">
-        <f>($F$14*'New vehicle sales'!M43)</f>
-        <v>0.390136755241906</v>
-      </c>
-      <c r="Q14" s="33">
-        <f>($F$14*'New vehicle sales'!N43)</f>
-        <v>0.65801571779124313</v>
-      </c>
-      <c r="R14" s="33">
-        <f>($F$14*'New vehicle sales'!O43)</f>
-        <v>0.62594601064918842</v>
-      </c>
-      <c r="S14" s="33">
-        <f>($F$14*'New vehicle sales'!P43)</f>
-        <v>0.52219081725332372</v>
-      </c>
-      <c r="T14" s="33">
-        <f>($F$14*'New vehicle sales'!Q43)</f>
-        <v>2.3858596377679739</v>
-      </c>
-      <c r="U14" s="33">
-        <f>($F$14*'New vehicle sales'!R43)</f>
-        <v>0.64915996064567105</v>
-      </c>
-      <c r="V14" s="33">
-        <f>($F$14*'New vehicle sales'!S43)</f>
-        <v>0.85656486943665922</v>
-      </c>
-      <c r="W14" s="33">
-        <f>($F$14*'New vehicle sales'!T43)</f>
-        <v>0.70122214384490067</v>
-      </c>
-      <c r="X14" s="33">
-        <f>($F$14*'New vehicle sales'!U43)</f>
-        <v>0.51058384225508247</v>
-      </c>
-      <c r="Y14" s="33">
-        <f>($F$14*'New vehicle sales'!V43)</f>
-        <v>1.134143413137499</v>
-      </c>
-      <c r="Z14" s="33">
-        <f>($F$14*'New vehicle sales'!W43)</f>
-        <v>0.14083071065643388</v>
-      </c>
-      <c r="AA14" s="33">
-        <f>($F$14*'New vehicle sales'!X43)</f>
-        <v>0.573567393447735</v>
-      </c>
-      <c r="AB14" s="33">
-        <f>($F$14*'New vehicle sales'!Y43)</f>
-        <v>0.28366550332695256</v>
-      </c>
-      <c r="AC14" s="33">
-        <f>($F$14*'New vehicle sales'!Z43)</f>
-        <v>0.28802086577422903</v>
-      </c>
-      <c r="AD14" s="33">
-        <f>($F$14*'New vehicle sales'!AA43)</f>
-        <v>0.33478717435290561</v>
-      </c>
-      <c r="AE14" s="33">
-        <f>($F$14*'New vehicle sales'!AB43)</f>
-        <v>0.69963557891708339</v>
-      </c>
-      <c r="AF14" s="33">
-        <f>($F$14*'New vehicle sales'!AC43)</f>
-        <v>0.26978635639607573</v>
-      </c>
-      <c r="AG14" t="str">
-        <f>'New vehicle sales'!B107</f>
-        <v>T-LGT-ICE_DST61</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34">
-      <c r="C15" t="s">
-        <v>223</v>
-      </c>
-      <c r="D15" t="s">
-        <v>222</v>
-      </c>
-      <c r="E15">
-        <v>2020</v>
-      </c>
-      <c r="F15" s="34">
-        <f>'New vehicle sales'!C20/1000</f>
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="G15" s="33">
-        <f>($F$15*'New vehicle sales'!D43)</f>
-        <v>8.6918810172064865E-3</v>
-      </c>
-      <c r="H15" s="33">
-        <f>($F$15*'New vehicle sales'!E43)</f>
-        <v>0.20570301615018505</v>
-      </c>
-      <c r="I15" s="33">
-        <f>($F$15*'New vehicle sales'!F43)</f>
-        <v>3.3969969329243871E-2</v>
-      </c>
-      <c r="J15" s="33">
-        <f>($F$15*'New vehicle sales'!G43)</f>
-        <v>1.51498759414641E-2</v>
-      </c>
-      <c r="K15" s="33">
-        <f>($F$15*'New vehicle sales'!H43)</f>
-        <v>1.2930798962171324E-2</v>
-      </c>
-      <c r="L15" s="33">
-        <f>($F$15*'New vehicle sales'!I43)</f>
-        <v>6.2401330151106724E-3</v>
-      </c>
-      <c r="M15" s="33">
-        <f>($F$15*'New vehicle sales'!J43)</f>
-        <v>1.9676884581986246E-2</v>
-      </c>
-      <c r="N15" s="33">
-        <f>($F$15*'New vehicle sales'!K43)</f>
-        <v>2.9777616123094604E-2</v>
-      </c>
-      <c r="O15" s="33">
-        <f>($F$15*'New vehicle sales'!L43)</f>
-        <v>1.190240525508387E-2</v>
-      </c>
-      <c r="P15" s="33">
-        <f>($F$15*'New vehicle sales'!M43)</f>
-        <v>1.3552629064452678E-2</v>
-      </c>
-      <c r="Q15" s="33">
-        <f>($F$15*'New vehicle sales'!N43)</f>
-        <v>2.2858248606375847E-2</v>
-      </c>
-      <c r="R15" s="33">
-        <f>($F$15*'New vehicle sales'!O43)</f>
-        <v>2.1744206314122706E-2</v>
-      </c>
-      <c r="S15" s="33">
-        <f>($F$15*'New vehicle sales'!P43)</f>
-        <v>1.8139942858522856E-2</v>
-      </c>
-      <c r="T15" s="33">
-        <f>($F$15*'New vehicle sales'!Q43)</f>
-        <v>8.2880349610919196E-2</v>
-      </c>
-      <c r="U15" s="33">
-        <f>($F$15*'New vehicle sales'!R43)</f>
-        <v>2.2550615987643484E-2</v>
-      </c>
-      <c r="V15" s="33">
-        <f>($F$15*'New vehicle sales'!S43)</f>
-        <v>2.9755478788247858E-2</v>
-      </c>
-      <c r="W15" s="33">
-        <f>($F$15*'New vehicle sales'!T43)</f>
-        <v>2.4359159908985226E-2</v>
-      </c>
-      <c r="X15" s="33">
-        <f>($F$15*'New vehicle sales'!U43)</f>
-        <v>1.7736738021762469E-2</v>
-      </c>
-      <c r="Y15" s="33">
-        <f>($F$15*'New vehicle sales'!V43)</f>
-        <v>3.9398043833665984E-2</v>
-      </c>
-      <c r="Z15" s="33">
-        <f>($F$15*'New vehicle sales'!W43)</f>
-        <v>4.8921983298560508E-3</v>
-      </c>
-      <c r="AA15" s="33">
-        <f>($F$15*'New vehicle sales'!X43)</f>
-        <v>1.9924670060994996E-2</v>
-      </c>
-      <c r="AB15" s="33">
-        <f>($F$15*'New vehicle sales'!Y43)</f>
-        <v>9.8540147610232456E-3</v>
-      </c>
-      <c r="AC15" s="33">
-        <f>($F$15*'New vehicle sales'!Z43)</f>
-        <v>1.0005311994355144E-2</v>
-      </c>
-      <c r="AD15" s="33">
-        <f>($F$15*'New vehicle sales'!AA43)</f>
-        <v>1.1629887029556687E-2</v>
-      </c>
-      <c r="AE15" s="33">
-        <f>($F$15*'New vehicle sales'!AB43)</f>
-        <v>2.4304045578780561E-2</v>
-      </c>
-      <c r="AF15" s="33">
-        <f>($F$15*'New vehicle sales'!AC43)</f>
-        <v>9.3718788751886006E-3</v>
-      </c>
-      <c r="AG15" t="str">
-        <f>'New vehicle sales'!B113</f>
-        <v>T-LGT-BEV_ELC61</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34">
-      <c r="B16" s="30"/>
-      <c r="C16" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>222</v>
-      </c>
-      <c r="E16" s="30">
-        <v>2020</v>
-      </c>
-      <c r="F16" s="32">
-        <f>'New vehicle sales'!C33/1000</f>
-        <v>2.0430000000000001</v>
-      </c>
-      <c r="G16" s="31">
-        <f>($F$16*'New vehicle sales'!D43)</f>
-        <v>2.4425739914928274E-2</v>
-      </c>
-      <c r="H16" s="31">
-        <f>($F$16*'New vehicle sales'!E43)</f>
-        <v>0.57806225858985982</v>
-      </c>
-      <c r="I16" s="31">
-        <f>($F$16*'New vehicle sales'!F43)</f>
-        <v>9.5461688225096611E-2</v>
-      </c>
-      <c r="J16" s="31">
-        <f>($F$16*'New vehicle sales'!G43)</f>
-        <v>4.2573860451734745E-2</v>
-      </c>
-      <c r="K16" s="31">
-        <f>($F$16*'New vehicle sales'!H43)</f>
-        <v>3.633785733110869E-2</v>
-      </c>
-      <c r="L16" s="31">
-        <f>($F$16*'New vehicle sales'!I43)</f>
-        <v>1.7535889614678273E-2</v>
-      </c>
-      <c r="M16" s="31">
-        <f>($F$16*'New vehicle sales'!J43)</f>
-        <v>5.5295564237961357E-2</v>
-      </c>
-      <c r="N16" s="31">
-        <f>($F$16*'New vehicle sales'!K43)</f>
-        <v>8.3680426051557469E-2</v>
-      </c>
-      <c r="O16" s="31">
-        <f>($F$16*'New vehicle sales'!L43)</f>
-        <v>3.3447887119857425E-2</v>
-      </c>
-      <c r="P16" s="31">
-        <f>($F$16*'New vehicle sales'!M43)</f>
-        <v>3.808531111234776E-2</v>
-      </c>
-      <c r="Q16" s="31">
-        <f>($F$16*'New vehicle sales'!N43)</f>
-        <v>6.4235766028646293E-2</v>
-      </c>
-      <c r="R16" s="31">
-        <f>($F$16*'New vehicle sales'!O43)</f>
-        <v>6.110510797765157E-2</v>
-      </c>
-      <c r="S16" s="31">
-        <f>($F$16*'New vehicle sales'!P43)</f>
-        <v>5.097648316363438E-2</v>
-      </c>
-      <c r="T16" s="31">
-        <f>($F$16*'New vehicle sales'!Q43)</f>
-        <v>0.23290860282683346</v>
-      </c>
-      <c r="U16" s="31">
-        <f>($F$16*'New vehicle sales'!R43)</f>
-        <v>6.3371263360049016E-2</v>
-      </c>
-      <c r="V16" s="31">
-        <f>($F$16*'New vehicle sales'!S43)</f>
-        <v>8.3618216182105062E-2</v>
-      </c>
-      <c r="W16" s="31">
-        <f>($F$16*'New vehicle sales'!T43)</f>
-        <v>6.8453595177519699E-2</v>
-      </c>
-      <c r="X16" s="31">
-        <f>($F$16*'New vehicle sales'!U43)</f>
-        <v>4.984340547243566E-2</v>
-      </c>
-      <c r="Y16" s="31">
-        <f>($F$16*'New vehicle sales'!V43)</f>
-        <v>0.11071554821482753</v>
-      </c>
-      <c r="Z16" s="31">
-        <f>($F$16*'New vehicle sales'!W43)</f>
-        <v>1.3747952115400154E-2</v>
-      </c>
-      <c r="AA16" s="31">
-        <f>($F$16*'New vehicle sales'!X43)</f>
-        <v>5.5991885742245916E-2</v>
-      </c>
-      <c r="AB16" s="31">
-        <f>($F$16*'New vehicle sales'!Y43)</f>
-        <v>2.7691543544388575E-2</v>
-      </c>
-      <c r="AC16" s="31">
-        <f>($F$16*'New vehicle sales'!Z43)</f>
-        <v>2.8116715824577115E-2</v>
-      </c>
-      <c r="AD16" s="31">
-        <f>($F$16*'New vehicle sales'!AA43)</f>
-        <v>3.2682062175219143E-2</v>
-      </c>
-      <c r="AE16" s="31">
-        <f>($F$16*'New vehicle sales'!AB43)</f>
-        <v>6.8298714054262299E-2</v>
-      </c>
-      <c r="AF16" s="31">
-        <f>($F$16*'New vehicle sales'!AC43)</f>
-        <v>2.6336655491073332E-2</v>
-      </c>
-      <c r="AG16" s="30" t="str">
-        <f>'New vehicle sales'!B123</f>
-        <v>T-HGT-ICE_DST81</v>
-      </c>
-      <c r="AH16" s="30" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40162BAB-2A61-4FF8-AC40-4BD254BCBC14}">
-  <dimension ref="B4:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C4" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","Emissions","CO2","2020")</f>
-        <v>UC_Emissions_CO2_2020</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" t="s">
-        <v>481</v>
-      </c>
-      <c r="C5" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"CO2 Emissions in 2020")</f>
-        <v>CO2 Emissions in 2020</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6">
-        <v>2018</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
-        <v>482</v>
-      </c>
-      <c r="C7" s="33">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" t="s">
-        <v>225</v>
-      </c>
-      <c r="C8" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C9" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" t="s">
-        <v>475</v>
-      </c>
-      <c r="C10" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" t="s">
-        <v>227</v>
-      </c>
-      <c r="C12" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
-        <v>477</v>
-      </c>
-      <c r="C13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" t="s">
-        <v>476</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Relax TRAELC bound in 2018
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564D4CAE-9409-406C-9709-3778A167363B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E37E1E6-59E5-49B5-9E04-48DDCABA2331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="2340" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -8744,8 +8744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8837,7 +8837,7 @@
       </c>
       <c r="I7" s="19">
         <f>F17</f>
-        <v>0.30000000000000004</v>
+        <v>0.38300000000000006</v>
       </c>
       <c r="J7" t="s">
         <v>511</v>
@@ -8934,9 +8934,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F17" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$45),1)</f>
-        <v>0.30000000000000004</v>
+      <c r="F17" s="378">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$45),1)+0.083</f>
+        <v>0.38300000000000006</v>
       </c>
       <c r="G17" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$45),1)</f>
@@ -8956,6 +8956,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -42442,8 +42443,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Constrain diesel, gasoline, biodiesel, ethanol and jet kerosene consumption in TRA in 2018-2021 to EB
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E37E1E6-59E5-49B5-9E04-48DDCABA2331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504BEDB8-0A2E-4E5D-B1A5-F66876C17973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2340" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="526">
   <si>
     <t>Development</t>
   </si>
@@ -1779,10 +1779,52 @@
     <t>TRAELC</t>
   </si>
   <si>
-    <t>UC_Historic_TRAELC-cons_Multi</t>
-  </si>
-  <si>
     <t>Historic electricity consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>FT-TRABDL</t>
+  </si>
+  <si>
+    <t>FT-TRADST</t>
+  </si>
+  <si>
+    <t>FT-TRAETH</t>
+  </si>
+  <si>
+    <t>FT-TRAGSL</t>
+  </si>
+  <si>
+    <t>FT-TRAKER</t>
+  </si>
+  <si>
+    <t>TRABDL</t>
+  </si>
+  <si>
+    <t>TRADST</t>
+  </si>
+  <si>
+    <t>TRAETH</t>
+  </si>
+  <si>
+    <t>TRAGSL</t>
+  </si>
+  <si>
+    <t>TRAKER</t>
+  </si>
+  <si>
+    <t>Historic jet kerosene consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>Historic gasoline consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>Historic ethanol consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>Historic biodiesel consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>Historic diesel consumption in TRA - Multi</t>
   </si>
 </sst>
 </file>
@@ -4146,7 +4188,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="390">
+  <cellXfs count="391">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5211,6 +5253,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8742,16 +8785,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -8820,11 +8863,12 @@
       <c r="J6" s="30"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" t="s">
-        <v>510</v>
+      <c r="B7" t="str">
+        <f>"UC_Historic_"&amp;C7&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRABDL-cons_Multi</v>
       </c>
       <c r="C7" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="F7">
         <v>2018</v>
@@ -8836,11 +8880,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="19">
-        <f>F17</f>
-        <v>0.38300000000000006</v>
+        <f>F43</f>
+        <v>5.3999999999999995</v>
       </c>
       <c r="J7" t="s">
-        <v>511</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -8851,8 +8895,8 @@
         <v>501</v>
       </c>
       <c r="I8" s="19">
-        <f>G17</f>
-        <v>0.30000000000000004</v>
+        <f>G43</f>
+        <v>6.8</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -8863,8 +8907,8 @@
         <v>501</v>
       </c>
       <c r="I9" s="19">
-        <f>H17</f>
-        <v>0.30000000000000004</v>
+        <f>H43</f>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="2:10">
@@ -8875,8 +8919,8 @@
         <v>501</v>
       </c>
       <c r="I10" s="19">
-        <f>I17</f>
-        <v>0.5</v>
+        <f>I43</f>
+        <v>6.6999999999999993</v>
       </c>
     </row>
     <row r="11" spans="2:10">
@@ -8888,69 +8932,574 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="str">
+        <f>"UC_Historic_"&amp;C12&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRADST-cons_Multi</v>
+      </c>
+      <c r="C12" t="s">
+        <v>517</v>
+      </c>
+      <c r="F12">
+        <v>2018</v>
+      </c>
+      <c r="G12" t="s">
+        <v>501</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="19">
+        <f>F44</f>
+        <v>129.19999999999999</v>
+      </c>
+      <c r="J12" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="F13">
+        <v>2019</v>
+      </c>
+      <c r="G13" t="s">
+        <v>501</v>
+      </c>
+      <c r="I13" s="19">
+        <f>G44</f>
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="F14">
+        <v>2020</v>
+      </c>
+      <c r="G14" t="s">
+        <v>501</v>
+      </c>
+      <c r="I14" s="19">
+        <f>H44</f>
+        <v>113.19999999999999</v>
+      </c>
+    </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="28" t="s">
+      <c r="F15">
+        <v>2021</v>
+      </c>
+      <c r="G15" t="s">
+        <v>501</v>
+      </c>
+      <c r="I15" s="19">
+        <f>I44</f>
+        <v>121.1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F16,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" t="str">
+        <f>"UC_Historic_"&amp;C17&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRAELC-cons_Multi</v>
+      </c>
+      <c r="C17" t="s">
+        <v>509</v>
+      </c>
+      <c r="F17">
+        <v>2018</v>
+      </c>
+      <c r="G17" t="s">
+        <v>501</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="19">
+        <f>F45</f>
+        <v>0.38300000000000006</v>
+      </c>
+      <c r="J17" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="F18">
+        <v>2019</v>
+      </c>
+      <c r="G18" t="s">
+        <v>501</v>
+      </c>
+      <c r="I18" s="19">
+        <f>G45</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="F19">
+        <v>2020</v>
+      </c>
+      <c r="G19" t="s">
+        <v>501</v>
+      </c>
+      <c r="I19" s="19">
+        <f>H45</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="F20">
+        <v>2021</v>
+      </c>
+      <c r="G20" t="s">
+        <v>501</v>
+      </c>
+      <c r="I20" s="19">
+        <f>I45</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F21,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" t="str">
+        <f>"UC_Historic_"&amp;C22&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRAETH-cons_Multi</v>
+      </c>
+      <c r="C22" t="s">
+        <v>518</v>
+      </c>
+      <c r="F22">
+        <v>2018</v>
+      </c>
+      <c r="G22" t="s">
+        <v>501</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="19">
+        <f>F46</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J22" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="F23">
+        <v>2019</v>
+      </c>
+      <c r="G23" t="s">
+        <v>501</v>
+      </c>
+      <c r="I23" s="19">
+        <f>G46</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="F24">
+        <v>2020</v>
+      </c>
+      <c r="G24" t="s">
+        <v>501</v>
+      </c>
+      <c r="I24" s="19">
+        <f>H46</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="F25">
+        <v>2021</v>
+      </c>
+      <c r="G25" t="s">
+        <v>501</v>
+      </c>
+      <c r="I25" s="19">
+        <f>I46</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F26,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" t="str">
+        <f>"UC_Historic_"&amp;C27&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRAGSL-cons_Multi</v>
+      </c>
+      <c r="C27" t="s">
+        <v>519</v>
+      </c>
+      <c r="F27">
+        <v>2018</v>
+      </c>
+      <c r="G27" t="s">
+        <v>501</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19">
+        <f>F47</f>
+        <v>34.6</v>
+      </c>
+      <c r="J27" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="F28">
+        <v>2019</v>
+      </c>
+      <c r="G28" t="s">
+        <v>501</v>
+      </c>
+      <c r="I28" s="19">
+        <f>G47</f>
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="F29">
+        <v>2020</v>
+      </c>
+      <c r="G29" t="s">
+        <v>501</v>
+      </c>
+      <c r="I29" s="19">
+        <f>H47</f>
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="F30">
+        <v>2021</v>
+      </c>
+      <c r="G30" t="s">
+        <v>501</v>
+      </c>
+      <c r="I30" s="19">
+        <f>I47</f>
+        <v>25.700000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F31,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" t="str">
+        <f>"UC_Historic_"&amp;C32&amp;"-cons_Multi"</f>
+        <v>UC_Historic_TRAKER-cons_Multi</v>
+      </c>
+      <c r="C32" t="s">
+        <v>520</v>
+      </c>
+      <c r="F32">
+        <v>2018</v>
+      </c>
+      <c r="G32" t="s">
+        <v>501</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" s="19">
+        <f>F48</f>
+        <v>46.2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="F33">
+        <v>2019</v>
+      </c>
+      <c r="G33" t="s">
+        <v>501</v>
+      </c>
+      <c r="I33" s="19">
+        <f>G48</f>
+        <v>46.800000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="F34">
+        <v>2020</v>
+      </c>
+      <c r="G34" t="s">
+        <v>501</v>
+      </c>
+      <c r="I34" s="19">
+        <f>H48</f>
+        <v>16.700000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="F35">
+        <v>2021</v>
+      </c>
+      <c r="G35" t="s">
+        <v>501</v>
+      </c>
+      <c r="I35" s="19">
+        <f>I48</f>
+        <v>18.700000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F36,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B16" s="29" t="s">
+      <c r="D41" s="18"/>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B42" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C42" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D42" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E42" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F42" s="29">
         <v>2018</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G42" s="29">
         <v>2019</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H42" s="29">
         <v>2020</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I42" s="29">
         <v>2021</v>
       </c>
-      <c r="J16" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" t="s">
-        <v>507</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="J42" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="C43" t="s">
+        <v>511</v>
+      </c>
+      <c r="D43" t="s">
         <v>200</v>
       </c>
-      <c r="E17" s="19" t="str">
+      <c r="E43" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F17" s="378">
+      <c r="F43" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$45),1)</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="G43" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$45),1)</f>
+        <v>6.8</v>
+      </c>
+      <c r="H43" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$45),1)</f>
+        <v>6.5</v>
+      </c>
+      <c r="I43" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$45),1)</f>
+        <v>6.6999999999999993</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="C44" t="s">
+        <v>512</v>
+      </c>
+      <c r="D44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F44" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$U$45),1)</f>
+        <v>129.19999999999999</v>
+      </c>
+      <c r="G44" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$U$45),1)</f>
+        <v>130.9</v>
+      </c>
+      <c r="H44" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$U$45),1)</f>
+        <v>113.19999999999999</v>
+      </c>
+      <c r="I44" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$U$45),1)</f>
+        <v>121.1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="C45" t="s">
+        <v>507</v>
+      </c>
+      <c r="D45" t="s">
+        <v>200</v>
+      </c>
+      <c r="E45" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F45" s="378">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$45),1)+0.083</f>
         <v>0.38300000000000006</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G45" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$45),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H45" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$45),1)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I45" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$45),1)</f>
         <v>0.5</v>
       </c>
-      <c r="J17">
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="C46" t="s">
+        <v>513</v>
+      </c>
+      <c r="D46" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F46" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$45),1)</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="G46" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$45),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H46" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$45),1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="I46" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$45),1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="C47" t="s">
+        <v>514</v>
+      </c>
+      <c r="D47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F47" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$P$45),1)</f>
+        <v>34.6</v>
+      </c>
+      <c r="G47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$P$45),1)</f>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="H47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$P$45),1)</f>
+        <v>22.6</v>
+      </c>
+      <c r="I47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$P$45),1)</f>
+        <v>25.700000000000003</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="C48" t="s">
+        <v>515</v>
+      </c>
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
+        <v>IE</v>
+      </c>
+      <c r="F48" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$R$45),1)</f>
+        <v>46.2</v>
+      </c>
+      <c r="G48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$R$45),1)</f>
+        <v>46.800000000000004</v>
+      </c>
+      <c r="H48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$R$45),1)</f>
+        <v>16.700000000000003</v>
+      </c>
+      <c r="I48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$R$45),1)</f>
+        <v>18.700000000000003</v>
+      </c>
+      <c r="J48">
         <v>1</v>
       </c>
     </row>
@@ -12084,11 +12633,11 @@
   <dimension ref="A1:AS80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O42" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="AO30" sqref="AO30"/>
+      <selection pane="bottomRight" activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -19368,11 +19917,11 @@
   <dimension ref="A1:AR80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AJ80" sqref="AJ80"/>
       <selection pane="topRight" activeCell="AJ80" sqref="AJ80"/>
       <selection pane="bottomLeft" activeCell="AJ80" sqref="AJ80"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -26631,11 +27180,11 @@
   <dimension ref="A1:AQ85"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AB23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="AK33" sqref="AK33"/>
+      <selection pane="bottomRight" activeCell="AQ45" sqref="AQ45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43721,7 +44270,7 @@
   <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Remove relaxation of SRVELC consumption in 2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504BEDB8-0A2E-4E5D-B1A5-F66876C17973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ABEEF5-EAF8-41B6-B0BF-D062836334A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -149,24 +149,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={EA2214DE-E5ED-4BA3-B779-4C671AA758DE}</author>
-  </authors>
-  <commentList>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{EA2214DE-E5ED-4BA3-B779-4C671AA758DE}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Relax this bound to avoid dummies</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
@@ -5229,7 +5211,6 @@
     <xf numFmtId="167" fontId="5" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -5241,6 +5222,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5253,7 +5235,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5654,9 +5636,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Balyk, Olexandr" id="{0EBAA6E2-D3EC-429B-B80A-AFBE5C02E277}" userId="Balyk, Olexandr" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5920,14 +5900,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I8" dT="2022-09-16T03:05:16.52" personId="{0EBAA6E2-D3EC-429B-B80A-AFBE5C02E277}" id="{EA2214DE-E5ED-4BA3-B779-4C671AA758DE}">
-    <text>Relax this bound to avoid dummies</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B28889-4A29-4B8D-BD3E-384099A070C4}">
   <sheetPr codeName="Sheet13"/>
@@ -8787,8 +8759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8802,13 +8774,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="379" t="str">
+      <c r="B2" s="378" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_S: IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="379" t="s">
+      <c r="B3" s="378" t="s">
         <v>459</v>
       </c>
     </row>
@@ -8819,31 +8791,31 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="380" t="s">
+      <c r="B5" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="381" t="s">
+      <c r="C5" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="381" t="s">
+      <c r="D5" s="380" t="s">
         <v>475</v>
       </c>
-      <c r="E5" s="381" t="s">
+      <c r="E5" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="381" t="s">
+      <c r="F5" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="381" t="s">
+      <c r="G5" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H5" s="382" t="s">
+      <c r="H5" s="381" t="s">
         <v>499</v>
       </c>
-      <c r="I5" s="383" t="s">
+      <c r="I5" s="382" t="s">
         <v>480</v>
       </c>
-      <c r="J5" s="380" t="s">
+      <c r="J5" s="379" t="s">
         <v>463</v>
       </c>
     </row>
@@ -9328,7 +9300,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F43" s="390">
+      <c r="F43" s="385">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$45),1)</f>
         <v>5.3999999999999995</v>
       </c>
@@ -9359,7 +9331,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F44" s="390">
+      <c r="F44" s="385">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$U$45),1)</f>
         <v>129.19999999999999</v>
       </c>
@@ -9390,7 +9362,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F45" s="378">
+      <c r="F45" s="377">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$45),1)+0.083</f>
         <v>0.38300000000000006</v>
       </c>
@@ -9421,7 +9393,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F46" s="390">
+      <c r="F46" s="385">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$45),1)</f>
         <v>1.2000000000000002</v>
       </c>
@@ -9452,7 +9424,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F47" s="390">
+      <c r="F47" s="385">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$P$45),1)</f>
         <v>34.6</v>
       </c>
@@ -9483,7 +9455,7 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
       </c>
-      <c r="F48" s="390">
+      <c r="F48" s="385">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$R$45),1)</f>
         <v>46.2</v>
       </c>
@@ -11089,13 +11061,13 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="379" t="str">
+      <c r="B2" s="378" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="379" t="s">
+      <c r="B3" s="378" t="s">
         <v>459</v>
       </c>
     </row>
@@ -11106,34 +11078,34 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="380" t="s">
+      <c r="B5" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="381" t="s">
+      <c r="C5" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="381" t="s">
+      <c r="D5" s="380" t="s">
         <v>475</v>
       </c>
-      <c r="E5" s="381" t="s">
+      <c r="E5" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="381" t="s">
+      <c r="F5" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="381" t="s">
+      <c r="G5" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H5" s="382" t="s">
+      <c r="H5" s="381" t="s">
         <v>476</v>
       </c>
-      <c r="I5" s="382" t="s">
+      <c r="I5" s="381" t="s">
         <v>477</v>
       </c>
-      <c r="J5" s="383" t="s">
+      <c r="J5" s="382" t="s">
         <v>462</v>
       </c>
-      <c r="K5" s="380" t="s">
+      <c r="K5" s="379" t="s">
         <v>463</v>
       </c>
     </row>
@@ -11151,7 +11123,7 @@
       <c r="J6" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="K6" s="384"/>
+      <c r="K6" s="383"/>
     </row>
     <row r="7" spans="1:11">
       <c r="B7" t="str">
@@ -11251,13 +11223,13 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="379" t="str">
+      <c r="B2" s="378" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="379" t="s">
+      <c r="B3" s="378" t="s">
         <v>459</v>
       </c>
     </row>
@@ -11268,34 +11240,34 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="380" t="s">
+      <c r="B5" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="381" t="s">
+      <c r="C5" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="381" t="s">
+      <c r="D5" s="380" t="s">
         <v>475</v>
       </c>
-      <c r="E5" s="381" t="s">
+      <c r="E5" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="381" t="s">
+      <c r="F5" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="381" t="s">
+      <c r="G5" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H5" s="382" t="s">
+      <c r="H5" s="381" t="s">
         <v>476</v>
       </c>
-      <c r="I5" s="382" t="s">
+      <c r="I5" s="381" t="s">
         <v>477</v>
       </c>
-      <c r="J5" s="383" t="s">
+      <c r="J5" s="382" t="s">
         <v>480</v>
       </c>
-      <c r="K5" s="380" t="s">
+      <c r="K5" s="379" t="s">
         <v>463</v>
       </c>
     </row>
@@ -19917,11 +19889,11 @@
   <dimension ref="A1:AR80"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G37" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AJ80" sqref="AJ80"/>
       <selection pane="topRight" activeCell="AJ80" sqref="AJ80"/>
       <selection pane="bottomLeft" activeCell="AJ80" sqref="AJ80"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42649,13 +42621,13 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="379" t="str">
+      <c r="B2" s="378" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="379" t="s">
+      <c r="B3" s="378" t="s">
         <v>459</v>
       </c>
     </row>
@@ -42666,34 +42638,34 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="380" t="s">
+      <c r="B5" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="381" t="s">
+      <c r="C5" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="381" t="s">
+      <c r="D5" s="380" t="s">
         <v>492</v>
       </c>
-      <c r="E5" s="381" t="s">
+      <c r="E5" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="381" t="s">
+      <c r="F5" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G5" s="381" t="s">
+      <c r="G5" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H5" s="381" t="s">
+      <c r="H5" s="380" t="s">
         <v>486</v>
       </c>
-      <c r="I5" s="382" t="s">
+      <c r="I5" s="381" t="s">
         <v>488</v>
       </c>
-      <c r="J5" s="383" t="s">
+      <c r="J5" s="382" t="s">
         <v>462</v>
       </c>
-      <c r="K5" s="380" t="s">
+      <c r="K5" s="379" t="s">
         <v>463</v>
       </c>
     </row>
@@ -42711,7 +42683,7 @@
       <c r="J6" s="30" t="s">
         <v>489</v>
       </c>
-      <c r="K6" s="384"/>
+      <c r="K6" s="383"/>
     </row>
     <row r="7" spans="1:11">
       <c r="B7" t="s">
@@ -42738,7 +42710,7 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="385">
+      <c r="J7" s="384">
         <f>Conversions!$B$2*'EB2018'!$AO$3</f>
         <v>5.8385184241824009</v>
       </c>
@@ -42753,7 +42725,7 @@
       <c r="G8" t="s">
         <v>223</v>
       </c>
-      <c r="J8" s="385">
+      <c r="J8" s="384">
         <f>Conversions!$B$2*'EB2019'!$AO$3</f>
         <v>7.8478965511531191</v>
       </c>
@@ -42765,7 +42737,7 @@
       <c r="G9" t="s">
         <v>223</v>
       </c>
-      <c r="J9" s="385">
+      <c r="J9" s="384">
         <f>Conversions!$B$2*'EB2020'!$AO$3</f>
         <v>6.3411436804464003</v>
       </c>
@@ -42777,7 +42749,7 @@
       <c r="G10" t="s">
         <v>223</v>
       </c>
-      <c r="J10" s="385">
+      <c r="J10" s="384">
         <f>Conversions!$B$2*'EB2021'!$AO$3</f>
         <v>8.8241634675727223</v>
       </c>
@@ -42818,7 +42790,7 @@
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="385">
+      <c r="J12" s="384">
         <f>Conversions!$B$2*'EB2018'!$AO$4</f>
         <v>5.9383641411770398</v>
       </c>
@@ -42833,7 +42805,7 @@
       <c r="G13" t="s">
         <v>223</v>
       </c>
-      <c r="J13" s="385">
+      <c r="J13" s="384">
         <f>Conversions!$B$2*'EB2019'!$AO$4</f>
         <v>5.5271334489739186</v>
       </c>
@@ -42845,7 +42817,7 @@
       <c r="G14" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="385">
+      <c r="J14" s="384">
         <f>Conversions!$B$2*'EB2020'!$AO$4</f>
         <v>6.8879157977152801</v>
       </c>
@@ -42857,7 +42829,7 @@
       <c r="G15" t="s">
         <v>223</v>
       </c>
-      <c r="J15" s="385">
+      <c r="J15" s="384">
         <f>Conversions!$B$2*'EB2021'!$AO$4</f>
         <v>3.1077995112374399</v>
       </c>
@@ -42879,34 +42851,34 @@
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="380" t="s">
+      <c r="B20" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C20" s="381" t="s">
+      <c r="C20" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D20" s="381" t="s">
+      <c r="D20" s="380" t="s">
         <v>492</v>
       </c>
-      <c r="E20" s="381" t="s">
+      <c r="E20" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F20" s="381" t="s">
+      <c r="F20" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G20" s="381" t="s">
+      <c r="G20" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H20" s="381" t="s">
+      <c r="H20" s="380" t="s">
         <v>486</v>
       </c>
       <c r="I20" t="s">
         <v>499</v>
       </c>
-      <c r="J20" s="383" t="s">
+      <c r="J20" s="382" t="s">
         <v>462</v>
       </c>
-      <c r="K20" s="380" t="s">
+      <c r="K20" s="379" t="s">
         <v>463</v>
       </c>
     </row>
@@ -43132,7 +43104,7 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$10,'EB2021'!$C$11),1)</f>
         <v>28.200000000000003</v>
       </c>
-      <c r="J6" s="378">
+      <c r="J6" s="377">
         <v>30</v>
       </c>
       <c r="K6">
@@ -43486,26 +43458,26 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="376" t="s">
+      <c r="B8" s="375" t="s">
         <v>466</v>
       </c>
-      <c r="C8" s="376" t="s">
+      <c r="C8" s="375" t="s">
         <v>467</v>
       </c>
-      <c r="D8" s="376">
+      <c r="D8" s="375">
         <v>2019</v>
       </c>
-      <c r="E8" s="376" t="s">
+      <c r="E8" s="375" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="376">
+      <c r="F8" s="375">
         <v>1</v>
       </c>
-      <c r="G8" s="377">
+      <c r="G8" s="376">
         <f>4.015-0.025</f>
         <v>3.9899999999999998</v>
       </c>
-      <c r="H8" s="376" t="s">
+      <c r="H8" s="375" t="s">
         <v>471</v>
       </c>
     </row>
@@ -43524,7 +43496,7 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="375">
+      <c r="G9" s="374">
         <f>4.3-0.025</f>
         <v>4.2749999999999995</v>
       </c>
@@ -43544,7 +43516,7 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="375">
+      <c r="G10" s="374">
         <v>4.5</v>
       </c>
     </row>
@@ -43563,7 +43535,7 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="375">
+      <c r="G11" s="374">
         <v>4.7</v>
       </c>
     </row>
@@ -43584,25 +43556,25 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="376" t="s">
+      <c r="B13" s="375" t="s">
         <v>469</v>
       </c>
-      <c r="C13" s="376" t="s">
+      <c r="C13" s="375" t="s">
         <v>472</v>
       </c>
-      <c r="D13" s="376">
+      <c r="D13" s="375">
         <v>2019</v>
       </c>
-      <c r="E13" s="376" t="s">
+      <c r="E13" s="375" t="s">
         <v>223</v>
       </c>
-      <c r="F13" s="376">
+      <c r="F13" s="375">
         <v>1</v>
       </c>
-      <c r="G13" s="377">
+      <c r="G13" s="376">
         <v>0.02</v>
       </c>
-      <c r="H13" s="376" t="s">
+      <c r="H13" s="375" t="s">
         <v>470</v>
       </c>
     </row>
@@ -43621,7 +43593,7 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" s="375">
+      <c r="G14" s="374">
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
@@ -43640,7 +43612,7 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="375">
+      <c r="G15" s="374">
         <v>0.26100000000000001</v>
       </c>
     </row>
@@ -43659,7 +43631,7 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" s="375">
+      <c r="G16" s="374">
         <v>0.38400000000000001</v>
       </c>
     </row>
@@ -43776,7 +43748,7 @@
   <dimension ref="B2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43863,7 +43835,7 @@
   <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44265,12 +44237,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44463,9 +44435,9 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$57),1)</f>
         <v>47.1</v>
       </c>
-      <c r="I8" s="374">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)+0.8</f>
-        <v>50.699999999999996</v>
+      <c r="I8" s="390">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)</f>
+        <v>49.9</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -44659,6 +44631,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Constraint ambient heat in SRV according to EB in 2018-2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ABEEF5-EAF8-41B6-B0BF-D062836334A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BE76F-3949-44F0-8589-E37A0CA4D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="527">
   <si>
     <t>Development</t>
   </si>
@@ -1807,6 +1807,9 @@
   </si>
   <si>
     <t>Historic diesel consumption in TRA - Multi</t>
+  </si>
+  <si>
+    <t>FT-SRVAHT</t>
   </si>
 </sst>
 </file>
@@ -4170,7 +4173,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="391">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5235,7 +5238,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5635,10 +5637,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12609,7 +12607,7 @@
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="R45" sqref="R45"/>
+      <selection pane="bottomRight" activeCell="AS53" sqref="AS53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -44239,10 +44237,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:J14"/>
+  <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44290,7 +44288,7 @@
     </row>
     <row r="4" spans="2:10">
       <c r="C4" t="s">
-        <v>216</v>
+        <v>526</v>
       </c>
       <c r="D4" t="s">
         <v>200</v>
@@ -44300,20 +44298,20 @@
         <v>IE,National</v>
       </c>
       <c r="F4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AM$57),1)</f>
+        <v>0.7</v>
       </c>
       <c r="G4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AM$57),1)</f>
+        <v>0.7</v>
       </c>
       <c r="H4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AM$57),1)</f>
+        <v>0.7</v>
       </c>
       <c r="I4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AM$57),1)</f>
+        <v>0.7</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -44321,7 +44319,7 @@
     </row>
     <row r="5" spans="2:10">
       <c r="C5" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D5" t="s">
         <v>200</v>
@@ -44331,20 +44329,20 @@
         <v>IE,National</v>
       </c>
       <c r="F5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AH$57),1)</f>
-        <v>0.30000000000000004</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$57),1)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AH$57),1)</f>
-        <v>0.30000000000000004</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$57),1)</f>
+        <v>0</v>
       </c>
       <c r="H5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AH$57),1)</f>
-        <v>0.30000000000000004</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$57),1)</f>
+        <v>0</v>
       </c>
       <c r="I5" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AH$57),1)</f>
-        <v>0.30000000000000004</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$57),1)</f>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -44352,7 +44350,7 @@
     </row>
     <row r="6" spans="2:10">
       <c r="C6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
         <v>200</v>
@@ -44362,20 +44360,20 @@
         <v>IE,National</v>
       </c>
       <c r="F6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$57),1)</f>
-        <v>0.79999999999999993</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AH$57),1)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="G6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$57),1)</f>
-        <v>0.6</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AH$57),1)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$57),1)</f>
-        <v>0.7</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AH$57),1)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I6" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$57),1)</f>
-        <v>0.79999999999999993</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AH$57),1)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -44383,7 +44381,7 @@
     </row>
     <row r="7" spans="2:10">
       <c r="C7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
         <v>200</v>
@@ -44393,20 +44391,20 @@
         <v>IE,National</v>
       </c>
       <c r="F7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$57),1)</f>
-        <v>0.1</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$57),1)</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="G7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$57),1)</f>
-        <v>0.1</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$57),1)</f>
+        <v>0.6</v>
       </c>
       <c r="H7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$57),1)</f>
-        <v>0.1</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$57),1)</f>
+        <v>0.7</v>
       </c>
       <c r="I7" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$57),1)</f>
-        <v>0.1</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$57),1)</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -44414,7 +44412,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="C8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D8" t="s">
         <v>200</v>
@@ -44424,20 +44422,20 @@
         <v>IE,National</v>
       </c>
       <c r="F8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$57),1)</f>
-        <v>45.2</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$57),1)</f>
+        <v>0.1</v>
       </c>
       <c r="G8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$57),1)</f>
-        <v>46.9</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$57),1)</f>
+        <v>0.1</v>
       </c>
       <c r="H8" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$57),1)</f>
-        <v>47.1</v>
-      </c>
-      <c r="I8" s="390">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)</f>
-        <v>49.9</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$57),1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$57),1)</f>
+        <v>0.1</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -44445,7 +44443,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="C9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
         <v>200</v>
@@ -44455,20 +44453,20 @@
         <v>IE,National</v>
       </c>
       <c r="F9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$57),1)</f>
+        <v>45.2</v>
       </c>
       <c r="G9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$57),1)</f>
+        <v>46.9</v>
       </c>
       <c r="H9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$57),1)</f>
+        <v>47.1</v>
       </c>
       <c r="I9" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$57),1)</f>
+        <v>49.9</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -44476,7 +44474,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="C10" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D10" t="s">
         <v>200</v>
@@ -44486,20 +44484,20 @@
         <v>IE,National</v>
       </c>
       <c r="F10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$57),1)</f>
-        <v>13.799999999999999</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$57),1)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$57),1)</f>
-        <v>14.2</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$57),1)</f>
+        <v>0</v>
       </c>
       <c r="H10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$57),1)</f>
-        <v>14.7</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$57),1)</f>
+        <v>0</v>
       </c>
       <c r="I10" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$57),1)</f>
-        <v>14.1</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$57),1)</f>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -44507,7 +44505,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="C11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
         <v>200</v>
@@ -44517,20 +44515,20 @@
         <v>IE,National</v>
       </c>
       <c r="F11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$57),1)</f>
+        <v>13.799999999999999</v>
       </c>
       <c r="G11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$57),1)</f>
+        <v>14.2</v>
       </c>
       <c r="H11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$57),1)</f>
+        <v>14.7</v>
       </c>
       <c r="I11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$57),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$57),1)</f>
+        <v>14.1</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -44538,7 +44536,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="C12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D12" t="s">
         <v>200</v>
@@ -44548,20 +44546,20 @@
         <v>IE,National</v>
       </c>
       <c r="F12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$57),1)</f>
-        <v>3</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$57),1)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$57),1)</f>
-        <v>3</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$57),1)</f>
+        <v>0</v>
       </c>
       <c r="H12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$57),1)</f>
-        <v>2.8000000000000003</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$57),1)</f>
+        <v>0</v>
       </c>
       <c r="I12" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$57),1)</f>
-        <v>3</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$57),1)</f>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -44569,7 +44567,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="C13" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D13" t="s">
         <v>200</v>
@@ -44579,20 +44577,20 @@
         <v>IE,National</v>
       </c>
       <c r="F13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$57,'EB2018'!$S$57,'EB2018'!$U$57),1)</f>
-        <v>7.1999999999999993</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$57),1)</f>
+        <v>3</v>
       </c>
       <c r="G13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$57,'EB2019'!$S$57,'EB2019'!$U$57),1)</f>
-        <v>6.3999999999999995</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$57),1)</f>
+        <v>3</v>
       </c>
       <c r="H13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$57,'EB2020'!$S$57,'EB2020'!$U$57),1)</f>
-        <v>6.8999999999999995</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$57),1)</f>
+        <v>2.8000000000000003</v>
       </c>
       <c r="I13" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$57,'EB2021'!$S$57,'EB2021'!$U$57),1)</f>
-        <v>6.5</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$57),1)</f>
+        <v>3</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -44600,7 +44598,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="C14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D14" t="s">
         <v>200</v>
@@ -44610,22 +44608,53 @@
         <v>IE,National</v>
       </c>
       <c r="F14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$57,'EB2018'!$S$57,'EB2018'!$U$57),1)</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="G14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$57,'EB2019'!$S$57,'EB2019'!$U$57),1)</f>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="H14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$57,'EB2020'!$S$57,'EB2020'!$U$57),1)</f>
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="I14" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$57,'EB2021'!$S$57,'EB2021'!$U$57),1)</f>
+        <v>6.5</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="C15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F15" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G15" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H15" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I15" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$57),1)</f>
         <v>0.1</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove 2021 EB restriction on NG consumption in SRV; add max growth rate for NG in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BE76F-3949-44F0-8589-E37A0CA4D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6041E7-05BA-49C0-873D-42226F6A0BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -4173,7 +4173,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="390">
+  <cellXfs count="391">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5226,6 +5226,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -6341,12 +6342,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="387" t="s">
+      <c r="A16" s="388" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="387"/>
-      <c r="C16" s="387"/>
-      <c r="D16" s="387"/>
+      <c r="B16" s="388"/>
+      <c r="C16" s="388"/>
+      <c r="D16" s="388"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6430,11 +6431,11 @@
       <c r="A19" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="386" t="s">
+      <c r="B19" s="387" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="386"/>
-      <c r="D19" s="386"/>
+      <c r="C19" s="387"/>
+      <c r="D19" s="387"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6462,11 +6463,11 @@
       <c r="A20" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="386" t="s">
+      <c r="B20" s="387" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="386"/>
-      <c r="D20" s="386"/>
+      <c r="C20" s="387"/>
+      <c r="D20" s="387"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6554,11 +6555,11 @@
       <c r="A23" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="386" t="s">
+      <c r="B23" s="387" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="386"/>
-      <c r="D23" s="386"/>
+      <c r="C23" s="387"/>
+      <c r="D23" s="387"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6584,11 +6585,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="386" t="s">
+      <c r="B24" s="387" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="386"/>
-      <c r="D24" s="386"/>
+      <c r="C24" s="387"/>
+      <c r="D24" s="387"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6646,11 +6647,11 @@
       <c r="A26" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="386" t="s">
+      <c r="B26" s="387" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="386"/>
-      <c r="D26" s="386"/>
+      <c r="C26" s="387"/>
+      <c r="D26" s="387"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6766,11 +6767,11 @@
       <c r="A30" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="388" t="s">
+      <c r="B30" s="389" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="386"/>
-      <c r="D30" s="386"/>
+      <c r="C30" s="387"/>
+      <c r="D30" s="387"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6798,11 +6799,11 @@
       <c r="A31" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="386" t="s">
+      <c r="B31" s="387" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="386"/>
-      <c r="D31" s="386"/>
+      <c r="C31" s="387"/>
+      <c r="D31" s="387"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -8757,8 +8758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9201,7 +9202,7 @@
       </c>
       <c r="I32" s="19">
         <f>F48</f>
-        <v>46.2</v>
+        <v>46.202000000000005</v>
       </c>
       <c r="J32" t="s">
         <v>521</v>
@@ -9454,8 +9455,8 @@
         <v>IE</v>
       </c>
       <c r="F48" s="385">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$R$45),1)</f>
-        <v>46.2</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$R$45),1)+0.002</f>
+        <v>46.202000000000005</v>
       </c>
       <c r="G48" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$R$45),1)</f>
@@ -11962,10 +11963,10 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="389" t="s">
+      <c r="B49" s="390" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="389"/>
+      <c r="C49" s="390"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
@@ -34472,11 +34473,11 @@
   <dimension ref="A1:AQ85"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M44" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="topRight" activeCell="C109" sqref="C109:AQ109"/>
       <selection pane="bottomLeft" activeCell="C109" sqref="C109:AQ109"/>
-      <selection pane="bottomRight" activeCell="AP45" sqref="AP45"/>
+      <selection pane="bottomRight" activeCell="AA65" sqref="AA65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44237,10 +44238,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6681CC-1473-4A80-91C2-43AA95BF8806}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:J15"/>
+  <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44526,10 +44527,7 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$57),1)</f>
         <v>14.7</v>
       </c>
-      <c r="I11" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$57),1)</f>
-        <v>14.1</v>
-      </c>
+      <c r="I11" s="386"/>
       <c r="J11">
         <v>1</v>
       </c>
@@ -44657,6 +44655,12 @@
       <c r="J15">
         <v>1</v>
       </c>
+    </row>
+    <row r="17" spans="6:9">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sync issue with RSDHET
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6041E7-05BA-49C0-873D-42226F6A0BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1623D-8E93-457C-A0DE-500CEE9AD892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -141,7 +141,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -195,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="527">
   <si>
     <t>Development</t>
   </si>
@@ -8758,7 +8757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
@@ -44240,8 +44239,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44533,6 +44532,9 @@
       </c>
     </row>
     <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>456</v>
+      </c>
       <c r="C12" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Add estimated bounds (FX) for electricity import/export in 2022
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6041E7-05BA-49C0-873D-42226F6A0BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C5F1B-D1B7-4957-A785-1E73AC2F37FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="527">
   <si>
     <t>Development</t>
   </si>
@@ -4173,7 +4173,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="391">
+  <cellXfs count="392">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5239,6 +5239,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="40" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8758,7 +8759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
@@ -42594,10 +42595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89305455-607F-41AA-8109-096F19F6FE72}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42755,206 +42756,228 @@
     </row>
     <row r="11" spans="1:11">
       <c r="F11">
-        <v>0</v>
+        <v>2022</v>
       </c>
       <c r="G11" t="s">
         <v>223</v>
       </c>
-      <c r="J11">
-        <v>1</v>
+      <c r="J11" s="391">
+        <v>5.8</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="B12" t="s">
-        <v>504</v>
-      </c>
-      <c r="C12" t="s">
-        <v>493</v>
-      </c>
-      <c r="D12" t="s">
-        <v>494</v>
-      </c>
-      <c r="E12" t="s">
-        <v>496</v>
-      </c>
       <c r="F12">
-        <v>2018</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
         <v>223</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C13" t="s">
+        <v>493</v>
+      </c>
+      <c r="D13" t="s">
+        <v>494</v>
+      </c>
+      <c r="E13" t="s">
+        <v>496</v>
+      </c>
+      <c r="F13">
+        <v>2018</v>
+      </c>
+      <c r="G13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" t="s">
         <v>498</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>1</v>
       </c>
-      <c r="J12" s="384">
+      <c r="J13" s="384">
         <f>Conversions!$B$2*'EB2018'!$AO$4</f>
         <v>5.9383641411770398</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="F13">
+    <row r="14" spans="1:11">
+      <c r="F14">
         <v>2019</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>223</v>
       </c>
-      <c r="J13" s="384">
+      <c r="J14" s="384">
         <f>Conversions!$B$2*'EB2019'!$AO$4</f>
         <v>5.5271334489739186</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="F14">
+    <row r="15" spans="1:11">
+      <c r="F15">
         <v>2020</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="384">
+      <c r="J15" s="384">
         <f>Conversions!$B$2*'EB2020'!$AO$4</f>
         <v>6.8879157977152801</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="F15">
+    <row r="16" spans="1:11">
+      <c r="F16">
         <v>2021</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>223</v>
       </c>
-      <c r="J15" s="384">
+      <c r="J16" s="384">
         <f>Conversions!$B$2*'EB2021'!$AO$4</f>
         <v>3.1077995112374399</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
+    <row r="17" spans="2:11">
+      <c r="F17">
+        <v>2022</v>
+      </c>
+      <c r="G17" t="s">
         <v>223</v>
       </c>
-      <c r="J16">
+      <c r="J17" s="391">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>223</v>
+      </c>
+      <c r="J18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
-      <c r="H19" t="s">
+    <row r="21" spans="2:11">
+      <c r="H21" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="379" t="s">
+    <row r="22" spans="2:11">
+      <c r="B22" s="379" t="s">
         <v>461</v>
       </c>
-      <c r="C20" s="380" t="s">
+      <c r="C22" s="380" t="s">
         <v>474</v>
       </c>
-      <c r="D20" s="380" t="s">
+      <c r="D22" s="380" t="s">
         <v>492</v>
       </c>
-      <c r="E20" s="380" t="s">
+      <c r="E22" s="380" t="s">
         <v>225</v>
       </c>
-      <c r="F20" s="380" t="s">
+      <c r="F22" s="380" t="s">
         <v>226</v>
       </c>
-      <c r="G20" s="380" t="s">
+      <c r="G22" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="H20" s="380" t="s">
+      <c r="H22" s="380" t="s">
         <v>486</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I22" t="s">
         <v>499</v>
       </c>
-      <c r="J20" s="382" t="s">
+      <c r="J22" s="382" t="s">
         <v>462</v>
       </c>
-      <c r="K20" s="379" t="s">
+      <c r="K22" s="379" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
-      <c r="B21" t="s">
+    <row r="23" spans="2:11">
+      <c r="B23" t="s">
         <v>503</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>500</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>2018</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>501</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>1</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J23" s="19">
         <f>Conversions!$B$2*'EB2018'!$AH$2</f>
         <v>0.70393223471436184</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
-      <c r="F22">
+    <row r="24" spans="2:11">
+      <c r="F24">
         <v>2019</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>501</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J24" s="19">
         <f>Conversions!$B$2*'EB2019'!$AH$2</f>
         <v>0.78962633124536741</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
-      <c r="F23">
+    <row r="25" spans="2:11">
+      <c r="F25">
         <v>2020</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G25" t="s">
         <v>501</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J25" s="19">
         <f>Conversions!$B$2*'EB2020'!$AH$2</f>
         <v>0.87833840712769273</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
-      <c r="F24">
+    <row r="26" spans="2:11">
+      <c r="F26">
         <v>2021</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>501</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J26" s="19">
         <f>Conversions!$B$2*'EB2021'!$AH$2</f>
         <v>0.94933194191684911</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="27" spans="2:11">
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
         <v>501</v>
       </c>
-      <c r="J25">
+      <c r="J27">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Limit coal and peat consumption by PWR in 2022 to 2021 values (UP)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C5F1B-D1B7-4957-A785-1E73AC2F37FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F735BE1-BBD7-47A9-A07B-B851B592C083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -5227,6 +5227,7 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="40" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5239,7 +5240,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="40" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6343,12 +6343,12 @@
       <c r="Z15" s="61"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="388" t="s">
+      <c r="A16" s="389" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="388"/>
-      <c r="C16" s="388"/>
-      <c r="D16" s="388"/>
+      <c r="B16" s="389"/>
+      <c r="C16" s="389"/>
+      <c r="D16" s="389"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
       <c r="G16" s="63"/>
@@ -6432,11 +6432,11 @@
       <c r="A19" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="387" t="s">
+      <c r="B19" s="388" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="387"/>
-      <c r="D19" s="387"/>
+      <c r="C19" s="388"/>
+      <c r="D19" s="388"/>
       <c r="E19" s="68"/>
       <c r="F19" s="68"/>
       <c r="G19" s="69"/>
@@ -6464,11 +6464,11 @@
       <c r="A20" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="387" t="s">
+      <c r="B20" s="388" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="387"/>
-      <c r="D20" s="387"/>
+      <c r="C20" s="388"/>
+      <c r="D20" s="388"/>
       <c r="E20" s="68"/>
       <c r="F20" s="68"/>
       <c r="G20" s="69"/>
@@ -6556,11 +6556,11 @@
       <c r="A23" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="387" t="s">
+      <c r="B23" s="388" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="387"/>
-      <c r="D23" s="387"/>
+      <c r="C23" s="388"/>
+      <c r="D23" s="388"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
@@ -6586,11 +6586,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="67"/>
-      <c r="B24" s="387" t="s">
+      <c r="B24" s="388" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="387"/>
-      <c r="D24" s="387"/>
+      <c r="C24" s="388"/>
+      <c r="D24" s="388"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
@@ -6648,11 +6648,11 @@
       <c r="A26" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="387" t="s">
+      <c r="B26" s="388" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="387"/>
-      <c r="D26" s="387"/>
+      <c r="C26" s="388"/>
+      <c r="D26" s="388"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
@@ -6768,11 +6768,11 @@
       <c r="A30" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="389" t="s">
+      <c r="B30" s="390" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="387"/>
-      <c r="D30" s="387"/>
+      <c r="C30" s="388"/>
+      <c r="D30" s="388"/>
       <c r="E30" s="72"/>
       <c r="F30" s="72"/>
       <c r="G30" s="61"/>
@@ -6800,11 +6800,11 @@
       <c r="A31" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="387" t="s">
+      <c r="B31" s="388" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="387"/>
-      <c r="D31" s="387"/>
+      <c r="C31" s="388"/>
+      <c r="D31" s="388"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72"/>
       <c r="G31" s="61"/>
@@ -11964,10 +11964,10 @@
       <c r="AC44" s="49"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="390" t="s">
+      <c r="B49" s="391" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="390"/>
+      <c r="C49" s="391"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="48" t="s">
@@ -42597,7 +42597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89305455-607F-41AA-8109-096F19F6FE72}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -42761,7 +42761,7 @@
       <c r="G11" t="s">
         <v>223</v>
       </c>
-      <c r="J11" s="391">
+      <c r="J11" s="387">
         <v>5.8</v>
       </c>
     </row>
@@ -42852,7 +42852,7 @@
       <c r="G17" t="s">
         <v>223</v>
       </c>
-      <c r="J17" s="391">
+      <c r="J17" s="387">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -42986,8 +42986,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43127,7 +43127,8 @@
         <v>28.200000000000003</v>
       </c>
       <c r="J6" s="377">
-        <v>30</v>
+        <f>I6</f>
+        <v>28.200000000000003</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -43195,7 +43196,7 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$10,'EB2021'!$AA$11),1)</f>
         <v>98.1</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="377"/>
       <c r="K8">
         <v>1</v>
       </c>
@@ -43326,7 +43327,10 @@
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$10,'EB2021'!$H$11),1)</f>
         <v>3</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="377">
+        <f>I12</f>
+        <v>3</v>
+      </c>
       <c r="K12">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Modify historic capacity of heavy trucks in 2019
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297978D7-01DC-4339-A28F-284DCB5B44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{297978D7-01DC-4339-A28F-284DCB5B44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B43B1A8C-CA03-4E23-91D8-C950F79D4750}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -5344,6 +5344,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5356,7 +5357,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="40" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5708,7 +5708,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -6028,17 +6028,17 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -6462,12 +6462,12 @@
       <c r="Z15" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="399" t="s">
+      <c r="A16" s="400" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="399"/>
-      <c r="C16" s="399"/>
-      <c r="D16" s="399"/>
+      <c r="B16" s="400"/>
+      <c r="C16" s="400"/>
+      <c r="D16" s="400"/>
       <c r="E16" s="60"/>
       <c r="F16" s="60"/>
       <c r="G16" s="61"/>
@@ -6551,11 +6551,11 @@
       <c r="A19" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="B19" s="398" t="s">
+      <c r="B19" s="399" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="398"/>
-      <c r="D19" s="398"/>
+      <c r="C19" s="399"/>
+      <c r="D19" s="399"/>
       <c r="E19" s="66"/>
       <c r="F19" s="66"/>
       <c r="G19" s="67"/>
@@ -6583,11 +6583,11 @@
       <c r="A20" s="65" t="s">
         <v>406</v>
       </c>
-      <c r="B20" s="398" t="s">
+      <c r="B20" s="399" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="398"/>
-      <c r="D20" s="398"/>
+      <c r="C20" s="399"/>
+      <c r="D20" s="399"/>
       <c r="E20" s="66"/>
       <c r="F20" s="66"/>
       <c r="G20" s="67"/>
@@ -6675,11 +6675,11 @@
       <c r="A23" s="65" t="s">
         <v>408</v>
       </c>
-      <c r="B23" s="398" t="s">
+      <c r="B23" s="399" t="s">
         <v>418</v>
       </c>
-      <c r="C23" s="398"/>
-      <c r="D23" s="398"/>
+      <c r="C23" s="399"/>
+      <c r="D23" s="399"/>
       <c r="E23" s="59"/>
       <c r="F23" s="59"/>
       <c r="G23" s="59"/>
@@ -6705,11 +6705,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="65"/>
-      <c r="B24" s="398" t="s">
+      <c r="B24" s="399" t="s">
         <v>417</v>
       </c>
-      <c r="C24" s="398"/>
-      <c r="D24" s="398"/>
+      <c r="C24" s="399"/>
+      <c r="D24" s="399"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
       <c r="G24" s="59"/>
@@ -6767,11 +6767,11 @@
       <c r="A26" s="65" t="s">
         <v>409</v>
       </c>
-      <c r="B26" s="398" t="s">
+      <c r="B26" s="399" t="s">
         <v>418</v>
       </c>
-      <c r="C26" s="398"/>
-      <c r="D26" s="398"/>
+      <c r="C26" s="399"/>
+      <c r="D26" s="399"/>
       <c r="E26" s="59"/>
       <c r="F26" s="59"/>
       <c r="G26" s="59"/>
@@ -6887,11 +6887,11 @@
       <c r="A30" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="B30" s="400" t="s">
+      <c r="B30" s="401" t="s">
         <v>412</v>
       </c>
-      <c r="C30" s="398"/>
-      <c r="D30" s="398"/>
+      <c r="C30" s="399"/>
+      <c r="D30" s="399"/>
       <c r="E30" s="70"/>
       <c r="F30" s="70"/>
       <c r="G30" s="59"/>
@@ -6919,11 +6919,11 @@
       <c r="A31" s="65" t="s">
         <v>413</v>
       </c>
-      <c r="B31" s="398" t="s">
+      <c r="B31" s="399" t="s">
         <v>414</v>
       </c>
-      <c r="C31" s="398"/>
-      <c r="D31" s="398"/>
+      <c r="C31" s="399"/>
+      <c r="D31" s="399"/>
       <c r="E31" s="70"/>
       <c r="F31" s="70"/>
       <c r="G31" s="59"/>
@@ -8882,14 +8882,14 @@
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -9379,7 +9379,7 @@
       </c>
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="2:10" ht="15.75" thickBot="1">
+    <row r="42" spans="2:10" ht="15" thickBot="1">
       <c r="B42" s="29" t="s">
         <v>227</v>
       </c>
@@ -9605,19 +9605,19 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="32" width="6.85546875" customWidth="1"/>
-    <col min="33" max="33" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="32" width="6.88671875" customWidth="1"/>
+    <col min="33" max="33" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="21">
@@ -9642,7 +9642,7 @@
       <c r="M5" s="37"/>
       <c r="N5" s="37"/>
     </row>
-    <row r="6" spans="1:34" ht="15.75" thickBot="1">
+    <row r="6" spans="1:34" ht="15" thickBot="1">
       <c r="B6" s="36" t="s">
         <v>228</v>
       </c>
@@ -11311,7 +11311,7 @@
       <c r="M25" s="37"/>
       <c r="N25" s="37"/>
     </row>
-    <row r="26" spans="1:34" ht="15.75" thickBot="1">
+    <row r="26" spans="1:34" ht="15" thickBot="1">
       <c r="B26" s="36" t="s">
         <v>228</v>
       </c>
@@ -12979,7 +12979,7 @@
       <c r="M47" s="37"/>
       <c r="N47" s="37"/>
     </row>
-    <row r="48" spans="1:34" ht="15.75" thickBot="1">
+    <row r="48" spans="1:34" ht="15" thickBot="1">
       <c r="B48" s="36" t="s">
         <v>228</v>
       </c>
@@ -14501,111 +14501,112 @@
         <v>2019</v>
       </c>
       <c r="F60" s="397">
-        <v>0</v>
+        <f>0.5*'New vehicle sales'!D33/1000</f>
+        <v>1.325</v>
       </c>
       <c r="G60" s="393">
         <f>$F60*'New vehicle sales'!D$43</f>
-        <v>0</v>
+        <v>1.5841461276201643E-2</v>
       </c>
       <c r="H60" s="393">
         <f>$F60*'New vehicle sales'!E$43</f>
-        <v>0</v>
+        <v>0.37490577221319837</v>
       </c>
       <c r="I60" s="393">
         <f>$F60*'New vehicle sales'!F$43</f>
-        <v>0</v>
+        <v>6.1912254967328925E-2</v>
       </c>
       <c r="J60" s="393">
         <f>$F60*'New vehicle sales'!G$43</f>
-        <v>0</v>
+        <v>2.7611534556313523E-2</v>
       </c>
       <c r="K60" s="393">
         <f>$F60*'New vehicle sales'!H$43</f>
-        <v>0</v>
+        <v>2.3567137035594227E-2</v>
       </c>
       <c r="L60" s="393">
         <f>$F60*'New vehicle sales'!I$43</f>
-        <v>0</v>
+        <v>1.1373007214610235E-2</v>
       </c>
       <c r="M60" s="393">
         <f>$F60*'New vehicle sales'!J$43</f>
-        <v>0</v>
+        <v>3.5862272449974933E-2</v>
       </c>
       <c r="N60" s="393">
         <f>$F60*'New vehicle sales'!K$43</f>
-        <v>0</v>
+        <v>5.4271446166575449E-2</v>
       </c>
       <c r="O60" s="393">
         <f>$F60*'New vehicle sales'!L$43</f>
-        <v>0</v>
+        <v>2.1692829385125349E-2</v>
       </c>
       <c r="P60" s="393">
         <f>$F60*'New vehicle sales'!M$43</f>
-        <v>0</v>
+        <v>2.4700458748830534E-2</v>
       </c>
       <c r="Q60" s="393">
         <f>$F60*'New vehicle sales'!N$43</f>
-        <v>0</v>
+        <v>4.1660494365127913E-2</v>
       </c>
       <c r="R60" s="393">
         <f>$F60*'New vehicle sales'!O$43</f>
-        <v>0</v>
+        <v>3.9630087161227762E-2</v>
       </c>
       <c r="S60" s="393">
         <f>$F60*'New vehicle sales'!P$43</f>
-        <v>0</v>
+        <v>3.3061106310237662E-2</v>
       </c>
       <c r="T60" s="393">
         <f>$F60*'New vehicle sales'!Q$43</f>
-        <v>0</v>
+        <v>0.15105428230325713</v>
       </c>
       <c r="U60" s="393">
         <f>$F60*'New vehicle sales'!R$43</f>
-        <v>0</v>
+        <v>4.109981593346302E-2</v>
       </c>
       <c r="V60" s="393">
         <f>$F60*'New vehicle sales'!S$43</f>
-        <v>0</v>
+        <v>5.4231099579681447E-2</v>
       </c>
       <c r="W60" s="393">
         <f>$F60*'New vehicle sales'!T$43</f>
-        <v>0</v>
+        <v>4.4395992956541161E-2</v>
       </c>
       <c r="X60" s="393">
         <f>$F60*'New vehicle sales'!U$43</f>
-        <v>0</v>
+        <v>3.2326241924120043E-2</v>
       </c>
       <c r="Y60" s="393">
         <f>$F60*'New vehicle sales'!V$43</f>
-        <v>0</v>
+        <v>7.1805238073737856E-2</v>
       </c>
       <c r="Z60" s="393">
         <f>$F60*'New vehicle sales'!W$43</f>
-        <v>0</v>
+        <v>8.9163174512507104E-3</v>
       </c>
       <c r="AA60" s="393">
         <f>$F60*'New vehicle sales'!X$43</f>
-        <v>0</v>
+        <v>3.6313875970864336E-2</v>
       </c>
       <c r="AB60" s="393">
         <f>$F60*'New vehicle sales'!Y$43</f>
-        <v>0</v>
+        <v>1.7959517961974966E-2</v>
       </c>
       <c r="AC60" s="393">
         <f>$F60*'New vehicle sales'!Z$43</f>
-        <v>0</v>
+        <v>1.8235266014471205E-2</v>
       </c>
       <c r="AD60" s="393">
         <f>$F60*'New vehicle sales'!AA$43</f>
-        <v>0</v>
+        <v>2.119614898784403E-2</v>
       </c>
       <c r="AE60" s="393">
         <f>$F60*'New vehicle sales'!AB$43</f>
-        <v>0</v>
+        <v>4.4295543867791255E-2</v>
       </c>
       <c r="AF60" s="393">
         <f>$F60*'New vehicle sales'!AC$43</f>
-        <v>0</v>
+        <v>1.7080797124655978E-2</v>
       </c>
       <c r="AG60" s="30" t="str">
         <f t="shared" si="4"/>
@@ -14630,11 +14631,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14745,17 +14746,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -14906,18 +14907,18 @@
       <selection activeCell="B2" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -15065,14 +15066,14 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AC179"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="7" width="12" customWidth="1"/>
   </cols>
@@ -15082,17 +15083,17 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.6">
       <c r="A2" s="57" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="57" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.6">
       <c r="A5" s="56" t="s">
         <v>393</v>
       </c>
@@ -15218,12 +15219,12 @@
         <v>117109</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75">
+    <row r="17" spans="1:5" ht="15.6">
       <c r="A17" s="57" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75">
+    <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="56" t="s">
         <v>393</v>
       </c>
@@ -15359,12 +15360,12 @@
         <v>25336</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75">
+    <row r="31" spans="1:5" ht="15.6">
       <c r="A31" s="57" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75">
+    <row r="32" spans="1:5" ht="15.6">
       <c r="A32" s="56" t="s">
         <v>393</v>
       </c>
@@ -15442,7 +15443,7 @@
         <v>2659</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="15.75">
+    <row r="40" spans="1:29" ht="15.6">
       <c r="B40" s="55" t="s">
         <v>386</v>
       </c>
@@ -15736,12 +15737,12 @@
       <c r="AC44" s="47"/>
     </row>
     <row r="49" spans="2:3" ht="21">
-      <c r="B49" s="401" t="s">
+      <c r="B49" s="402" t="s">
         <v>382</v>
       </c>
-      <c r="C49" s="401"/>
-    </row>
-    <row r="50" spans="2:3" ht="15.75" thickBot="1">
+      <c r="C49" s="402"/>
+    </row>
+    <row r="50" spans="2:3" ht="15" thickBot="1">
       <c r="B50" s="46" t="s">
         <v>381</v>
       </c>
@@ -15749,7 +15750,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15.75" thickBot="1">
+    <row r="51" spans="2:3" ht="15" thickBot="1">
       <c r="B51" s="45" t="s">
         <v>379</v>
       </c>
@@ -16380,7 +16381,7 @@
       <c r="C131" s="389"/>
       <c r="D131" s="389"/>
     </row>
-    <row r="132" spans="1:9" ht="15.75">
+    <row r="132" spans="1:9" ht="15.6">
       <c r="A132" s="390" t="s">
         <v>536</v>
       </c>
@@ -16388,7 +16389,7 @@
       <c r="C132" s="389"/>
       <c r="D132" s="389"/>
     </row>
-    <row r="134" spans="1:9" ht="15.75">
+    <row r="134" spans="1:9" ht="15.6">
       <c r="A134" s="390" t="s">
         <v>401</v>
       </c>
@@ -16404,7 +16405,7 @@
       <c r="C135" s="389"/>
       <c r="D135" s="389"/>
     </row>
-    <row r="137" spans="1:9" ht="15.75">
+    <row r="137" spans="1:9" ht="15.6">
       <c r="A137" s="387" t="s">
         <v>393</v>
       </c>
@@ -16656,7 +16657,7 @@
       <c r="F149" s="389"/>
       <c r="G149" s="389"/>
     </row>
-    <row r="150" spans="1:9" ht="15.75">
+    <row r="150" spans="1:9" ht="15.6">
       <c r="A150" s="390" t="s">
         <v>536</v>
       </c>
@@ -16667,7 +16668,7 @@
       <c r="F150" s="389"/>
       <c r="G150" s="389"/>
     </row>
-    <row r="152" spans="1:9" ht="15.75">
+    <row r="152" spans="1:9" ht="15.6">
       <c r="A152" s="390" t="s">
         <v>400</v>
       </c>
@@ -16689,7 +16690,7 @@
       <c r="F153" s="389"/>
       <c r="G153" s="389"/>
     </row>
-    <row r="155" spans="1:9" ht="15.75">
+    <row r="155" spans="1:9" ht="15.6">
       <c r="A155" s="390" t="s">
         <v>393</v>
       </c>
@@ -16918,7 +16919,7 @@
       <c r="F166" s="389"/>
       <c r="G166" s="389"/>
     </row>
-    <row r="167" spans="1:9" ht="15.75">
+    <row r="167" spans="1:9" ht="15.6">
       <c r="A167" s="390" t="s">
         <v>536</v>
       </c>
@@ -16929,7 +16930,7 @@
       <c r="F167" s="389"/>
       <c r="G167" s="389"/>
     </row>
-    <row r="169" spans="1:9" ht="15.75">
+    <row r="169" spans="1:9" ht="15.6">
       <c r="A169" s="390" t="s">
         <v>394</v>
       </c>
@@ -16951,7 +16952,7 @@
       <c r="F170" s="389"/>
       <c r="G170" s="389"/>
     </row>
-    <row r="172" spans="1:9" ht="15.75">
+    <row r="172" spans="1:9" ht="15.6">
       <c r="A172" s="390" t="s">
         <v>393</v>
       </c>
@@ -17163,46 +17164,46 @@
       <selection pane="bottomRight" activeCell="AS53" sqref="AS53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="12"/>
+    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="5.5703125" style="7" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7109375" style="7" customWidth="1"/>
-    <col min="33" max="33" width="5.5703125" style="7" customWidth="1"/>
-    <col min="34" max="34" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="5.5546875" style="7" customWidth="1"/>
+    <col min="31" max="31" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.6640625" style="7" customWidth="1"/>
+    <col min="33" max="33" width="5.5546875" style="7" customWidth="1"/>
+    <col min="34" max="34" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" style="7"/>
-    <col min="45" max="45" width="9.140625" style="9"/>
-    <col min="46" max="16384" width="9.140625" style="7"/>
+    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.109375" style="7"/>
+    <col min="45" max="45" width="9.109375" style="9"/>
+    <col min="46" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="105.75" customHeight="1" thickBot="1">
@@ -24447,45 +24448,45 @@
       <selection pane="bottomRight" activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
     <col min="7" max="7" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
+    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
+    <col min="27" max="27" width="7.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="35" width="7" style="7" customWidth="1"/>
-    <col min="36" max="36" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.5703125" style="7" customWidth="1"/>
-    <col min="39" max="39" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.5703125" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="7"/>
+    <col min="36" max="36" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.5546875" style="7" customWidth="1"/>
+    <col min="39" max="39" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.5546875" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="105.75" customHeight="1" thickBot="1">
@@ -31710,41 +31711,41 @@
       <selection pane="bottomRight" activeCell="AQ45" sqref="AQ45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="12"/>
+    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="7"/>
+    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
@@ -38737,7 +38738,7 @@
       <c r="AP76" s="23"/>
       <c r="AQ76" s="23"/>
     </row>
-    <row r="77" spans="1:43" ht="15">
+    <row r="77" spans="1:43" ht="14.4">
       <c r="A77" s="363" t="s">
         <v>437</v>
       </c>
@@ -38784,7 +38785,7 @@
       <c r="AP77" s="23"/>
       <c r="AQ77" s="23"/>
     </row>
-    <row r="78" spans="1:43" ht="15">
+    <row r="78" spans="1:43" ht="14.4">
       <c r="A78" s="24" t="s">
         <v>438</v>
       </c>
@@ -38831,7 +38832,7 @@
       <c r="AP78" s="23"/>
       <c r="AQ78" s="23"/>
     </row>
-    <row r="79" spans="1:43" ht="15">
+    <row r="79" spans="1:43" ht="14.4">
       <c r="A79" s="364" t="s">
         <v>153</v>
       </c>
@@ -38878,7 +38879,7 @@
       <c r="AP79" s="369"/>
       <c r="AQ79" s="366"/>
     </row>
-    <row r="80" spans="1:43" ht="15">
+    <row r="80" spans="1:43" ht="14.4">
       <c r="A80" s="364" t="s">
         <v>154</v>
       </c>
@@ -39032,41 +39033,41 @@
       <selection pane="bottomRight" activeCell="AA65" sqref="AA65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="12"/>
+    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="7"/>
+    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
@@ -46059,7 +46060,7 @@
       <c r="AP76" s="23"/>
       <c r="AQ76" s="23"/>
     </row>
-    <row r="77" spans="1:43" ht="15">
+    <row r="77" spans="1:43" ht="14.4">
       <c r="A77" s="363" t="s">
         <v>443</v>
       </c>
@@ -46106,7 +46107,7 @@
       <c r="AP77" s="23"/>
       <c r="AQ77" s="23"/>
     </row>
-    <row r="78" spans="1:43" ht="15">
+    <row r="78" spans="1:43" ht="14.4">
       <c r="A78" s="24" t="s">
         <v>444</v>
       </c>
@@ -46153,7 +46154,7 @@
       <c r="AP78" s="23"/>
       <c r="AQ78" s="23"/>
     </row>
-    <row r="79" spans="1:43" ht="15">
+    <row r="79" spans="1:43" ht="14.4">
       <c r="A79" s="364" t="s">
         <v>153</v>
       </c>
@@ -46200,7 +46201,7 @@
       <c r="AP79" s="369"/>
       <c r="AQ79" s="366"/>
     </row>
-    <row r="80" spans="1:43" ht="15">
+    <row r="80" spans="1:43" ht="14.4">
       <c r="A80" s="364" t="s">
         <v>154</v>
       </c>
@@ -46351,35 +46352,35 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:30">
@@ -46850,7 +46851,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1">
+    <row r="10" spans="1:30" ht="15" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -47092,7 +47093,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>30480</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -47118,9 +47119,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -47152,18 +47153,18 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -47312,7 +47313,7 @@
       <c r="G11" t="s">
         <v>223</v>
       </c>
-      <c r="J11" s="402">
+      <c r="J11" s="398">
         <v>5.8</v>
       </c>
     </row>
@@ -47403,7 +47404,7 @@
       <c r="G17" t="s">
         <v>223</v>
       </c>
-      <c r="J17" s="402">
+      <c r="J17" s="398">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -47537,15 +47538,15 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
@@ -47554,7 +47555,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1">
+    <row r="3" spans="2:11" ht="15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -47976,15 +47977,15 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -48003,7 +48004,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1">
+    <row r="6" spans="2:8" ht="15" thickBot="1">
       <c r="B6" s="29" t="s">
         <v>461</v>
       </c>
@@ -48241,12 +48242,12 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48255,7 +48256,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48328,12 +48329,12 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48342,7 +48343,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48415,12 +48416,12 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48429,7 +48430,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48822,12 +48823,12 @@
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48836,7 +48837,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
Historic bound fix for regions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1623D-8E93-457C-A0DE-500CEE9AD892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F312E64F-9153-4479-9DB4-94AD2D0E6A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="534">
   <si>
     <t>Development</t>
   </si>
@@ -1809,6 +1809,27 @@
   </si>
   <si>
     <t>FT-SRVAHT</t>
+  </si>
+  <si>
+    <t>Historic wood consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic coal consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic peat consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic electric consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic gas consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic LPG consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>Historic Kerosene consumption in RSD - Multi</t>
   </si>
 </sst>
 </file>
@@ -8757,7 +8778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2D405-BB6D-42D0-B84A-79AAA54CB8B4}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
@@ -43830,402 +43851,1034 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
-  <dimension ref="B2:J14"/>
+  <dimension ref="B2:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="378" t="str">
+        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!P5:AO5)</f>
+        <v>~UC_Sets: R_S: IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="378" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="G4" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="379" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="380" t="s">
+        <v>474</v>
+      </c>
+      <c r="D5" s="380" t="s">
+        <v>475</v>
+      </c>
+      <c r="E5" s="380" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="380" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="380" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="381" t="s">
+        <v>499</v>
+      </c>
+      <c r="I5" s="382" t="s">
+        <v>480</v>
+      </c>
+      <c r="J5" s="379" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="str">
+        <f>"UC_Historic_"&amp;C7&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDBDL-cons_Multi</v>
+      </c>
+      <c r="C7" t="str">
+        <f>RIGHT(C55, LEN(C55) - 3)</f>
+        <v>RSDBDL</v>
+      </c>
+      <c r="F7">
+        <v>2018</v>
+      </c>
+      <c r="G7" t="s">
+        <v>501</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19">
+        <f>F56</f>
+        <v>1.3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8" t="s">
+        <v>501</v>
+      </c>
+      <c r="I8" s="19">
+        <f>G56</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9" t="s">
+        <v>501</v>
+      </c>
+      <c r="I9" s="19">
+        <f>H56</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="F10">
+        <v>2021</v>
+      </c>
+      <c r="G10" t="s">
+        <v>501</v>
+      </c>
+      <c r="I10" s="19">
+        <f>I56</f>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F11,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="str">
+        <f>"UC_Historic_"&amp;C12&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDCOA-cons_Multi</v>
+      </c>
+      <c r="C12" t="str">
+        <f>RIGHT(C57, LEN(C57) - 3)</f>
+        <v>RSDCOA</v>
+      </c>
+      <c r="F12">
+        <v>2018</v>
+      </c>
+      <c r="G12" t="s">
+        <v>501</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="19">
+        <f>F57</f>
+        <v>9.1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="F13">
+        <v>2019</v>
+      </c>
+      <c r="G13" t="s">
+        <v>501</v>
+      </c>
+      <c r="I13" s="19">
+        <f>G57</f>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="F14">
+        <v>2020</v>
+      </c>
+      <c r="G14" t="s">
+        <v>501</v>
+      </c>
+      <c r="I14" s="19">
+        <f>H57</f>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="F15">
+        <v>2021</v>
+      </c>
+      <c r="G15" t="s">
+        <v>501</v>
+      </c>
+      <c r="I15" s="19">
+        <f>I57</f>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F16,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" t="str">
+        <f>"UC_Historic_"&amp;C17&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDPEA-cons_Multi</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RIGHT(C58, LEN(C58) - 3)</f>
+        <v>RSDPEA</v>
+      </c>
+      <c r="F17">
+        <v>2018</v>
+      </c>
+      <c r="G17" t="s">
+        <v>501</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="19">
+        <f>F58</f>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="J17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="F18">
+        <v>2019</v>
+      </c>
+      <c r="G18" t="s">
+        <v>501</v>
+      </c>
+      <c r="I18" s="19">
+        <f>G58</f>
+        <v>7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="F19">
+        <v>2020</v>
+      </c>
+      <c r="G19" t="s">
+        <v>501</v>
+      </c>
+      <c r="I19" s="19">
+        <f>H58</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="F20">
+        <v>2021</v>
+      </c>
+      <c r="G20" t="s">
+        <v>501</v>
+      </c>
+      <c r="I20" s="19">
+        <f>I58</f>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F21,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" t="str">
+        <f>"UC_Historic_"&amp;C22&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDELC-cons_Multi</v>
+      </c>
+      <c r="C22" t="str">
+        <f>RIGHT(C59, LEN(C59) - 3)</f>
+        <v>RSDELC</v>
+      </c>
+      <c r="F22">
+        <v>2018</v>
+      </c>
+      <c r="G22" t="s">
+        <v>501</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="19">
+        <f>F59</f>
+        <v>29.5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="F23">
+        <v>2019</v>
+      </c>
+      <c r="G23" t="s">
+        <v>501</v>
+      </c>
+      <c r="I23" s="19">
+        <f>G59</f>
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="F24">
+        <v>2020</v>
+      </c>
+      <c r="G24" t="s">
+        <v>501</v>
+      </c>
+      <c r="I24" s="19">
+        <f>H59</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="F25">
+        <v>2021</v>
+      </c>
+      <c r="G25" t="s">
+        <v>501</v>
+      </c>
+      <c r="I25" s="19">
+        <f>I59</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F26,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" t="str">
+        <f>"UC_Historic_"&amp;C27&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDGAS-cons_Multi</v>
+      </c>
+      <c r="C27" t="str">
+        <f>RIGHT(C61, LEN(C61) - 3)</f>
+        <v>RSDGAS</v>
+      </c>
+      <c r="F27">
+        <v>2018</v>
+      </c>
+      <c r="G27" t="s">
+        <v>501</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19">
+        <f>F61</f>
+        <v>25.3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="F28">
+        <v>2019</v>
+      </c>
+      <c r="G28" t="s">
+        <v>501</v>
+      </c>
+      <c r="I28" s="19">
+        <f>G61</f>
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="F29">
+        <v>2020</v>
+      </c>
+      <c r="G29" t="s">
+        <v>501</v>
+      </c>
+      <c r="I29" s="19">
+        <f>H61</f>
+        <v>24.700000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="F30">
+        <v>2021</v>
+      </c>
+      <c r="G30" t="s">
+        <v>501</v>
+      </c>
+      <c r="I30" s="19">
+        <f>I61</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F31,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" t="str">
+        <f>"UC_Historic_"&amp;C32&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDLPG-cons_Multi</v>
+      </c>
+      <c r="C32" t="str">
+        <f>RIGHT(C63, LEN(C63) - 3)</f>
+        <v>RSDLPG</v>
+      </c>
+      <c r="F32">
+        <v>2018</v>
+      </c>
+      <c r="G32" t="s">
+        <v>501</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" s="19">
+        <f>F63</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="J32" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="F33">
+        <v>2019</v>
+      </c>
+      <c r="G33" t="s">
+        <v>501</v>
+      </c>
+      <c r="I33" s="19">
+        <f>G63</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="F34">
+        <v>2020</v>
+      </c>
+      <c r="G34" t="s">
+        <v>501</v>
+      </c>
+      <c r="I34" s="19">
+        <f>H63</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="F35">
+        <v>2021</v>
+      </c>
+      <c r="G35" t="s">
+        <v>501</v>
+      </c>
+      <c r="I35" s="19">
+        <f>I63</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F36,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" t="str">
+        <f>"UC_Historic_"&amp;C37&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDKER-cons_Multi</v>
+      </c>
+      <c r="C37" t="str">
+        <f>RIGHT(C64, LEN(C64) - 3)</f>
+        <v>RSDKER</v>
+      </c>
+      <c r="F37">
+        <v>2018</v>
+      </c>
+      <c r="G37" t="s">
+        <v>501</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37" s="19">
+        <f>F64</f>
+        <v>50.300000000000004</v>
+      </c>
+      <c r="J37" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="F38">
+        <v>2019</v>
+      </c>
+      <c r="G38" t="s">
+        <v>501</v>
+      </c>
+      <c r="I38" s="19">
+        <f>G64</f>
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="F39">
+        <v>2020</v>
+      </c>
+      <c r="G39" t="s">
+        <v>501</v>
+      </c>
+      <c r="I39" s="19">
+        <f>H64</f>
+        <v>56.2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="F40">
+        <v>2021</v>
+      </c>
+      <c r="G40" t="s">
+        <v>501</v>
+      </c>
+      <c r="I40" s="19">
+        <f>I64</f>
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F41,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" t="str">
+        <f>"UC_Historic_"&amp;C42&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDSOL-cons_Multi</v>
+      </c>
+      <c r="C42" t="str">
+        <f>RIGHT(C65, LEN(C65) - 3)</f>
+        <v>RSDSOL</v>
+      </c>
+      <c r="F42">
+        <v>2018</v>
+      </c>
+      <c r="G42" t="s">
+        <v>501</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" s="19">
+        <f>F65</f>
+        <v>0.6</v>
+      </c>
+      <c r="J42" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="F43">
+        <v>2019</v>
+      </c>
+      <c r="G43" t="s">
+        <v>501</v>
+      </c>
+      <c r="I43" s="19">
+        <f>G65</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="F44">
+        <v>2020</v>
+      </c>
+      <c r="G44" t="s">
+        <v>501</v>
+      </c>
+      <c r="I44" s="19">
+        <f>H65</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="F45">
+        <v>2021</v>
+      </c>
+      <c r="G45" t="s">
+        <v>501</v>
+      </c>
+      <c r="I45" s="19">
+        <f>I65</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F46,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B3" s="29" t="s">
+      <c r="D53" s="18"/>
+    </row>
+    <row r="54" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B54" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C54" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D54" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E54" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F54" s="29">
         <v>2018</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G54" s="29">
         <v>2019</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H54" s="29">
         <v>2020</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I54" s="29">
         <v>2021</v>
       </c>
-      <c r="J3" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" t="s">
+      <c r="J54" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" t="s">
         <v>456</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C55" t="s">
         <v>453</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D55" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="19" t="str">
+      <c r="E55" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F55" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G55" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H55" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I55" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="J55">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="C5" t="s">
+    <row r="56" spans="2:10">
+      <c r="C56" t="s">
         <v>450</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D56" t="s">
         <v>200</v>
       </c>
-      <c r="E5" s="19" t="str">
+      <c r="E56" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F56" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
         <v>1.3</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G56" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H56" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I56" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="J5">
+      <c r="J56">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="C6" t="s">
+    <row r="57" spans="2:10">
+      <c r="C57" t="s">
         <v>445</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D57" t="s">
         <v>200</v>
       </c>
-      <c r="E6" s="19" t="str">
+      <c r="E57" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
         <v>9.1</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
         <v>7.8</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
         <v>7.8</v>
       </c>
-      <c r="J6">
+      <c r="J57">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="C7" t="s">
+    <row r="58" spans="2:10">
+      <c r="C58" t="s">
         <v>452</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D58" t="s">
         <v>200</v>
       </c>
-      <c r="E7" s="19" t="str">
+      <c r="E58" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F58" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
         <v>8.2999999999999989</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G58" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
         <v>7.6999999999999993</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H58" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
         <v>8</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I58" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
         <v>7.6</v>
       </c>
-      <c r="J7">
+      <c r="J58">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="C8" t="s">
+    <row r="59" spans="2:10">
+      <c r="C59" t="s">
         <v>446</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D59" t="s">
         <v>200</v>
       </c>
-      <c r="E8" s="19" t="str">
+      <c r="E59" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F59" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
         <v>29.5</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G59" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
         <v>30.8</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H59" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
         <v>31.5</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I59" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
         <v>31.5</v>
       </c>
-      <c r="J8">
+      <c r="J59">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" t="s">
+    <row r="60" spans="2:10">
+      <c r="B60" t="s">
         <v>456</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C60" t="s">
         <v>454</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D60" t="s">
         <v>200</v>
       </c>
-      <c r="E9" s="19" t="str">
+      <c r="E60" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F60" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G60" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H60" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I60" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="J60">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="C10" t="s">
+    <row r="61" spans="2:10">
+      <c r="C61" t="s">
         <v>447</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D61" t="s">
         <v>200</v>
       </c>
-      <c r="E10" s="19" t="str">
+      <c r="E61" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F61" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
         <v>25.3</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G61" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
         <v>24.8</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H61" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
         <v>24.700000000000003</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I61" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
         <v>25</v>
       </c>
-      <c r="J10">
+      <c r="J61">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" t="s">
+    <row r="62" spans="2:10">
+      <c r="B62" t="s">
         <v>456</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C62" t="s">
         <v>455</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D62" t="s">
         <v>200</v>
       </c>
-      <c r="E11" s="19" t="str">
+      <c r="E62" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F62" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G62" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H62" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I62" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="J62">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="C12" t="s">
+    <row r="63" spans="2:10">
+      <c r="C63" t="s">
         <v>448</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D63" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="19" t="str">
+      <c r="E63" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F63" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
         <v>2.3000000000000003</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G63" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
         <v>2.1</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H63" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
         <v>2.4</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I63" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
         <v>2.1</v>
       </c>
-      <c r="J12">
+      <c r="J63">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="C13" t="s">
+    <row r="64" spans="2:10">
+      <c r="C64" t="s">
         <v>451</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D64" t="s">
         <v>200</v>
       </c>
-      <c r="E13" s="19" t="str">
+      <c r="E64" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F64" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
         <v>50.300000000000004</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G64" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
         <v>49.9</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H64" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
         <v>56.2</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I64" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
         <v>51.2</v>
       </c>
-      <c r="J13">
+      <c r="J64">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="C14" t="s">
+    <row r="65" spans="3:10">
+      <c r="C65" t="s">
         <v>449</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D65" t="s">
         <v>200</v>
       </c>
-      <c r="E14" s="19" t="str">
+      <c r="E65" s="19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F65" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G65" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H65" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I65" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="J14">
+      <c r="J65">
         <v>1</v>
       </c>
     </row>
@@ -44239,7 +44892,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove 2018 RSD historic bounds
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F312E64F-9153-4479-9DB4-94AD2D0E6A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1336882A-4DAC-45D7-9995-C34B841FB568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="535">
   <si>
     <t>Development</t>
   </si>
@@ -1830,6 +1830,9 @@
   </si>
   <si>
     <t>Historic Kerosene consumption in RSD - Multi</t>
+  </si>
+  <si>
+    <t>*2018</t>
   </si>
 </sst>
 </file>
@@ -43851,10 +43854,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F351D98-D2D4-43AF-AC16-FF530EC6F60A}">
-  <dimension ref="B2:J65"/>
+  <dimension ref="B2:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43935,21 +43938,18 @@
         <v>UC_Historic_RSDBDL-cons_Multi</v>
       </c>
       <c r="C7" t="str">
-        <f>RIGHT(C55, LEN(C55) - 3)</f>
+        <f>RIGHT(C47, LEN(C47) - 3)</f>
         <v>RSDBDL</v>
       </c>
       <c r="F7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G7" t="s">
         <v>501</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="I7" s="19">
-        <f>F56</f>
-        <v>1.3</v>
+        <f>G48</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J7" t="s">
         <v>527</v>
@@ -43957,218 +43957,214 @@
     </row>
     <row r="8" spans="2:10">
       <c r="F8">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G8" t="s">
         <v>501</v>
       </c>
       <c r="I8" s="19">
-        <f>G56</f>
+        <f>H48</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="F9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G9" t="s">
         <v>501</v>
       </c>
       <c r="I9" s="19">
-        <f>H56</f>
-        <v>1.1000000000000001</v>
+        <f>I48</f>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="F10">
-        <v>2021</v>
-      </c>
-      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F10,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="str">
+        <f>"UC_Historic_"&amp;C11&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDCOA-cons_Multi</v>
+      </c>
+      <c r="C11" t="str">
+        <f>RIGHT(C49, LEN(C49) - 3)</f>
+        <v>RSDCOA</v>
+      </c>
+      <c r="F11">
+        <v>2019</v>
+      </c>
+      <c r="G11" t="s">
         <v>501</v>
       </c>
-      <c r="I10" s="19">
-        <f>I56</f>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F11,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
+      <c r="I11" s="19">
+        <f>G49</f>
+        <v>7.8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" t="str">
-        <f>"UC_Historic_"&amp;C12&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDCOA-cons_Multi</v>
-      </c>
-      <c r="C12" t="str">
-        <f>RIGHT(C57, LEN(C57) - 3)</f>
-        <v>RSDCOA</v>
-      </c>
       <c r="F12">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G12" t="s">
         <v>501</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
       <c r="I12" s="19">
-        <f>F57</f>
-        <v>9.1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>528</v>
+        <f>H49</f>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="F13">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G13" t="s">
         <v>501</v>
       </c>
       <c r="I13" s="19">
-        <f>G57</f>
+        <f>I49</f>
         <v>7.8</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="F14">
-        <v>2020</v>
-      </c>
-      <c r="G14" t="s">
-        <v>501</v>
-      </c>
-      <c r="I14" s="19">
-        <f>H57</f>
-        <v>8.1999999999999993</v>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F14,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:10">
+      <c r="B15" t="str">
+        <f>"UC_Historic_"&amp;C15&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDPEA-cons_Multi</v>
+      </c>
+      <c r="C15" t="str">
+        <f>RIGHT(C50, LEN(C50) - 3)</f>
+        <v>RSDPEA</v>
+      </c>
       <c r="F15">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="G15" t="s">
         <v>501</v>
       </c>
       <c r="I15" s="19">
-        <f>I57</f>
-        <v>7.8</v>
+        <f>G50</f>
+        <v>7.6999999999999993</v>
+      </c>
+      <c r="J15" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F16,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
+        <v>2020</v>
+      </c>
+      <c r="G16" t="s">
+        <v>501</v>
+      </c>
+      <c r="I16" s="19">
+        <f>H50</f>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" t="str">
-        <f>"UC_Historic_"&amp;C17&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDPEA-cons_Multi</v>
-      </c>
-      <c r="C17" t="str">
-        <f>RIGHT(C58, LEN(C58) - 3)</f>
-        <v>RSDPEA</v>
-      </c>
       <c r="F17">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="G17" t="s">
         <v>501</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
       <c r="I17" s="19">
-        <f>F58</f>
-        <v>8.2999999999999989</v>
-      </c>
-      <c r="J17" t="s">
-        <v>529</v>
+        <f>I50</f>
+        <v>7.6</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F18,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" t="str">
+        <f>"UC_Historic_"&amp;C19&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDELC-cons_Multi</v>
+      </c>
+      <c r="C19" t="str">
+        <f>RIGHT(C51, LEN(C51) - 3)</f>
+        <v>RSDELC</v>
+      </c>
+      <c r="F19">
         <v>2019</v>
-      </c>
-      <c r="G18" t="s">
-        <v>501</v>
-      </c>
-      <c r="I18" s="19">
-        <f>G58</f>
-        <v>7.6999999999999993</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="F19">
-        <v>2020</v>
       </c>
       <c r="G19" t="s">
         <v>501</v>
       </c>
       <c r="I19" s="19">
-        <f>H58</f>
-        <v>8</v>
+        <f>G51</f>
+        <v>30.8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="F20">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="G20" t="s">
         <v>501</v>
       </c>
       <c r="I20" s="19">
-        <f>I58</f>
-        <v>7.6</v>
+        <f>H51</f>
+        <v>31.5</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F21,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>2021</v>
+      </c>
+      <c r="G21" t="s">
+        <v>501</v>
+      </c>
+      <c r="I21" s="19">
+        <f>I51</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F22,'CO2-config'!$B$6:$D$6,),FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
-      <c r="B22" t="str">
-        <f>"UC_Historic_"&amp;C22&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDELC-cons_Multi</v>
-      </c>
-      <c r="C22" t="str">
-        <f>RIGHT(C59, LEN(C59) - 3)</f>
-        <v>RSDELC</v>
-      </c>
-      <c r="F22">
-        <v>2018</v>
-      </c>
-      <c r="G22" t="s">
-        <v>501</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="19">
-        <f>F59</f>
-        <v>29.5</v>
-      </c>
-      <c r="J22" t="s">
-        <v>530</v>
-      </c>
-    </row>
     <row r="23" spans="2:10">
+      <c r="B23" t="str">
+        <f>"UC_Historic_"&amp;C23&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDGAS-cons_Multi</v>
+      </c>
+      <c r="C23" t="str">
+        <f>RIGHT(C53, LEN(C53) - 3)</f>
+        <v>RSDGAS</v>
+      </c>
       <c r="F23">
         <v>2019</v>
       </c>
@@ -44176,8 +44172,11 @@
         <v>501</v>
       </c>
       <c r="I23" s="19">
-        <f>G59</f>
-        <v>30.8</v>
+        <f>G53</f>
+        <v>24.8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -44188,8 +44187,8 @@
         <v>501</v>
       </c>
       <c r="I24" s="19">
-        <f>H59</f>
-        <v>31.5</v>
+        <f>H53</f>
+        <v>24.700000000000003</v>
       </c>
     </row>
     <row r="25" spans="2:10">
@@ -44200,8 +44199,8 @@
         <v>501</v>
       </c>
       <c r="I25" s="19">
-        <f>I59</f>
-        <v>31.5</v>
+        <f>I53</f>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -44216,328 +44215,466 @@
     <row r="27" spans="2:10">
       <c r="B27" t="str">
         <f>"UC_Historic_"&amp;C27&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDGAS-cons_Multi</v>
+        <v>UC_Historic_RSDLPG-cons_Multi</v>
       </c>
       <c r="C27" t="str">
-        <f>RIGHT(C61, LEN(C61) - 3)</f>
-        <v>RSDGAS</v>
+        <f>RIGHT(C55, LEN(C55) - 3)</f>
+        <v>RSDLPG</v>
       </c>
       <c r="F27">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G27" t="s">
         <v>501</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
       <c r="I27" s="19">
-        <f>F61</f>
-        <v>25.3</v>
+        <f>G55</f>
+        <v>2.1</v>
       </c>
       <c r="J27" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="F28">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G28" t="s">
         <v>501</v>
       </c>
       <c r="I28" s="19">
-        <f>G61</f>
-        <v>24.8</v>
+        <f>H55</f>
+        <v>2.4</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="F29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G29" t="s">
         <v>501</v>
       </c>
       <c r="I29" s="19">
-        <f>H61</f>
-        <v>24.700000000000003</v>
+        <f>I55</f>
+        <v>2.1</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="F30">
-        <v>2021</v>
-      </c>
-      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F30,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" t="str">
+        <f>"UC_Historic_"&amp;C31&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDKER-cons_Multi</v>
+      </c>
+      <c r="C31" t="str">
+        <f>RIGHT(C56, LEN(C56) - 3)</f>
+        <v>RSDKER</v>
+      </c>
+      <c r="F31">
+        <v>2019</v>
+      </c>
+      <c r="G31" t="s">
         <v>501</v>
       </c>
-      <c r="I30" s="19">
-        <f>I61</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F31,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
+      <c r="I31" s="19">
+        <f>G56</f>
+        <v>49.9</v>
+      </c>
+      <c r="J31" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" t="str">
-        <f>"UC_Historic_"&amp;C32&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDLPG-cons_Multi</v>
-      </c>
-      <c r="C32" t="str">
-        <f>RIGHT(C63, LEN(C63) - 3)</f>
-        <v>RSDLPG</v>
-      </c>
       <c r="F32">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G32" t="s">
         <v>501</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
       <c r="I32" s="19">
-        <f>F63</f>
-        <v>2.3000000000000003</v>
-      </c>
-      <c r="J32" t="s">
-        <v>532</v>
+        <f>H56</f>
+        <v>56.2</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="F33">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G33" t="s">
         <v>501</v>
       </c>
       <c r="I33" s="19">
-        <f>G63</f>
-        <v>2.1</v>
+        <f>I56</f>
+        <v>51.2</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="F34">
-        <v>2020</v>
-      </c>
-      <c r="G34" t="s">
-        <v>501</v>
-      </c>
-      <c r="I34" s="19">
-        <f>H63</f>
-        <v>2.4</v>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F34,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:10">
+      <c r="B35" t="str">
+        <f>"UC_Historic_"&amp;C35&amp;"-cons_Multi"</f>
+        <v>UC_Historic_RSDSOL-cons_Multi</v>
+      </c>
+      <c r="C35" t="str">
+        <f>RIGHT(C57, LEN(C57) - 3)</f>
+        <v>RSDSOL</v>
+      </c>
       <c r="F35">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="G35" t="s">
         <v>501</v>
       </c>
       <c r="I35" s="19">
-        <f>I63</f>
-        <v>2.1</v>
+        <f>G57</f>
+        <v>0.6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F36,'CO2-config'!$B$6:$D$6,),FALSE)</f>
-        <v>1</v>
+        <v>2020</v>
+      </c>
+      <c r="G36" t="s">
+        <v>501</v>
+      </c>
+      <c r="I36" s="19">
+        <f>H57</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37" spans="2:10">
-      <c r="B37" t="str">
-        <f>"UC_Historic_"&amp;C37&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDKER-cons_Multi</v>
-      </c>
-      <c r="C37" t="str">
-        <f>RIGHT(C64, LEN(C64) - 3)</f>
-        <v>RSDKER</v>
-      </c>
       <c r="F37">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="G37" t="s">
         <v>501</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
       <c r="I37" s="19">
-        <f>F64</f>
-        <v>50.300000000000004</v>
-      </c>
-      <c r="J37" t="s">
-        <v>533</v>
+        <f>I57</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="38" spans="2:10">
       <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F38,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D45" s="18"/>
+    </row>
+    <row r="46" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B46" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>534</v>
+      </c>
+      <c r="G46" s="29">
         <v>2019</v>
       </c>
-      <c r="G38" t="s">
-        <v>501</v>
-      </c>
-      <c r="I38" s="19">
-        <f>G64</f>
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="F39">
+      <c r="H46" s="29">
         <v>2020</v>
       </c>
-      <c r="G39" t="s">
-        <v>501</v>
-      </c>
-      <c r="I39" s="19">
-        <f>H64</f>
-        <v>56.2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="F40">
+      <c r="I46" s="29">
         <v>2021</v>
       </c>
-      <c r="G40" t="s">
-        <v>501</v>
-      </c>
-      <c r="I40" s="19">
-        <f>I64</f>
-        <v>51.2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F41,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+      <c r="J46" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" t="s">
+        <v>456</v>
+      </c>
+      <c r="C47" t="s">
+        <v>453</v>
+      </c>
+      <c r="D47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J47">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
-      <c r="B42" t="str">
-        <f>"UC_Historic_"&amp;C42&amp;"-cons_Multi"</f>
-        <v>UC_Historic_RSDSOL-cons_Multi</v>
-      </c>
-      <c r="C42" t="str">
-        <f>RIGHT(C65, LEN(C65) - 3)</f>
-        <v>RSDSOL</v>
-      </c>
-      <c r="F42">
-        <v>2018</v>
-      </c>
-      <c r="G42" t="s">
-        <v>501</v>
-      </c>
-      <c r="H42">
+    <row r="48" spans="2:10">
+      <c r="C48" t="s">
+        <v>450</v>
+      </c>
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="G48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I48" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J48">
         <v>1</v>
       </c>
-      <c r="I42" s="19">
-        <f>F65</f>
-        <v>0.6</v>
-      </c>
-      <c r="J42" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10">
-      <c r="F43">
-        <v>2019</v>
-      </c>
-      <c r="G43" t="s">
-        <v>501</v>
-      </c>
-      <c r="I43" s="19">
-        <f>G65</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10">
-      <c r="F44">
-        <v>2020</v>
-      </c>
-      <c r="G44" t="s">
-        <v>501</v>
-      </c>
-      <c r="I44" s="19">
-        <f>H65</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10">
-      <c r="F45">
-        <v>2021</v>
-      </c>
-      <c r="G45" t="s">
-        <v>501</v>
-      </c>
-      <c r="I45" s="19">
-        <f>I65</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10">
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <f>VLOOKUP("Value", 'CO2-config'!$B$4:$D$14,MATCH($F46,'CO2-config'!$B$6:$D$6,),FALSE)</f>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="C49" t="s">
+        <v>445</v>
+      </c>
+      <c r="D49" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F49" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
+        <v>9.1</v>
+      </c>
+      <c r="G49" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
+        <v>7.8</v>
+      </c>
+      <c r="H49" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I49" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
+        <v>7.8</v>
+      </c>
+      <c r="J49">
         <v>1</v>
       </c>
     </row>
+    <row r="50" spans="2:10">
+      <c r="C50" t="s">
+        <v>452</v>
+      </c>
+      <c r="D50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F50" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="G50" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
+        <v>7.6999999999999993</v>
+      </c>
+      <c r="H50" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
+        <v>8</v>
+      </c>
+      <c r="I50" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
+        <v>7.6</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="C51" t="s">
+        <v>446</v>
+      </c>
+      <c r="D51" t="s">
+        <v>200</v>
+      </c>
+      <c r="E51" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F51" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
+        <v>29.5</v>
+      </c>
+      <c r="G51" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
+        <v>30.8</v>
+      </c>
+      <c r="H51" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
+        <v>31.5</v>
+      </c>
+      <c r="I51" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
+        <v>31.5</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" t="s">
+        <v>456</v>
+      </c>
+      <c r="C52" t="s">
+        <v>454</v>
+      </c>
+      <c r="D52" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F52" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
     <row r="53" spans="2:10">
-      <c r="B53" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="D53" s="18"/>
-    </row>
-    <row r="54" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B54" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="F54" s="29">
-        <v>2018</v>
-      </c>
-      <c r="G54" s="29">
-        <v>2019</v>
-      </c>
-      <c r="H54" s="29">
-        <v>2020</v>
-      </c>
-      <c r="I54" s="29">
-        <v>2021</v>
-      </c>
-      <c r="J54" s="29">
-        <v>0</v>
+      <c r="C53" t="s">
+        <v>447</v>
+      </c>
+      <c r="D53" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F53" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
+        <v>25.3</v>
+      </c>
+      <c r="G53" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
+        <v>24.8</v>
+      </c>
+      <c r="H53" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
+        <v>24.700000000000003</v>
+      </c>
+      <c r="I53" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
+        <v>25</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" t="s">
+        <v>456</v>
+      </c>
+      <c r="C54" t="s">
+        <v>455</v>
+      </c>
+      <c r="D54" t="s">
+        <v>200</v>
+      </c>
+      <c r="E54" s="19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="F54" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="19">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" t="s">
-        <v>456</v>
-      </c>
       <c r="C55" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D55" t="s">
         <v>200</v>
@@ -44547,20 +44684,20 @@
         <v>IE,National</v>
       </c>
       <c r="F55" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
+        <v>2.3000000000000003</v>
       </c>
       <c r="G55" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
+        <v>2.1</v>
       </c>
       <c r="H55" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
+        <v>2.4</v>
       </c>
       <c r="I55" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AI$56),1)</f>
-        <v>0</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
+        <v>2.1</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -44568,7 +44705,7 @@
     </row>
     <row r="56" spans="2:10">
       <c r="C56" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D56" t="s">
         <v>200</v>
@@ -44578,20 +44715,20 @@
         <v>IE,National</v>
       </c>
       <c r="F56" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AE$56),1)</f>
-        <v>1.3</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
+        <v>50.300000000000004</v>
       </c>
       <c r="G56" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AE$56),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
+        <v>49.9</v>
       </c>
       <c r="H56" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AE$56),1)</f>
-        <v>1.1000000000000001</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
+        <v>56.2</v>
       </c>
       <c r="I56" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AE$56),1)</f>
-        <v>1.2000000000000002</v>
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
+        <v>51.2</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -44599,7 +44736,7 @@
     </row>
     <row r="57" spans="2:10">
       <c r="C57" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D57" t="s">
         <v>200</v>
@@ -44609,276 +44746,22 @@
         <v>IE,National</v>
       </c>
       <c r="F57" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$C$56),1)</f>
-        <v>9.1</v>
-      </c>
-      <c r="G57" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$C$56),1)</f>
-        <v>7.8</v>
-      </c>
-      <c r="H57" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$C$56),1)</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I57" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$C$56),1)</f>
-        <v>7.8</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10">
-      <c r="C58" t="s">
-        <v>452</v>
-      </c>
-      <c r="D58" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F58" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$H$56),1)</f>
-        <v>8.2999999999999989</v>
-      </c>
-      <c r="G58" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$H$56),1)</f>
-        <v>7.6999999999999993</v>
-      </c>
-      <c r="H58" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$H$56),1)</f>
-        <v>8</v>
-      </c>
-      <c r="I58" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$H$56),1)</f>
-        <v>7.6</v>
-      </c>
-      <c r="J58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10">
-      <c r="C59" t="s">
-        <v>446</v>
-      </c>
-      <c r="D59" t="s">
-        <v>200</v>
-      </c>
-      <c r="E59" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F59" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AO$56),1)</f>
-        <v>29.5</v>
-      </c>
-      <c r="G59" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AO$56),1)+1.5</f>
-        <v>30.8</v>
-      </c>
-      <c r="H59" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AO$56),1)</f>
-        <v>31.5</v>
-      </c>
-      <c r="I59" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AO$56),1)</f>
-        <v>31.5</v>
-      </c>
-      <c r="J59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10">
-      <c r="B60" t="s">
-        <v>456</v>
-      </c>
-      <c r="C60" t="s">
-        <v>454</v>
-      </c>
-      <c r="D60" t="s">
-        <v>200</v>
-      </c>
-      <c r="E60" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F60" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AJ$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10">
-      <c r="C61" t="s">
-        <v>447</v>
-      </c>
-      <c r="D61" t="s">
-        <v>200</v>
-      </c>
-      <c r="E61" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F61" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AA$56),1)</f>
-        <v>25.3</v>
-      </c>
-      <c r="G61" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AA$56),1)</f>
-        <v>24.8</v>
-      </c>
-      <c r="H61" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AA$56),1)</f>
-        <v>24.700000000000003</v>
-      </c>
-      <c r="I61" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AA$56),1)</f>
-        <v>25</v>
-      </c>
-      <c r="J61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10">
-      <c r="B62" t="s">
-        <v>456</v>
-      </c>
-      <c r="C62" t="s">
-        <v>455</v>
-      </c>
-      <c r="D62" t="s">
-        <v>200</v>
-      </c>
-      <c r="E62" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F62" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AP$56),1)</f>
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10">
-      <c r="C63" t="s">
-        <v>448</v>
-      </c>
-      <c r="D63" t="s">
-        <v>200</v>
-      </c>
-      <c r="E63" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F63" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$T$56),1)</f>
-        <v>2.3000000000000003</v>
-      </c>
-      <c r="G63" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$T$56),1)</f>
-        <v>2.1</v>
-      </c>
-      <c r="H63" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$T$56),1)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I63" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$T$56),1)</f>
-        <v>2.1</v>
-      </c>
-      <c r="J63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10">
-      <c r="C64" t="s">
-        <v>451</v>
-      </c>
-      <c r="D64" t="s">
-        <v>200</v>
-      </c>
-      <c r="E64" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F64" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$Q$56,'EB2018'!$U$56,'EB2018'!$V$56),1)</f>
-        <v>50.300000000000004</v>
-      </c>
-      <c r="G64" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$Q$56,'EB2019'!$U$56,'EB2019'!$V$56),1)</f>
-        <v>49.9</v>
-      </c>
-      <c r="H64" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$Q$56,'EB2020'!$U$56,'EB2020'!$V$56),1)</f>
-        <v>56.2</v>
-      </c>
-      <c r="I64" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$Q$56,'EB2021'!$U$56,'EB2021'!$V$56),1)</f>
-        <v>51.2</v>
-      </c>
-      <c r="J64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="3:10">
-      <c r="C65" t="s">
-        <v>449</v>
-      </c>
-      <c r="D65" t="s">
-        <v>200</v>
-      </c>
-      <c r="E65" s="19" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="F65" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="G65" s="19">
+      <c r="G57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="H65" s="19">
+      <c r="H57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="I65" s="19">
+      <c r="I57" s="19">
         <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AL$56),1)</f>
         <v>0.6</v>
       </c>
-      <c r="J65">
+      <c r="J57">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AF changed to 1.03, 2018 historic bounds added
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1336882A-4DAC-45D7-9995-C34B841FB568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEBC0E6-B271-4550-888E-ACCFB8C43F2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="534">
   <si>
     <t>Development</t>
   </si>
@@ -1830,9 +1830,6 @@
   </si>
   <si>
     <t>Historic Kerosene consumption in RSD - Multi</t>
-  </si>
-  <si>
-    <t>*2018</t>
   </si>
 </sst>
 </file>
@@ -43857,7 +43854,7 @@
   <dimension ref="B2:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44399,8 +44396,8 @@
       <c r="E46" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="F46" s="29" t="s">
-        <v>534</v>
+      <c r="F46" s="29">
+        <v>2018</v>
       </c>
       <c r="G46" s="29">
         <v>2019</v>

</xml_diff>

<commit_message>
Allow Fireplace in 2018 to fix EB -
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11C4A2A-5556-4678-AA13-0258F043CBAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8BFD0C-950E-4E5E-92F6-99FC0FD4C52B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="534">
   <si>
     <t>Development</t>
   </si>
@@ -1830,9 +1830,6 @@
   </si>
   <si>
     <t>Historic Kerosene consumption in RSD - Multi</t>
-  </si>
-  <si>
-    <t>*2018</t>
   </si>
 </sst>
 </file>
@@ -43857,7 +43854,7 @@
   <dimension ref="B2:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44399,8 +44396,8 @@
       <c r="E46" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="F46" s="29" t="s">
-        <v>534</v>
+      <c r="F46" s="29">
+        <v>2018</v>
       </c>
       <c r="G46" s="29">
         <v>2019</v>

</xml_diff>